<commit_message>
dar report test case added
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
+++ b/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B11625-085D-45E4-B01A-B3A1FBFD10E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3889621E-5893-4101-950E-0BE5C77616FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="240">
   <si>
     <t>Environment</t>
   </si>
@@ -769,6 +769,68 @@
   </si>
   <si>
     <t>mubashir_SoGo@123</t>
+  </si>
+  <si>
+    <t>Smoke_TC15</t>
+  </si>
+  <si>
+    <t>Dar report</t>
+  </si>
+  <si>
+    <t>1. Login in to given account.
+2. Enter user credential and click on login. (After every release there will be a banner for some time, "e,g https://www.sogosurvey.com/static/maintenance.aspx", need to continue ahead by clicking X icon on top right corner)
+3. Click on Project dashboard.
+3. Select folder named as 'DAR DP'
+4. Hover over survey named as 'Safe Schools Survey - Students 2018' and click 'Report' icon.
+5. Click on Special Reports button and select 'Dimenssion Analysis' report in drop down
+6. From Time Period 1 column and Target Group 1, select DAR DP folder &gt; Safe Schools Survey - Students 2018
+6. From Time Period 2 column and Target Group 1, select DAR DP folder &gt; Safe Schools Survey - Students 2019
+7. Click on Generate button
+"8. Add follwing elements onto the canvas by clicking on Star icon:
+i) Overall score graph and data table
+ii) Comparion by time graph of overall score and and data table
+iii) Dimension score graph and data table
+iv) Comparion by time graph of Dimenscore score and and data table
+v) Rules and Regulations graph and data table
+vi) Comparion by time graph of Rules and Regulations and and data table
+vii) Highest and Lowerst ranking indicator
+viii) What is your ethnic group graph and data table
+ix) Please respond to the following statements.graph and data table
+x) Response Rate graph and data table
+xi)  Response Sorce graph and data table"
+9. Click on Report Canvas.
+10. Enter Report title as 'DAR DP'
+11. Enter Report description as 'Today's Date'
+12. Click on Segment icon given at top right corner
+13. Select Safe Schools Survey - Students 2018 in Select Survey drop down
+14. Select Q.5 a) in Select Segmentation Question drop down
+15. Select All answer options.
+16. Enter given email id in To field and click on Email Report button
+17. Accept alert message.</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>Safe Schools Survey - Students 2018</t>
+  </si>
+  <si>
+    <t>sogo_ruksar_ep</t>
+  </si>
+  <si>
+    <t>Sogo@excx339</t>
+  </si>
+  <si>
+    <t>RMX2</t>
+  </si>
+  <si>
+    <t>DAR DP,Safe Schools Survey - Students 2018,DAR DP,Safe Schools Survey - Students 2019</t>
+  </si>
+  <si>
+    <t>DAR DP</t>
+  </si>
+  <si>
+    <t>9428824</t>
   </si>
 </sst>
 </file>
@@ -1315,10 +1377,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:D5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,6 +1461,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
@@ -1410,10 +1486,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CO15"/>
+  <dimension ref="A1:CO16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,6 +3553,140 @@
         <v>196</v>
       </c>
     </row>
+    <row r="16" spans="1:93" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="J16" s="23"/>
+      <c r="K16" s="22" t="s">
+        <v>238</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M16" s="24" t="s">
+        <v>239</v>
+      </c>
+      <c r="N16" s="22"/>
+      <c r="O16" s="24" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q16" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="R16" s="24" t="s">
+        <v>216</v>
+      </c>
+      <c r="S16" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="T16" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="U16" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="V16" s="24"/>
+      <c r="W16" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
+      <c r="AA16" s="24"/>
+      <c r="AB16" s="24"/>
+      <c r="AC16" s="24"/>
+      <c r="AD16" s="24"/>
+      <c r="AE16" s="24"/>
+      <c r="AF16" s="24"/>
+      <c r="AG16" s="24"/>
+      <c r="AH16" s="24"/>
+      <c r="AI16" s="24"/>
+      <c r="AJ16" s="24"/>
+      <c r="AK16" s="24"/>
+      <c r="AL16" s="24"/>
+      <c r="AM16" s="24"/>
+      <c r="AN16" s="22"/>
+      <c r="AO16" s="25"/>
+      <c r="AP16" s="25"/>
+      <c r="AQ16" s="25"/>
+      <c r="AR16" s="25"/>
+      <c r="AS16" s="25"/>
+      <c r="AT16" s="25"/>
+      <c r="AU16" s="25"/>
+      <c r="AV16" s="25"/>
+      <c r="AW16" s="25"/>
+      <c r="AX16" s="25"/>
+      <c r="AY16" s="25"/>
+      <c r="AZ16" s="25"/>
+      <c r="BA16" s="25"/>
+      <c r="BB16" s="25"/>
+      <c r="BC16" s="25"/>
+      <c r="BD16" s="25"/>
+      <c r="BE16" s="26"/>
+      <c r="BF16" s="25"/>
+      <c r="BG16" s="25"/>
+      <c r="BH16" s="25"/>
+      <c r="BI16" s="25"/>
+      <c r="BJ16" s="25"/>
+      <c r="BK16" s="25"/>
+      <c r="BL16" s="25"/>
+      <c r="BM16" s="25"/>
+      <c r="BN16" s="25"/>
+      <c r="BO16" s="25"/>
+      <c r="BP16" s="25"/>
+      <c r="BQ16" s="25"/>
+      <c r="BR16" s="25"/>
+      <c r="BS16" s="25"/>
+      <c r="BT16" s="25"/>
+      <c r="BU16" s="25"/>
+      <c r="BV16" s="25"/>
+      <c r="BW16" s="25"/>
+      <c r="BX16" s="25"/>
+      <c r="BY16" s="25"/>
+      <c r="BZ16" s="25"/>
+      <c r="CA16" s="25"/>
+      <c r="CB16" s="25"/>
+      <c r="CC16" s="25"/>
+      <c r="CD16" s="25"/>
+      <c r="CE16" s="25"/>
+      <c r="CF16" s="25"/>
+      <c r="CG16" s="25"/>
+      <c r="CH16" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="CI16" s="26"/>
+      <c r="CJ16" s="26"/>
+      <c r="CK16" s="26"/>
+      <c r="CL16" s="26"/>
+      <c r="CM16" s="26"/>
+      <c r="CN16" s="26"/>
+      <c r="CO16" s="26" t="s">
+        <v>233</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Adding Smx smoke testing cases
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
+++ b/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA90D5A-5F67-48C6-8F9E-6C17DDD9B756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C96437-0CBD-4942-BC5B-B635E74D9CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="600" windowWidth="15150" windowHeight="10920" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="280">
   <si>
     <t>Environment</t>
   </si>
@@ -827,58 +827,121 @@
     <t>Test Invitation List [4 records]</t>
   </si>
   <si>
+    <t xml:space="preserve"> List Name not present on page.</t>
+  </si>
+  <si>
+    <t>Smoke_TC17</t>
+  </si>
+  <si>
+    <t>DATA</t>
+  </si>
+  <si>
+    <t>Data Import</t>
+  </si>
+  <si>
+    <t>DATA DP SURVEY 2</t>
+  </si>
+  <si>
+    <t>SoGo Data Import File.xls</t>
+  </si>
+  <si>
+    <t>sogo_mjitender1</t>
+  </si>
+  <si>
+    <t>Jittu@123</t>
+  </si>
+  <si>
+    <t>Smoke_TC18</t>
+  </si>
+  <si>
+    <t>Data Export</t>
+  </si>
+  <si>
+    <t>DATA DP SURVEY 3</t>
+  </si>
+  <si>
+    <t>DP - Segment group</t>
+  </si>
+  <si>
+    <t>Q 1(b). Please provide your details: Gender</t>
+  </si>
+  <si>
+    <t>ayadav@zarca.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> From fieldis not present on page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Email Engagement Report not present on page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The file was not downloaded.</t>
+  </si>
+  <si>
+    <t>SMX</t>
+  </si>
+  <si>
+    <t>Create All Control Survey</t>
+  </si>
+  <si>
+    <t>All Questions</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>quesHint</t>
+  </si>
+  <si>
+    <t>Emp####</t>
+  </si>
+  <si>
+    <t>Custom format</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Error occured while reading JSON file. Error : E:\Project\engage\Engage\Sogo-Smoke\src\main\resources\jsonFiles\localData.json (The system cannot find the file specified)</t>
+  </si>
+  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t xml:space="preserve"> You have sent not present on page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> List Name not present on page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Not able to find element Toaster - Close on page.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> This report has been saved as is not present on page.</t>
-  </si>
-  <si>
-    <t>Smoke_TC17</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>Data Import</t>
-  </si>
-  <si>
-    <t>DATA DP SURVEY 2</t>
-  </si>
-  <si>
-    <t>SoGo Data Import File.xls</t>
-  </si>
-  <si>
-    <t>sogo_mjitender1</t>
-  </si>
-  <si>
-    <t>Jittu@123</t>
-  </si>
-  <si>
-    <t>Smoke_TC18</t>
-  </si>
-  <si>
-    <t>Data Export</t>
-  </si>
-  <si>
-    <t>DATA DP SURVEY 3</t>
-  </si>
-  <si>
-    <t>DP - Segment group</t>
-  </si>
-  <si>
-    <t>Q 1(b). Please provide your details: Gender</t>
-  </si>
-  <si>
-    <t>ayadav@zarca.com</t>
+    <t xml:space="preserve"> Import data module not present on page.</t>
+  </si>
+  <si>
+    <t>subQuestionCount</t>
+  </si>
+  <si>
+    <t>srsFormat</t>
+  </si>
+  <si>
+    <t>Star;Thumb up;Heart;Check mark;Dollar sign;Person</t>
+  </si>
+  <si>
+    <t>Mountain;Harley</t>
+  </si>
+  <si>
+    <t>MTBSubqueCount</t>
+  </si>
+  <si>
+    <t>mtbFormat</t>
+  </si>
+  <si>
+    <t>General;Currency;Email;Phone Number;Number;Percentage;Social Security Number;US ZIP Code;US ZIP Code + 4;Custom</t>
+  </si>
+  <si>
+    <t>Lowest-0;Middle-3;Highest-5;Not Applicable</t>
+  </si>
+  <si>
+    <t>attachmentQDetails1</t>
+  </si>
+  <si>
+    <t>4/~~/Attachment 1/~/Attachment 2/~/Attachment 3/~/Attachment 4/~~/.jpg,.png/~/.pdf/~/.xlsx/~/.pptx</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Text Box Label Added null not present on page.</t>
+  </si>
+  <si>
+    <t>Smoke_TC119</t>
   </si>
 </sst>
 </file>
@@ -1337,7 +1400,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1381,7 +1444,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +1490,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" activeCellId="1" sqref="A7:D8 C13"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1545,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>258</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>158</v>
@@ -1524,13 +1587,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B7" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>251</v>
-      </c>
       <c r="C7" s="28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D7" s="25" t="s">
         <v>3</v>
@@ -1538,13 +1601,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="B8" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>251</v>
-      </c>
       <c r="C8" s="28" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D8" s="25" t="s">
         <v>3</v>
@@ -1564,10 +1627,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CO19"/>
+  <dimension ref="A1:CV20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1592,7 +1655,7 @@
     <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1831,49 +1894,70 @@
         <v>137</v>
       </c>
       <c r="CB1" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="CC1" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="CC1" s="9" t="s">
+      <c r="CD1" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="CD1" s="9" t="s">
+      <c r="CE1" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="CE1" s="9" t="s">
+      <c r="CF1" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="CF1" s="9" t="s">
+      <c r="CG1" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="CG1" s="9" t="s">
+      <c r="CH1" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="CH1" s="9" t="s">
+      <c r="CI1" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="CJ1" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="CK1" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="CL1" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="CM1" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="CN1" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="CI1" s="9" t="s">
+      <c r="CO1" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="CJ1" s="9" t="s">
+      <c r="CP1" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="CK1" s="9" t="s">
+      <c r="CQ1" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="CL1" s="9" t="s">
+      <c r="CR1" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="CM1" s="9" t="s">
+      <c r="CS1" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="CN1" s="9" t="s">
+      <c r="CT1" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="CO1" s="9" t="s">
+      <c r="CU1" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="CV1" s="9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1985,8 +2069,15 @@
       <c r="CM2" s="6"/>
       <c r="CN2" s="6"/>
       <c r="CO2" s="6"/>
+      <c r="CP2" s="6"/>
+      <c r="CQ2" s="6"/>
+      <c r="CR2" s="6"/>
+      <c r="CS2" s="6"/>
+      <c r="CT2" s="6"/>
+      <c r="CU2" s="6"/>
+      <c r="CV2" s="6"/>
     </row>
-    <row r="3" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -2000,7 +2091,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>7</v>
+        <v>258</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>30</v>
@@ -2150,25 +2241,25 @@
       <c r="CA3" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="CB3" s="15" t="s">
+      <c r="CB3" s="15"/>
+      <c r="CC3" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="CC3" s="15" t="s">
+      <c r="CD3" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="CD3" s="15" t="s">
+      <c r="CE3" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="CE3" s="15" t="s">
+      <c r="CF3" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="CF3" s="15" t="s">
+      <c r="CG3" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="CG3" s="15" t="s">
+      <c r="CH3" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="CH3" s="15"/>
       <c r="CI3" s="15"/>
       <c r="CJ3" s="15"/>
       <c r="CK3" s="15"/>
@@ -2176,8 +2267,15 @@
       <c r="CM3" s="15"/>
       <c r="CN3" s="15"/>
       <c r="CO3" s="15"/>
+      <c r="CP3" s="15"/>
+      <c r="CQ3" s="15"/>
+      <c r="CR3" s="15"/>
+      <c r="CS3" s="15"/>
+      <c r="CT3" s="15"/>
+      <c r="CU3" s="15"/>
+      <c r="CV3" s="15"/>
     </row>
-    <row r="4" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>180</v>
       </c>
@@ -2279,30 +2377,37 @@
       <c r="CE4" s="15"/>
       <c r="CF4" s="15"/>
       <c r="CG4" s="15"/>
-      <c r="CH4" s="1">
+      <c r="CH4" s="15"/>
+      <c r="CI4" s="15"/>
+      <c r="CJ4" s="15"/>
+      <c r="CK4" s="15"/>
+      <c r="CL4" s="15"/>
+      <c r="CM4" s="15"/>
+      <c r="CN4" s="1">
         <v>282</v>
       </c>
-      <c r="CI4" s="16" t="s">
+      <c r="CO4" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="CJ4" s="16" t="s">
+      <c r="CP4" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="CK4" s="16" t="s">
+      <c r="CQ4" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="CL4" s="16" t="s">
+      <c r="CR4" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="CM4" s="16" t="s">
+      <c r="CS4" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="CN4" s="16" t="s">
+      <c r="CT4" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="CO4" s="16"/>
+      <c r="CU4" s="16"/>
+      <c r="CV4" s="16"/>
     </row>
-    <row r="5" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>181</v>
       </c>
@@ -2328,7 +2433,9 @@
       <c r="I5" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="14" t="s">
+        <v>265</v>
+      </c>
       <c r="K5" s="1"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14"/>
@@ -2404,30 +2511,37 @@
       <c r="CE5" s="15"/>
       <c r="CF5" s="15"/>
       <c r="CG5" s="15"/>
-      <c r="CH5" s="1">
+      <c r="CH5" s="15"/>
+      <c r="CI5" s="15"/>
+      <c r="CJ5" s="15"/>
+      <c r="CK5" s="15"/>
+      <c r="CL5" s="15"/>
+      <c r="CM5" s="15"/>
+      <c r="CN5" s="1">
         <v>283</v>
       </c>
-      <c r="CI5" s="16" t="s">
+      <c r="CO5" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="CJ5" s="16" t="s">
+      <c r="CP5" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="CK5" s="16" t="s">
+      <c r="CQ5" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="CL5" s="16" t="s">
+      <c r="CR5" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="CM5" s="16" t="s">
+      <c r="CS5" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="CN5" s="16" t="s">
+      <c r="CT5" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="CO5" s="16"/>
+      <c r="CU5" s="16"/>
+      <c r="CV5" s="16"/>
     </row>
-    <row r="6" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>182</v>
       </c>
@@ -2454,7 +2568,7 @@
         <v>185</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="14"/>
@@ -2531,20 +2645,27 @@
       <c r="CE6" s="15"/>
       <c r="CF6" s="15"/>
       <c r="CG6" s="15"/>
-      <c r="CH6" s="1">
+      <c r="CH6" s="15"/>
+      <c r="CI6" s="15"/>
+      <c r="CJ6" s="15"/>
+      <c r="CK6" s="15"/>
+      <c r="CL6" s="15"/>
+      <c r="CM6" s="15"/>
+      <c r="CN6" s="1">
         <v>283</v>
       </c>
-      <c r="CI6" s="16"/>
-      <c r="CJ6" s="16" t="s">
+      <c r="CO6" s="16"/>
+      <c r="CP6" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="CK6" s="16"/>
-      <c r="CL6" s="16"/>
-      <c r="CM6" s="16"/>
-      <c r="CN6" s="16"/>
-      <c r="CO6" s="16"/>
+      <c r="CQ6" s="16"/>
+      <c r="CR6" s="16"/>
+      <c r="CS6" s="16"/>
+      <c r="CT6" s="16"/>
+      <c r="CU6" s="16"/>
+      <c r="CV6" s="16"/>
     </row>
-    <row r="7" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>183</v>
       </c>
@@ -2646,22 +2767,29 @@
       <c r="CE7" s="15"/>
       <c r="CF7" s="15"/>
       <c r="CG7" s="15"/>
-      <c r="CH7" s="1">
+      <c r="CH7" s="15"/>
+      <c r="CI7" s="15"/>
+      <c r="CJ7" s="15"/>
+      <c r="CK7" s="15"/>
+      <c r="CL7" s="15"/>
+      <c r="CM7" s="15"/>
+      <c r="CN7" s="1">
         <v>283</v>
       </c>
-      <c r="CI7" s="16"/>
-      <c r="CJ7" s="16" t="s">
+      <c r="CO7" s="16"/>
+      <c r="CP7" s="16" t="s">
         <v>239</v>
       </c>
-      <c r="CK7" s="16"/>
-      <c r="CL7" s="16"/>
-      <c r="CM7" s="16" t="s">
+      <c r="CQ7" s="16"/>
+      <c r="CR7" s="16"/>
+      <c r="CS7" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="CN7" s="16"/>
-      <c r="CO7" s="16"/>
+      <c r="CT7" s="16"/>
+      <c r="CU7" s="16"/>
+      <c r="CV7" s="16"/>
     </row>
-    <row r="8" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>184</v>
       </c>
@@ -2688,7 +2816,7 @@
         <v>185</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="17"/>
@@ -2765,22 +2893,29 @@
       <c r="CE8" s="18"/>
       <c r="CF8" s="18"/>
       <c r="CG8" s="18"/>
-      <c r="CH8" s="1">
+      <c r="CH8" s="18"/>
+      <c r="CI8" s="18"/>
+      <c r="CJ8" s="18"/>
+      <c r="CK8" s="18"/>
+      <c r="CL8" s="18"/>
+      <c r="CM8" s="18"/>
+      <c r="CN8" s="1">
         <v>283</v>
       </c>
-      <c r="CI8" s="19"/>
-      <c r="CJ8" s="19" t="s">
+      <c r="CO8" s="19"/>
+      <c r="CP8" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="CK8" s="19"/>
-      <c r="CL8" s="19"/>
-      <c r="CM8" s="19" t="s">
+      <c r="CQ8" s="19"/>
+      <c r="CR8" s="19"/>
+      <c r="CS8" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="CN8" s="19"/>
-      <c r="CO8" s="19"/>
+      <c r="CT8" s="19"/>
+      <c r="CU8" s="19"/>
+      <c r="CV8" s="19"/>
     </row>
-    <row r="9" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>159</v>
       </c>
@@ -2884,26 +3019,33 @@
       <c r="CE9" s="1"/>
       <c r="CF9" s="1"/>
       <c r="CG9" s="1"/>
-      <c r="CH9" s="1">
+      <c r="CH9" s="1"/>
+      <c r="CI9" s="1"/>
+      <c r="CJ9" s="1"/>
+      <c r="CK9" s="1"/>
+      <c r="CL9" s="1"/>
+      <c r="CM9" s="1"/>
+      <c r="CN9" s="1">
         <v>311</v>
       </c>
-      <c r="CI9" s="1" t="s">
+      <c r="CO9" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="CJ9" s="16" t="s">
+      <c r="CP9" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="CK9" s="1" t="s">
+      <c r="CQ9" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="CL9" s="1" t="s">
+      <c r="CR9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="CM9" s="1"/>
-      <c r="CN9" s="1"/>
-      <c r="CO9" s="1"/>
+      <c r="CS9" s="1"/>
+      <c r="CT9" s="1"/>
+      <c r="CU9" s="1"/>
+      <c r="CV9" s="1"/>
     </row>
-    <row r="10" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>216</v>
       </c>
@@ -2930,7 +3072,7 @@
         <v>185</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="K10" s="20" t="s">
         <v>190</v>
@@ -2939,10 +3081,10 @@
       <c r="M10" s="21"/>
       <c r="N10" s="20"/>
       <c r="O10" s="20" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="P10" s="20" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="Q10" s="20"/>
       <c r="R10" s="20"/>
@@ -2951,7 +3093,7 @@
       <c r="U10" s="22"/>
       <c r="V10" s="22"/>
       <c r="W10" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X10" s="22"/>
       <c r="Y10" s="22"/>
@@ -3015,20 +3157,27 @@
       <c r="CE10" s="23"/>
       <c r="CF10" s="23"/>
       <c r="CG10" s="23"/>
-      <c r="CH10" s="24" t="s">
+      <c r="CH10" s="23"/>
+      <c r="CI10" s="23"/>
+      <c r="CJ10" s="23"/>
+      <c r="CK10" s="23"/>
+      <c r="CL10" s="23"/>
+      <c r="CM10" s="23"/>
+      <c r="CN10" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="CI10" s="24"/>
-      <c r="CJ10" s="24"/>
-      <c r="CK10" s="24"/>
-      <c r="CL10" s="24"/>
-      <c r="CM10" s="24"/>
-      <c r="CN10" s="24"/>
-      <c r="CO10" s="24" t="s">
+      <c r="CO10" s="24"/>
+      <c r="CP10" s="24"/>
+      <c r="CQ10" s="24"/>
+      <c r="CR10" s="24"/>
+      <c r="CS10" s="24"/>
+      <c r="CT10" s="24"/>
+      <c r="CU10" s="24"/>
+      <c r="CV10" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>217</v>
       </c>
@@ -3055,7 +3204,7 @@
         <v>185</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>244</v>
+        <v>255</v>
       </c>
       <c r="K11" s="20" t="s">
         <v>195</v>
@@ -3072,7 +3221,7 @@
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
       <c r="W11" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X11" s="22"/>
       <c r="Y11" s="22"/>
@@ -3136,20 +3285,27 @@
       <c r="CE11" s="23"/>
       <c r="CF11" s="23"/>
       <c r="CG11" s="23"/>
-      <c r="CH11" s="24" t="s">
+      <c r="CH11" s="23"/>
+      <c r="CI11" s="23"/>
+      <c r="CJ11" s="23"/>
+      <c r="CK11" s="23"/>
+      <c r="CL11" s="23"/>
+      <c r="CM11" s="23"/>
+      <c r="CN11" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="CI11" s="24"/>
-      <c r="CJ11" s="24"/>
-      <c r="CK11" s="24"/>
-      <c r="CL11" s="24"/>
-      <c r="CM11" s="24"/>
-      <c r="CN11" s="24"/>
-      <c r="CO11" s="24" t="s">
+      <c r="CO11" s="24"/>
+      <c r="CP11" s="24"/>
+      <c r="CQ11" s="24"/>
+      <c r="CR11" s="24"/>
+      <c r="CS11" s="24"/>
+      <c r="CT11" s="24"/>
+      <c r="CU11" s="24"/>
+      <c r="CV11" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>218</v>
       </c>
@@ -3191,7 +3347,7 @@
       <c r="U12" s="22"/>
       <c r="V12" s="22"/>
       <c r="W12" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X12" s="22"/>
       <c r="Y12" s="22"/>
@@ -3255,20 +3411,27 @@
       <c r="CE12" s="23"/>
       <c r="CF12" s="23"/>
       <c r="CG12" s="23"/>
-      <c r="CH12" s="24" t="s">
+      <c r="CH12" s="23"/>
+      <c r="CI12" s="23"/>
+      <c r="CJ12" s="23"/>
+      <c r="CK12" s="23"/>
+      <c r="CL12" s="23"/>
+      <c r="CM12" s="23"/>
+      <c r="CN12" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="CI12" s="24"/>
-      <c r="CJ12" s="24"/>
-      <c r="CK12" s="24"/>
-      <c r="CL12" s="24"/>
-      <c r="CM12" s="24"/>
-      <c r="CN12" s="24"/>
-      <c r="CO12" s="24" t="s">
+      <c r="CO12" s="24"/>
+      <c r="CP12" s="24"/>
+      <c r="CQ12" s="24"/>
+      <c r="CR12" s="24"/>
+      <c r="CS12" s="24"/>
+      <c r="CT12" s="24"/>
+      <c r="CU12" s="24"/>
+      <c r="CV12" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>219</v>
       </c>
@@ -3310,7 +3473,7 @@
       <c r="U13" s="22"/>
       <c r="V13" s="22"/>
       <c r="W13" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X13" s="22"/>
       <c r="Y13" s="22"/>
@@ -3374,20 +3537,27 @@
       <c r="CE13" s="23"/>
       <c r="CF13" s="23"/>
       <c r="CG13" s="23"/>
-      <c r="CH13" s="24" t="s">
+      <c r="CH13" s="23"/>
+      <c r="CI13" s="23"/>
+      <c r="CJ13" s="23"/>
+      <c r="CK13" s="23"/>
+      <c r="CL13" s="23"/>
+      <c r="CM13" s="23"/>
+      <c r="CN13" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="CI13" s="24"/>
-      <c r="CJ13" s="24"/>
-      <c r="CK13" s="24"/>
-      <c r="CL13" s="24"/>
-      <c r="CM13" s="24"/>
-      <c r="CN13" s="24"/>
-      <c r="CO13" s="24" t="s">
+      <c r="CO13" s="24"/>
+      <c r="CP13" s="24"/>
+      <c r="CQ13" s="24"/>
+      <c r="CR13" s="24"/>
+      <c r="CS13" s="24"/>
+      <c r="CT13" s="24"/>
+      <c r="CU13" s="24"/>
+      <c r="CV13" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>220</v>
       </c>
@@ -3429,7 +3599,7 @@
       <c r="U14" s="22"/>
       <c r="V14" s="22"/>
       <c r="W14" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X14" s="22"/>
       <c r="Y14" s="22"/>
@@ -3493,20 +3663,27 @@
       <c r="CE14" s="23"/>
       <c r="CF14" s="23"/>
       <c r="CG14" s="23"/>
-      <c r="CH14" s="24" t="s">
+      <c r="CH14" s="23"/>
+      <c r="CI14" s="23"/>
+      <c r="CJ14" s="23"/>
+      <c r="CK14" s="23"/>
+      <c r="CL14" s="23"/>
+      <c r="CM14" s="23"/>
+      <c r="CN14" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="CI14" s="24"/>
-      <c r="CJ14" s="24"/>
-      <c r="CK14" s="24"/>
-      <c r="CL14" s="24"/>
-      <c r="CM14" s="24"/>
-      <c r="CN14" s="24"/>
-      <c r="CO14" s="24" t="s">
+      <c r="CO14" s="24"/>
+      <c r="CP14" s="24"/>
+      <c r="CQ14" s="24"/>
+      <c r="CR14" s="24"/>
+      <c r="CS14" s="24"/>
+      <c r="CT14" s="24"/>
+      <c r="CU14" s="24"/>
+      <c r="CV14" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>221</v>
       </c>
@@ -3532,7 +3709,9 @@
       <c r="I15" s="30" t="s">
         <v>185</v>
       </c>
-      <c r="J15" s="21"/>
+      <c r="J15" s="21" t="s">
+        <v>256</v>
+      </c>
       <c r="K15" s="20" t="s">
         <v>207</v>
       </c>
@@ -3566,7 +3745,7 @@
       </c>
       <c r="V15" s="22"/>
       <c r="W15" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X15" s="22"/>
       <c r="Y15" s="22"/>
@@ -3630,20 +3809,27 @@
       <c r="CE15" s="23"/>
       <c r="CF15" s="23"/>
       <c r="CG15" s="23"/>
-      <c r="CH15" s="24" t="s">
+      <c r="CH15" s="23"/>
+      <c r="CI15" s="23"/>
+      <c r="CJ15" s="23"/>
+      <c r="CK15" s="23"/>
+      <c r="CL15" s="23"/>
+      <c r="CM15" s="23"/>
+      <c r="CN15" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="CI15" s="24"/>
-      <c r="CJ15" s="24"/>
-      <c r="CK15" s="24"/>
-      <c r="CL15" s="24"/>
-      <c r="CM15" s="24"/>
-      <c r="CN15" s="24"/>
-      <c r="CO15" s="24" t="s">
+      <c r="CO15" s="24"/>
+      <c r="CP15" s="24"/>
+      <c r="CQ15" s="24"/>
+      <c r="CR15" s="24"/>
+      <c r="CS15" s="24"/>
+      <c r="CT15" s="24"/>
+      <c r="CU15" s="24"/>
+      <c r="CV15" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>225</v>
       </c>
@@ -3700,7 +3886,7 @@
       </c>
       <c r="V16" s="22"/>
       <c r="W16" s="27" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="X16" s="22"/>
       <c r="Y16" s="22"/>
@@ -3764,20 +3950,27 @@
       <c r="CE16" s="23"/>
       <c r="CF16" s="23"/>
       <c r="CG16" s="23"/>
-      <c r="CH16" s="24" t="s">
+      <c r="CH16" s="23"/>
+      <c r="CI16" s="23"/>
+      <c r="CJ16" s="23"/>
+      <c r="CK16" s="23"/>
+      <c r="CL16" s="23"/>
+      <c r="CM16" s="23"/>
+      <c r="CN16" s="24" t="s">
         <v>228</v>
       </c>
-      <c r="CI16" s="24"/>
-      <c r="CJ16" s="24"/>
-      <c r="CK16" s="24"/>
-      <c r="CL16" s="24"/>
-      <c r="CM16" s="24"/>
-      <c r="CN16" s="24"/>
-      <c r="CO16" s="24" t="s">
+      <c r="CO16" s="24"/>
+      <c r="CP16" s="24"/>
+      <c r="CQ16" s="24"/>
+      <c r="CR16" s="24"/>
+      <c r="CS16" s="24"/>
+      <c r="CT16" s="24"/>
+      <c r="CU16" s="24"/>
+      <c r="CV16" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>237</v>
       </c>
@@ -3879,25 +4072,32 @@
       <c r="CE17" s="15"/>
       <c r="CF17" s="15"/>
       <c r="CG17" s="15"/>
-      <c r="CH17" s="1">
+      <c r="CH17" s="15"/>
+      <c r="CI17" s="15"/>
+      <c r="CJ17" s="15"/>
+      <c r="CK17" s="15"/>
+      <c r="CL17" s="15"/>
+      <c r="CM17" s="15"/>
+      <c r="CN17" s="1">
         <v>282</v>
       </c>
-      <c r="CI17" s="16"/>
-      <c r="CJ17" s="16"/>
-      <c r="CK17" s="16"/>
-      <c r="CL17" s="16"/>
-      <c r="CM17" s="16"/>
-      <c r="CN17" s="16" t="s">
+      <c r="CO17" s="16"/>
+      <c r="CP17" s="16"/>
+      <c r="CQ17" s="16"/>
+      <c r="CR17" s="16"/>
+      <c r="CS17" s="16"/>
+      <c r="CT17" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="CO17" s="16"/>
+      <c r="CU17" s="16"/>
+      <c r="CV17" s="16"/>
     </row>
-    <row r="18" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>15</v>
@@ -3906,17 +4106,19 @@
         <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="29" t="s">
-        <v>241</v>
-      </c>
-      <c r="J18" s="14"/>
+      <c r="I18" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>267</v>
+      </c>
       <c r="K18" s="1"/>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
@@ -3953,7 +4155,7 @@
       <c r="AR18" s="15"/>
       <c r="AS18" s="15"/>
       <c r="AT18" s="15" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AU18" s="15"/>
       <c r="AV18" s="15"/>
@@ -3994,25 +4196,32 @@
       <c r="CE18" s="15"/>
       <c r="CF18" s="15"/>
       <c r="CG18" s="15"/>
-      <c r="CH18" s="1">
+      <c r="CH18" s="15"/>
+      <c r="CI18" s="15"/>
+      <c r="CJ18" s="15"/>
+      <c r="CK18" s="15"/>
+      <c r="CL18" s="15"/>
+      <c r="CM18" s="15"/>
+      <c r="CN18" s="1">
         <v>320</v>
       </c>
-      <c r="CI18" s="16"/>
-      <c r="CJ18" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="CK18" s="16"/>
-      <c r="CL18" s="16"/>
-      <c r="CM18" s="16"/>
-      <c r="CN18" s="16"/>
       <c r="CO18" s="16"/>
+      <c r="CP18" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="CQ18" s="16"/>
+      <c r="CR18" s="16"/>
+      <c r="CS18" s="16"/>
+      <c r="CT18" s="16"/>
+      <c r="CU18" s="16"/>
+      <c r="CV18" s="16"/>
     </row>
-    <row r="19" spans="1:93" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:100" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>15</v>
@@ -4021,15 +4230,15 @@
         <v>17</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="29" t="s">
-        <v>241</v>
+      <c r="I19" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J19" s="14"/>
       <c r="K19" s="1"/>
@@ -4070,7 +4279,7 @@
       <c r="AR19" s="15"/>
       <c r="AS19" s="15"/>
       <c r="AT19" s="15" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="AU19" s="15"/>
       <c r="AV19" s="15"/>
@@ -4111,16 +4320,177 @@
       <c r="CE19" s="15"/>
       <c r="CF19" s="15"/>
       <c r="CG19" s="15"/>
-      <c r="CH19" s="1">
+      <c r="CH19" s="15"/>
+      <c r="CI19" s="15"/>
+      <c r="CJ19" s="15"/>
+      <c r="CK19" s="15"/>
+      <c r="CL19" s="15"/>
+      <c r="CM19" s="15"/>
+      <c r="CN19" s="1">
         <v>256</v>
       </c>
-      <c r="CI19" s="16"/>
-      <c r="CJ19" s="16"/>
-      <c r="CK19" s="16"/>
-      <c r="CL19" s="16"/>
-      <c r="CM19" s="16"/>
-      <c r="CN19" s="16"/>
       <c r="CO19" s="16"/>
+      <c r="CP19" s="16"/>
+      <c r="CQ19" s="16"/>
+      <c r="CR19" s="16"/>
+      <c r="CS19" s="16"/>
+      <c r="CT19" s="16"/>
+      <c r="CU19" s="16"/>
+      <c r="CV19" s="16"/>
+    </row>
+    <row r="20" spans="1:100" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="29" t="s">
+        <v>266</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+      <c r="W20" s="5"/>
+      <c r="X20" s="5"/>
+      <c r="Y20" s="5"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="5"/>
+      <c r="AB20" s="5"/>
+      <c r="AC20" s="5"/>
+      <c r="AD20" s="5"/>
+      <c r="AE20" s="5"/>
+      <c r="AF20" s="5"/>
+      <c r="AG20" s="5"/>
+      <c r="AH20" s="5"/>
+      <c r="AI20" s="5"/>
+      <c r="AJ20" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="AK20" s="5"/>
+      <c r="AL20" s="5"/>
+      <c r="AM20" s="5"/>
+      <c r="AN20" s="1"/>
+      <c r="AO20" s="15"/>
+      <c r="AP20" s="15"/>
+      <c r="AQ20" s="15"/>
+      <c r="AR20" s="15"/>
+      <c r="AS20" s="15"/>
+      <c r="AT20" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="AU20" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV20" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW20" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX20" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY20" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB20" s="15"/>
+      <c r="BC20" s="15"/>
+      <c r="BD20" s="15"/>
+      <c r="BE20" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="BF20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="BG20" s="15"/>
+      <c r="BH20" s="15"/>
+      <c r="BI20" s="15"/>
+      <c r="BJ20" s="15"/>
+      <c r="BK20" s="15"/>
+      <c r="BL20" s="15"/>
+      <c r="BM20" s="15"/>
+      <c r="BN20" s="15"/>
+      <c r="BO20" s="15"/>
+      <c r="BP20" s="15"/>
+      <c r="BQ20" s="15"/>
+      <c r="BR20" s="15"/>
+      <c r="BS20" s="15"/>
+      <c r="BT20" s="15"/>
+      <c r="BU20" s="15"/>
+      <c r="BV20" s="15"/>
+      <c r="BW20" s="15"/>
+      <c r="BX20" s="15"/>
+      <c r="BY20" s="15"/>
+      <c r="BZ20" s="15"/>
+      <c r="CA20" s="15"/>
+      <c r="CB20" s="16" t="s">
+        <v>277</v>
+      </c>
+      <c r="CC20" s="15"/>
+      <c r="CD20" s="15"/>
+      <c r="CE20" s="15"/>
+      <c r="CF20" s="15"/>
+      <c r="CG20" s="15"/>
+      <c r="CH20" s="15"/>
+      <c r="CI20" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ20" s="15">
+        <v>6</v>
+      </c>
+      <c r="CK20" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="CL20" s="15">
+        <v>10</v>
+      </c>
+      <c r="CM20" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="CN20" s="1"/>
+      <c r="CO20" s="16"/>
+      <c r="CP20" s="16"/>
+      <c r="CQ20" s="16"/>
+      <c r="CR20" s="16"/>
+      <c r="CS20" s="16"/>
+      <c r="CT20" s="16"/>
+      <c r="CU20" s="16" t="s">
+        <v>263</v>
+      </c>
+      <c r="CV20" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Merge Sogo smoke excel
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
+++ b/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80C96437-0CBD-4942-BC5B-B635E74D9CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA7AEFDE-C97B-4AD2-BFE7-A4A5CC2AFDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="368">
   <si>
     <t>Environment</t>
   </si>
@@ -866,9 +866,6 @@
     <t>Q 1(b). Please provide your details: Gender</t>
   </si>
   <si>
-    <t>ayadav@zarca.com</t>
-  </si>
-  <si>
     <t xml:space="preserve"> From fieldis not present on page.</t>
   </si>
   <si>
@@ -942,6 +939,273 @@
   </si>
   <si>
     <t>Smoke_TC119</t>
+  </si>
+  <si>
+    <t>Smoke_TC19</t>
+  </si>
+  <si>
+    <t>Smoke_TC20</t>
+  </si>
+  <si>
+    <t>Smoke_TC21</t>
+  </si>
+  <si>
+    <t>Smoke_TC22</t>
+  </si>
+  <si>
+    <t>Smoke_TC23</t>
+  </si>
+  <si>
+    <t>Smoke_TC24</t>
+  </si>
+  <si>
+    <t>Smoke_TC25</t>
+  </si>
+  <si>
+    <t>Smoke_TC26</t>
+  </si>
+  <si>
+    <t>Smoke_TC27</t>
+  </si>
+  <si>
+    <t>Smoke_TC28</t>
+  </si>
+  <si>
+    <t>Smoke_TC29</t>
+  </si>
+  <si>
+    <t>Smoke_TC30</t>
+  </si>
+  <si>
+    <t>Smoke_TC31</t>
+  </si>
+  <si>
+    <t>Vivek</t>
+  </si>
+  <si>
+    <t>SMX2</t>
+  </si>
+  <si>
+    <t>sogo_abhandi</t>
+  </si>
+  <si>
+    <t>Sogo@bhandi4</t>
+  </si>
+  <si>
+    <t>Logo Upload From Computer</t>
+  </si>
+  <si>
+    <t>Use account logo</t>
+  </si>
+  <si>
+    <t>Copy from another project</t>
+  </si>
+  <si>
+    <t>Insert logo using URL</t>
+  </si>
+  <si>
+    <t>Uploading JPG file</t>
+  </si>
+  <si>
+    <t>Uploading GIF file</t>
+  </si>
+  <si>
+    <t>Align logo to left</t>
+  </si>
+  <si>
+    <t>Align logo to Right</t>
+  </si>
+  <si>
+    <t>Uploading JPEG file</t>
+  </si>
+  <si>
+    <t>Logo greater than 5mb</t>
+  </si>
+  <si>
+    <t>Unsupported file for logo</t>
+  </si>
+  <si>
+    <t>Delete use account logo</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. Logo is going to upload from computer(.png). 4.After uploading  it will delete the uploaded logo</t>
+  </si>
+  <si>
+    <t>logo should be uploaded and deleted</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3.It will use account logo as survey logo</t>
+  </si>
+  <si>
+    <t>logo should be uploaded</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. It will select logo from other survey and use that copied logo as survey logo. 4.After uploading it will delete the logo</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3.With the help of the entered URL it will upload survey logo . 4.After uploading it will delete the logo</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. Logo is going to upload from computer which is .jpg format image.</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. Logo is going to upload from computer which is .gif format image.</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. Logo is going to upload from computer. 4.After uploading  it will align survey logo to left side</t>
+  </si>
+  <si>
+    <t>logo should be uploaded and align to left</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. Logo is going to upload from computer. 4.After uploading  it will align survey logo to right side</t>
+  </si>
+  <si>
+    <t>logo should be uploaded and align to right</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3. Logo is going to upload from computer which is .jpeg format image.</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3.It will try to upload image which is greater than 5 mb.</t>
+  </si>
+  <si>
+    <t>1. logo should not upload 2. should get an alert</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3.It will try to upload unsupported file</t>
+  </si>
+  <si>
+    <t>1. logo should not upload 2. should get an alert which format of files is supporting</t>
+  </si>
+  <si>
+    <t>1. It will create a new survey. 2. Add textbox question. 3.It will use account logo as survey logo.  4.After uploading  it will delete the uploaded logo</t>
+  </si>
+  <si>
+    <t>Comparison I</t>
+  </si>
+  <si>
+    <t>image of mountain.jpg</t>
+  </si>
+  <si>
+    <t>DANCING_BABY.gif</t>
+  </si>
+  <si>
+    <t>green.jpeg</t>
+  </si>
+  <si>
+    <t>hotel.jpg</t>
+  </si>
+  <si>
+    <t>pdf.pdf</t>
+  </si>
+  <si>
+    <t>Alert Box message: The Image file to upload cannot exceed 5 MB.</t>
+  </si>
+  <si>
+    <t>Alert Box message: Your file should be of the following format .gif, .jpg, .png or .jpeg.</t>
+  </si>
+  <si>
+    <t>amulla@zarca.com,vgrandhi@zarca.com</t>
+  </si>
+  <si>
+    <t>testsogo31@gmail.com</t>
+  </si>
+  <si>
+    <t>DP-POLL</t>
+  </si>
+  <si>
+    <t>Survey-Logo-20</t>
+  </si>
+  <si>
+    <t>Survey-Logo-21</t>
+  </si>
+  <si>
+    <t>1111111 do not delete (dp check)</t>
+  </si>
+  <si>
+    <t>Survey-Logo-22</t>
+  </si>
+  <si>
+    <t>Survey-Logo-23</t>
+  </si>
+  <si>
+    <t>Survey-Logo-24</t>
+  </si>
+  <si>
+    <t>Survey-Logo-25</t>
+  </si>
+  <si>
+    <t>Survey-Logo-26</t>
+  </si>
+  <si>
+    <t>Survey-Logo-27</t>
+  </si>
+  <si>
+    <t>Survey-Logo-28</t>
+  </si>
+  <si>
+    <t>Survey-Logo-29</t>
+  </si>
+  <si>
+    <t>Survey-Logo-30</t>
+  </si>
+  <si>
+    <t>Survey-Logo-31</t>
+  </si>
+  <si>
+    <t>Arabic</t>
+  </si>
+  <si>
+    <t>harley-davidson-logo-vector.png</t>
+  </si>
+  <si>
+    <t>question 1</t>
+  </si>
+  <si>
+    <t>question 2</t>
+  </si>
+  <si>
+    <t>question 3</t>
+  </si>
+  <si>
+    <t>https://image.shutterstock.com/image-vector/link-icon-hyperlink-chain-symbol-260nw-1186749931.jpg</t>
+  </si>
+  <si>
+    <t>question 4</t>
+  </si>
+  <si>
+    <t>question 5</t>
+  </si>
+  <si>
+    <t>question 6</t>
+  </si>
+  <si>
+    <t>question 8</t>
+  </si>
+  <si>
+    <t>question 9</t>
+  </si>
+  <si>
+    <t>question 10</t>
+  </si>
+  <si>
+    <t>question 11</t>
+  </si>
+  <si>
+    <t>question 12</t>
+  </si>
+  <si>
+    <t>question 13</t>
+  </si>
+  <si>
+    <t>Much less than others</t>
+  </si>
+  <si>
+    <t>surveyType</t>
+  </si>
+  <si>
+    <t>Survey</t>
   </si>
 </sst>
 </file>
@@ -1487,10 +1751,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1545,7 +1809,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>158</v>
@@ -1610,6 +1874,20 @@
         <v>248</v>
       </c>
       <c r="D8" s="25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>294</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>295</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1619,6 +1897,7 @@
     <hyperlink ref="C2" r:id="rId1" display="Prod_17.1v@2019" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="C7" r:id="rId2" xr:uid="{702B9475-C84C-4FE3-827C-5DA32183EACA}"/>
     <hyperlink ref="C8" r:id="rId3" xr:uid="{F0C2501D-C643-42A3-B68D-840128CAECCA}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{9B47117C-96DC-4F4E-832D-C8206ECDEA30}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1627,10 +1906,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:CV20"/>
+  <dimension ref="A1:CW33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="CC1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="CV20" sqref="CV20:CV32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1655,7 +1934,7 @@
     <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -1894,7 +2173,7 @@
         <v>137</v>
       </c>
       <c r="CB1" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="CC1" s="9" t="s">
         <v>138</v>
@@ -1915,19 +2194,19 @@
         <v>143</v>
       </c>
       <c r="CI1" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="CJ1" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="CK1" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="CK1" s="9" t="s">
-        <v>269</v>
-      </c>
       <c r="CL1" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="CM1" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="CM1" s="9" t="s">
-        <v>273</v>
       </c>
       <c r="CN1" s="9" t="s">
         <v>144</v>
@@ -1951,13 +2230,16 @@
         <v>150</v>
       </c>
       <c r="CU1" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="CV1" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="CW1" s="9" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -2076,8 +2358,9 @@
       <c r="CT2" s="6"/>
       <c r="CU2" s="6"/>
       <c r="CV2" s="6"/>
+      <c r="CW2" s="6"/>
     </row>
-    <row r="3" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
@@ -2091,7 +2374,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>30</v>
@@ -2274,8 +2557,9 @@
       <c r="CT3" s="15"/>
       <c r="CU3" s="15"/>
       <c r="CV3" s="15"/>
+      <c r="CW3" s="15"/>
     </row>
-    <row r="4" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>180</v>
       </c>
@@ -2406,8 +2690,9 @@
       </c>
       <c r="CU4" s="16"/>
       <c r="CV4" s="16"/>
+      <c r="CW4" s="16"/>
     </row>
-    <row r="5" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>181</v>
       </c>
@@ -2434,7 +2719,7 @@
         <v>185</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="14"/>
@@ -2540,8 +2825,9 @@
       </c>
       <c r="CU5" s="16"/>
       <c r="CV5" s="16"/>
+      <c r="CW5" s="16"/>
     </row>
-    <row r="6" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>182</v>
       </c>
@@ -2568,7 +2854,7 @@
         <v>185</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="14"/>
@@ -2664,8 +2950,9 @@
       <c r="CT6" s="16"/>
       <c r="CU6" s="16"/>
       <c r="CV6" s="16"/>
+      <c r="CW6" s="16"/>
     </row>
-    <row r="7" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>183</v>
       </c>
@@ -2788,8 +3075,9 @@
       <c r="CT7" s="16"/>
       <c r="CU7" s="16"/>
       <c r="CV7" s="16"/>
+      <c r="CW7" s="16"/>
     </row>
-    <row r="8" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>184</v>
       </c>
@@ -2914,8 +3202,9 @@
       <c r="CT8" s="19"/>
       <c r="CU8" s="19"/>
       <c r="CV8" s="19"/>
+      <c r="CW8" s="19"/>
     </row>
-    <row r="9" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>159</v>
       </c>
@@ -3044,8 +3333,9 @@
       <c r="CT9" s="1"/>
       <c r="CU9" s="1"/>
       <c r="CV9" s="1"/>
+      <c r="CW9" s="1"/>
     </row>
-    <row r="10" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>216</v>
       </c>
@@ -3072,7 +3362,7 @@
         <v>185</v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K10" s="20" t="s">
         <v>190</v>
@@ -3093,7 +3383,7 @@
       <c r="U10" s="22"/>
       <c r="V10" s="22"/>
       <c r="W10" s="27" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="X10" s="22"/>
       <c r="Y10" s="22"/>
@@ -3173,11 +3463,12 @@
       <c r="CS10" s="24"/>
       <c r="CT10" s="24"/>
       <c r="CU10" s="24"/>
-      <c r="CV10" s="24" t="s">
+      <c r="CV10" s="24"/>
+      <c r="CW10" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>217</v>
       </c>
@@ -3204,7 +3495,7 @@
         <v>185</v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="K11" s="20" t="s">
         <v>195</v>
@@ -3221,7 +3512,7 @@
       <c r="U11" s="22"/>
       <c r="V11" s="22"/>
       <c r="W11" s="27" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="X11" s="22"/>
       <c r="Y11" s="22"/>
@@ -3301,11 +3592,12 @@
       <c r="CS11" s="24"/>
       <c r="CT11" s="24"/>
       <c r="CU11" s="24"/>
-      <c r="CV11" s="24" t="s">
+      <c r="CV11" s="24"/>
+      <c r="CW11" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>218</v>
       </c>
@@ -3347,7 +3639,7 @@
       <c r="U12" s="22"/>
       <c r="V12" s="22"/>
       <c r="W12" s="27" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="X12" s="22"/>
       <c r="Y12" s="22"/>
@@ -3427,11 +3719,12 @@
       <c r="CS12" s="24"/>
       <c r="CT12" s="24"/>
       <c r="CU12" s="24"/>
-      <c r="CV12" s="24" t="s">
+      <c r="CV12" s="24"/>
+      <c r="CW12" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>219</v>
       </c>
@@ -3473,7 +3766,7 @@
       <c r="U13" s="22"/>
       <c r="V13" s="22"/>
       <c r="W13" s="27" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="X13" s="22"/>
       <c r="Y13" s="22"/>
@@ -3553,11 +3846,12 @@
       <c r="CS13" s="24"/>
       <c r="CT13" s="24"/>
       <c r="CU13" s="24"/>
-      <c r="CV13" s="24" t="s">
+      <c r="CV13" s="24"/>
+      <c r="CW13" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>220</v>
       </c>
@@ -3599,7 +3893,7 @@
       <c r="U14" s="22"/>
       <c r="V14" s="22"/>
       <c r="W14" s="27" t="s">
-        <v>254</v>
+        <v>335</v>
       </c>
       <c r="X14" s="22"/>
       <c r="Y14" s="22"/>
@@ -3679,11 +3973,12 @@
       <c r="CS14" s="24"/>
       <c r="CT14" s="24"/>
       <c r="CU14" s="24"/>
-      <c r="CV14" s="24" t="s">
+      <c r="CV14" s="24"/>
+      <c r="CW14" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="15" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>221</v>
       </c>
@@ -3710,7 +4005,7 @@
         <v>185</v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K15" s="20" t="s">
         <v>207</v>
@@ -3745,7 +4040,7 @@
       </c>
       <c r="V15" s="22"/>
       <c r="W15" s="27" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="X15" s="22"/>
       <c r="Y15" s="22"/>
@@ -3825,11 +4120,12 @@
       <c r="CS15" s="24"/>
       <c r="CT15" s="24"/>
       <c r="CU15" s="24"/>
-      <c r="CV15" s="24" t="s">
+      <c r="CV15" s="24"/>
+      <c r="CW15" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="16" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>225</v>
       </c>
@@ -3886,7 +4182,7 @@
       </c>
       <c r="V16" s="22"/>
       <c r="W16" s="27" t="s">
-        <v>254</v>
+        <v>334</v>
       </c>
       <c r="X16" s="22"/>
       <c r="Y16" s="22"/>
@@ -3966,11 +4262,12 @@
       <c r="CS16" s="24"/>
       <c r="CT16" s="24"/>
       <c r="CU16" s="24"/>
-      <c r="CV16" s="24" t="s">
+      <c r="CV16" s="24"/>
+      <c r="CW16" s="24" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>237</v>
       </c>
@@ -4091,8 +4388,9 @@
       </c>
       <c r="CU17" s="16"/>
       <c r="CV17" s="16"/>
+      <c r="CW17" s="16"/>
     </row>
-    <row r="18" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>242</v>
       </c>
@@ -4117,7 +4415,7 @@
         <v>185</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K18" s="1"/>
       <c r="L18" s="14"/>
@@ -4215,8 +4513,9 @@
       <c r="CT18" s="16"/>
       <c r="CU18" s="16"/>
       <c r="CV18" s="16"/>
+      <c r="CW18" s="16"/>
     </row>
-    <row r="19" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>249</v>
       </c>
@@ -4337,46 +4636,43 @@
       <c r="CT19" s="16"/>
       <c r="CU19" s="16"/>
       <c r="CV19" s="16"/>
+      <c r="CW19" s="16"/>
     </row>
-    <row r="20" spans="1:100" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>279</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>261</v>
+        <v>292</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>258</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>259</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="29" t="s">
-        <v>266</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>278</v>
-      </c>
+      <c r="I20" s="30"/>
+      <c r="J20" s="14"/>
       <c r="K20" s="1"/>
       <c r="L20" s="14"/>
       <c r="M20" s="14"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="P20" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="5"/>
-      <c r="V20" s="5"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
       <c r="W20" s="5"/>
       <c r="X20" s="5"/>
       <c r="Y20" s="5"/>
@@ -4390,9 +4686,7 @@
       <c r="AG20" s="5"/>
       <c r="AH20" s="5"/>
       <c r="AI20" s="5"/>
-      <c r="AJ20" s="5" t="s">
-        <v>275</v>
-      </c>
+      <c r="AJ20" s="5"/>
       <c r="AK20" s="5"/>
       <c r="AL20" s="5"/>
       <c r="AM20" s="5"/>
@@ -4401,40 +4695,28 @@
       <c r="AP20" s="15"/>
       <c r="AQ20" s="15"/>
       <c r="AR20" s="15"/>
-      <c r="AS20" s="15"/>
-      <c r="AT20" s="15" t="s">
-        <v>260</v>
-      </c>
-      <c r="AU20" s="15" t="s">
-        <v>33</v>
-      </c>
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="AU20" s="15"/>
       <c r="AV20" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="AW20" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="AX20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AY20" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AZ20" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="AW20" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="AX20" s="1"/>
+      <c r="AY20" s="1"/>
+      <c r="AZ20" s="15"/>
       <c r="BA20" s="15" t="s">
-        <v>39</v>
+        <v>365</v>
       </c>
       <c r="BB20" s="15"/>
       <c r="BC20" s="15"/>
       <c r="BD20" s="15"/>
-      <c r="BE20" s="16" t="s">
-        <v>271</v>
-      </c>
-      <c r="BF20" s="15" t="s">
-        <v>44</v>
-      </c>
+      <c r="BE20" s="16"/>
+      <c r="BF20" s="15"/>
       <c r="BG20" s="15"/>
       <c r="BH20" s="15"/>
       <c r="BI20" s="15"/>
@@ -4456,30 +4738,18 @@
       <c r="BY20" s="15"/>
       <c r="BZ20" s="15"/>
       <c r="CA20" s="15"/>
-      <c r="CB20" s="16" t="s">
-        <v>277</v>
-      </c>
+      <c r="CB20" s="15"/>
       <c r="CC20" s="15"/>
       <c r="CD20" s="15"/>
       <c r="CE20" s="15"/>
       <c r="CF20" s="15"/>
       <c r="CG20" s="15"/>
       <c r="CH20" s="15"/>
-      <c r="CI20" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="CJ20" s="15">
-        <v>6</v>
-      </c>
-      <c r="CK20" s="15" t="s">
-        <v>270</v>
-      </c>
-      <c r="CL20" s="15">
-        <v>10</v>
-      </c>
-      <c r="CM20" s="15" t="s">
-        <v>274</v>
-      </c>
+      <c r="CI20" s="15"/>
+      <c r="CJ20" s="15"/>
+      <c r="CK20" s="15"/>
+      <c r="CL20" s="15"/>
+      <c r="CM20" s="15"/>
       <c r="CN20" s="1"/>
       <c r="CO20" s="16"/>
       <c r="CP20" s="16"/>
@@ -4487,19 +4757,1698 @@
       <c r="CR20" s="16"/>
       <c r="CS20" s="16"/>
       <c r="CT20" s="16"/>
-      <c r="CU20" s="16" t="s">
-        <v>263</v>
-      </c>
-      <c r="CV20" s="16"/>
+      <c r="CU20" s="16"/>
+      <c r="CV20" s="1"/>
+      <c r="CW20" s="16"/>
+    </row>
+    <row r="21" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I21" s="30"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="1"/>
+      <c r="AO21" s="15"/>
+      <c r="AP21" s="15"/>
+      <c r="AQ21" s="15"/>
+      <c r="AR21" s="15"/>
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="AU21" s="15"/>
+      <c r="AV21" s="26"/>
+      <c r="AW21" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="AZ21" s="15"/>
+      <c r="BA21" s="15"/>
+      <c r="BB21" s="15"/>
+      <c r="BC21" s="15"/>
+      <c r="BD21" s="15"/>
+      <c r="BE21" s="16"/>
+      <c r="BF21" s="15"/>
+      <c r="BG21" s="15"/>
+      <c r="BH21" s="15"/>
+      <c r="BI21" s="15"/>
+      <c r="BJ21" s="15"/>
+      <c r="BK21" s="15"/>
+      <c r="BL21" s="15"/>
+      <c r="BM21" s="15"/>
+      <c r="BN21" s="15"/>
+      <c r="BO21" s="15"/>
+      <c r="BP21" s="15"/>
+      <c r="BQ21" s="15"/>
+      <c r="BR21" s="15"/>
+      <c r="BS21" s="15"/>
+      <c r="BT21" s="15"/>
+      <c r="BU21" s="15"/>
+      <c r="BV21" s="15"/>
+      <c r="BW21" s="15"/>
+      <c r="BX21" s="15"/>
+      <c r="BY21" s="15"/>
+      <c r="BZ21" s="15"/>
+      <c r="CA21" s="15"/>
+      <c r="CB21" s="15"/>
+      <c r="CC21" s="15"/>
+      <c r="CD21" s="15"/>
+      <c r="CE21" s="15"/>
+      <c r="CF21" s="15"/>
+      <c r="CG21" s="15"/>
+      <c r="CH21" s="15"/>
+      <c r="CI21" s="15"/>
+      <c r="CJ21" s="15"/>
+      <c r="CK21" s="15"/>
+      <c r="CL21" s="15"/>
+      <c r="CM21" s="15"/>
+      <c r="CN21" s="1"/>
+      <c r="CO21" s="16"/>
+      <c r="CP21" s="16"/>
+      <c r="CQ21" s="16"/>
+      <c r="CR21" s="16"/>
+      <c r="CS21" s="16"/>
+      <c r="CT21" s="16"/>
+      <c r="CU21" s="16"/>
+      <c r="CV21" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW21" s="16"/>
+    </row>
+    <row r="22" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I22" s="30"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5"/>
+      <c r="Y22" s="5"/>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="5"/>
+      <c r="AB22" s="5"/>
+      <c r="AC22" s="5"/>
+      <c r="AD22" s="5"/>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+      <c r="AH22" s="5"/>
+      <c r="AI22" s="5"/>
+      <c r="AJ22" s="5"/>
+      <c r="AK22" s="5"/>
+      <c r="AL22" s="5"/>
+      <c r="AM22" s="5"/>
+      <c r="AN22" s="1"/>
+      <c r="AO22" s="15"/>
+      <c r="AP22" s="15"/>
+      <c r="AQ22" s="15"/>
+      <c r="AR22" s="15"/>
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="AU22" s="15"/>
+      <c r="AV22" s="26"/>
+      <c r="AW22" s="1"/>
+      <c r="AX22" s="1"/>
+      <c r="AY22" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="AZ22" s="15"/>
+      <c r="BA22" s="15"/>
+      <c r="BB22" s="15"/>
+      <c r="BC22" s="15"/>
+      <c r="BD22" s="15"/>
+      <c r="BE22" s="16"/>
+      <c r="BF22" s="15"/>
+      <c r="BG22" s="15"/>
+      <c r="BH22" s="15"/>
+      <c r="BI22" s="15"/>
+      <c r="BJ22" s="15"/>
+      <c r="BK22" s="15"/>
+      <c r="BL22" s="15"/>
+      <c r="BM22" s="15"/>
+      <c r="BN22" s="15"/>
+      <c r="BO22" s="15"/>
+      <c r="BP22" s="15"/>
+      <c r="BQ22" s="15"/>
+      <c r="BR22" s="15"/>
+      <c r="BS22" s="15"/>
+      <c r="BT22" s="15"/>
+      <c r="BU22" s="15"/>
+      <c r="BV22" s="15"/>
+      <c r="BW22" s="15"/>
+      <c r="BX22" s="15"/>
+      <c r="BY22" s="15"/>
+      <c r="BZ22" s="15"/>
+      <c r="CA22" s="15"/>
+      <c r="CB22" s="15"/>
+      <c r="CC22" s="15"/>
+      <c r="CD22" s="15"/>
+      <c r="CE22" s="15"/>
+      <c r="CF22" s="15"/>
+      <c r="CG22" s="15"/>
+      <c r="CH22" s="15"/>
+      <c r="CI22" s="15"/>
+      <c r="CJ22" s="15"/>
+      <c r="CK22" s="15"/>
+      <c r="CL22" s="15"/>
+      <c r="CM22" s="15"/>
+      <c r="CN22" s="1"/>
+      <c r="CO22" s="16"/>
+      <c r="CP22" s="16"/>
+      <c r="CQ22" s="16"/>
+      <c r="CR22" s="16"/>
+      <c r="CS22" s="16"/>
+      <c r="CT22" s="16"/>
+      <c r="CU22" s="16"/>
+      <c r="CV22" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW22" s="16"/>
+    </row>
+    <row r="23" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I23" s="30"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="5"/>
+      <c r="X23" s="5"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
+      <c r="AC23" s="5"/>
+      <c r="AD23" s="5"/>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
+      <c r="AH23" s="5"/>
+      <c r="AI23" s="5"/>
+      <c r="AJ23" s="5"/>
+      <c r="AK23" s="5"/>
+      <c r="AL23" s="5"/>
+      <c r="AM23" s="5"/>
+      <c r="AN23" s="1"/>
+      <c r="AO23" s="15"/>
+      <c r="AP23" s="15"/>
+      <c r="AQ23" s="15"/>
+      <c r="AR23" s="15"/>
+      <c r="AS23" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="AT23" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="AU23" s="15"/>
+      <c r="AV23" s="26"/>
+      <c r="AW23" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="AX23" s="1"/>
+      <c r="AY23" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="AZ23" s="15"/>
+      <c r="BA23" s="15"/>
+      <c r="BB23" s="15"/>
+      <c r="BC23" s="15"/>
+      <c r="BD23" s="15"/>
+      <c r="BE23" s="16"/>
+      <c r="BF23" s="15"/>
+      <c r="BG23" s="15"/>
+      <c r="BH23" s="15"/>
+      <c r="BI23" s="15"/>
+      <c r="BJ23" s="15"/>
+      <c r="BK23" s="15"/>
+      <c r="BL23" s="15"/>
+      <c r="BM23" s="15"/>
+      <c r="BN23" s="15"/>
+      <c r="BO23" s="15"/>
+      <c r="BP23" s="15"/>
+      <c r="BQ23" s="15"/>
+      <c r="BR23" s="15"/>
+      <c r="BS23" s="15"/>
+      <c r="BT23" s="15"/>
+      <c r="BU23" s="15"/>
+      <c r="BV23" s="15"/>
+      <c r="BW23" s="15"/>
+      <c r="BX23" s="15"/>
+      <c r="BY23" s="15"/>
+      <c r="BZ23" s="15"/>
+      <c r="CA23" s="15"/>
+      <c r="CB23" s="15"/>
+      <c r="CC23" s="15"/>
+      <c r="CD23" s="15"/>
+      <c r="CE23" s="15"/>
+      <c r="CF23" s="15"/>
+      <c r="CG23" s="15"/>
+      <c r="CH23" s="15"/>
+      <c r="CI23" s="15"/>
+      <c r="CJ23" s="15"/>
+      <c r="CK23" s="15"/>
+      <c r="CL23" s="15"/>
+      <c r="CM23" s="15"/>
+      <c r="CN23" s="1"/>
+      <c r="CO23" s="16"/>
+      <c r="CP23" s="16"/>
+      <c r="CQ23" s="16"/>
+      <c r="CR23" s="16"/>
+      <c r="CS23" s="16"/>
+      <c r="CT23" s="16"/>
+      <c r="CU23" s="16"/>
+      <c r="CV23" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW23" s="16"/>
+    </row>
+    <row r="24" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I24" s="30"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5"/>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="5"/>
+      <c r="AB24" s="5"/>
+      <c r="AC24" s="5"/>
+      <c r="AD24" s="5"/>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AG24" s="5"/>
+      <c r="AH24" s="5"/>
+      <c r="AI24" s="5"/>
+      <c r="AJ24" s="5"/>
+      <c r="AK24" s="5"/>
+      <c r="AL24" s="5"/>
+      <c r="AM24" s="5"/>
+      <c r="AN24" s="1"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
+      <c r="AQ24" s="15"/>
+      <c r="AR24" s="15"/>
+      <c r="AS24" s="1"/>
+      <c r="AT24" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="AU24" s="15"/>
+      <c r="AV24" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="AW24" s="1"/>
+      <c r="AX24" s="1"/>
+      <c r="AY24" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="AZ24" s="15"/>
+      <c r="BA24" s="15"/>
+      <c r="BB24" s="15"/>
+      <c r="BC24" s="15"/>
+      <c r="BD24" s="15"/>
+      <c r="BE24" s="16"/>
+      <c r="BF24" s="15"/>
+      <c r="BG24" s="15"/>
+      <c r="BH24" s="15"/>
+      <c r="BI24" s="15"/>
+      <c r="BJ24" s="15"/>
+      <c r="BK24" s="15"/>
+      <c r="BL24" s="15"/>
+      <c r="BM24" s="15"/>
+      <c r="BN24" s="15"/>
+      <c r="BO24" s="15"/>
+      <c r="BP24" s="15"/>
+      <c r="BQ24" s="15"/>
+      <c r="BR24" s="15"/>
+      <c r="BS24" s="15"/>
+      <c r="BT24" s="15"/>
+      <c r="BU24" s="15"/>
+      <c r="BV24" s="15"/>
+      <c r="BW24" s="15"/>
+      <c r="BX24" s="15"/>
+      <c r="BY24" s="15"/>
+      <c r="BZ24" s="15"/>
+      <c r="CA24" s="15"/>
+      <c r="CB24" s="15"/>
+      <c r="CC24" s="15"/>
+      <c r="CD24" s="15"/>
+      <c r="CE24" s="15"/>
+      <c r="CF24" s="15"/>
+      <c r="CG24" s="15"/>
+      <c r="CH24" s="15"/>
+      <c r="CI24" s="15"/>
+      <c r="CJ24" s="15"/>
+      <c r="CK24" s="15"/>
+      <c r="CL24" s="15"/>
+      <c r="CM24" s="15"/>
+      <c r="CN24" s="1"/>
+      <c r="CO24" s="16"/>
+      <c r="CP24" s="16"/>
+      <c r="CQ24" s="16"/>
+      <c r="CR24" s="16"/>
+      <c r="CS24" s="16"/>
+      <c r="CT24" s="16"/>
+      <c r="CU24" s="16"/>
+      <c r="CV24" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW24" s="16"/>
+    </row>
+    <row r="25" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I25" s="30"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="5"/>
+      <c r="X25" s="5"/>
+      <c r="Y25" s="5"/>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="5"/>
+      <c r="AB25" s="5"/>
+      <c r="AC25" s="5"/>
+      <c r="AD25" s="5"/>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="1"/>
+      <c r="AO25" s="15"/>
+      <c r="AP25" s="15"/>
+      <c r="AQ25" s="15"/>
+      <c r="AR25" s="15"/>
+      <c r="AS25" s="1"/>
+      <c r="AT25" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AU25" s="15"/>
+      <c r="AV25" s="26"/>
+      <c r="AW25" s="1"/>
+      <c r="AX25" s="1"/>
+      <c r="AY25" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="AZ25" s="15"/>
+      <c r="BA25" s="15"/>
+      <c r="BB25" s="15"/>
+      <c r="BC25" s="15"/>
+      <c r="BD25" s="15"/>
+      <c r="BE25" s="16"/>
+      <c r="BF25" s="15"/>
+      <c r="BG25" s="15"/>
+      <c r="BH25" s="15"/>
+      <c r="BI25" s="15"/>
+      <c r="BJ25" s="15"/>
+      <c r="BK25" s="15"/>
+      <c r="BL25" s="15"/>
+      <c r="BM25" s="15"/>
+      <c r="BN25" s="15"/>
+      <c r="BO25" s="15"/>
+      <c r="BP25" s="15"/>
+      <c r="BQ25" s="15"/>
+      <c r="BR25" s="15"/>
+      <c r="BS25" s="15"/>
+      <c r="BT25" s="15"/>
+      <c r="BU25" s="15"/>
+      <c r="BV25" s="15"/>
+      <c r="BW25" s="15"/>
+      <c r="BX25" s="15"/>
+      <c r="BY25" s="15"/>
+      <c r="BZ25" s="15"/>
+      <c r="CA25" s="15"/>
+      <c r="CB25" s="15"/>
+      <c r="CC25" s="15"/>
+      <c r="CD25" s="15"/>
+      <c r="CE25" s="15"/>
+      <c r="CF25" s="15"/>
+      <c r="CG25" s="15"/>
+      <c r="CH25" s="15"/>
+      <c r="CI25" s="15"/>
+      <c r="CJ25" s="15"/>
+      <c r="CK25" s="15"/>
+      <c r="CL25" s="15"/>
+      <c r="CM25" s="15"/>
+      <c r="CN25" s="1"/>
+      <c r="CO25" s="16"/>
+      <c r="CP25" s="16"/>
+      <c r="CQ25" s="16"/>
+      <c r="CR25" s="16"/>
+      <c r="CS25" s="16"/>
+      <c r="CT25" s="16"/>
+      <c r="CU25" s="16"/>
+      <c r="CV25" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW25" s="16"/>
+    </row>
+    <row r="26" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I26" s="30"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="5"/>
+      <c r="X26" s="5"/>
+      <c r="Y26" s="5"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="5"/>
+      <c r="AB26" s="5"/>
+      <c r="AC26" s="5"/>
+      <c r="AD26" s="5"/>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="1"/>
+      <c r="AO26" s="15"/>
+      <c r="AP26" s="15"/>
+      <c r="AQ26" s="15"/>
+      <c r="AR26" s="15"/>
+      <c r="AS26" s="1"/>
+      <c r="AT26" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="AU26" s="15"/>
+      <c r="AV26" s="26"/>
+      <c r="AW26" s="1"/>
+      <c r="AX26" s="1"/>
+      <c r="AY26" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="AZ26" s="15"/>
+      <c r="BA26" s="15"/>
+      <c r="BB26" s="15"/>
+      <c r="BC26" s="15"/>
+      <c r="BD26" s="15"/>
+      <c r="BE26" s="16"/>
+      <c r="BF26" s="15"/>
+      <c r="BG26" s="15"/>
+      <c r="BH26" s="15"/>
+      <c r="BI26" s="15"/>
+      <c r="BJ26" s="15"/>
+      <c r="BK26" s="15"/>
+      <c r="BL26" s="15"/>
+      <c r="BM26" s="15"/>
+      <c r="BN26" s="15"/>
+      <c r="BO26" s="15"/>
+      <c r="BP26" s="15"/>
+      <c r="BQ26" s="15"/>
+      <c r="BR26" s="15"/>
+      <c r="BS26" s="15"/>
+      <c r="BT26" s="15"/>
+      <c r="BU26" s="15"/>
+      <c r="BV26" s="15"/>
+      <c r="BW26" s="15"/>
+      <c r="BX26" s="15"/>
+      <c r="BY26" s="15"/>
+      <c r="BZ26" s="15"/>
+      <c r="CA26" s="15"/>
+      <c r="CB26" s="15"/>
+      <c r="CC26" s="15"/>
+      <c r="CD26" s="15"/>
+      <c r="CE26" s="15"/>
+      <c r="CF26" s="15"/>
+      <c r="CG26" s="15"/>
+      <c r="CH26" s="15"/>
+      <c r="CI26" s="15"/>
+      <c r="CJ26" s="15"/>
+      <c r="CK26" s="15"/>
+      <c r="CL26" s="15"/>
+      <c r="CM26" s="15"/>
+      <c r="CN26" s="1"/>
+      <c r="CO26" s="16"/>
+      <c r="CP26" s="16"/>
+      <c r="CQ26" s="16"/>
+      <c r="CR26" s="16"/>
+      <c r="CS26" s="16"/>
+      <c r="CT26" s="16"/>
+      <c r="CU26" s="16"/>
+      <c r="CV26" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW26" s="16"/>
+    </row>
+    <row r="27" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="I27" s="30"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5"/>
+      <c r="Y27" s="5"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="5"/>
+      <c r="AB27" s="5"/>
+      <c r="AC27" s="5"/>
+      <c r="AD27" s="5"/>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="1"/>
+      <c r="AO27" s="15"/>
+      <c r="AP27" s="15"/>
+      <c r="AQ27" s="15"/>
+      <c r="AR27" s="15"/>
+      <c r="AS27" s="1"/>
+      <c r="AT27" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="AU27" s="15"/>
+      <c r="AV27" s="26"/>
+      <c r="AW27" s="1"/>
+      <c r="AX27" s="1"/>
+      <c r="AY27" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="AZ27" s="15"/>
+      <c r="BA27" s="15"/>
+      <c r="BB27" s="15"/>
+      <c r="BC27" s="15"/>
+      <c r="BD27" s="15"/>
+      <c r="BE27" s="16"/>
+      <c r="BF27" s="15"/>
+      <c r="BG27" s="15"/>
+      <c r="BH27" s="15"/>
+      <c r="BI27" s="15"/>
+      <c r="BJ27" s="15"/>
+      <c r="BK27" s="15"/>
+      <c r="BL27" s="15"/>
+      <c r="BM27" s="15"/>
+      <c r="BN27" s="15"/>
+      <c r="BO27" s="15"/>
+      <c r="BP27" s="15"/>
+      <c r="BQ27" s="15"/>
+      <c r="BR27" s="15"/>
+      <c r="BS27" s="15"/>
+      <c r="BT27" s="15"/>
+      <c r="BU27" s="15"/>
+      <c r="BV27" s="15"/>
+      <c r="BW27" s="15"/>
+      <c r="BX27" s="15"/>
+      <c r="BY27" s="15"/>
+      <c r="BZ27" s="15"/>
+      <c r="CA27" s="15"/>
+      <c r="CB27" s="15"/>
+      <c r="CC27" s="15"/>
+      <c r="CD27" s="15"/>
+      <c r="CE27" s="15"/>
+      <c r="CF27" s="15"/>
+      <c r="CG27" s="15"/>
+      <c r="CH27" s="15"/>
+      <c r="CI27" s="15"/>
+      <c r="CJ27" s="15"/>
+      <c r="CK27" s="15"/>
+      <c r="CL27" s="15"/>
+      <c r="CM27" s="15"/>
+      <c r="CN27" s="1"/>
+      <c r="CO27" s="16"/>
+      <c r="CP27" s="16"/>
+      <c r="CQ27" s="16"/>
+      <c r="CR27" s="16"/>
+      <c r="CS27" s="16"/>
+      <c r="CT27" s="16"/>
+      <c r="CU27" s="16"/>
+      <c r="CV27" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW27" s="16"/>
+    </row>
+    <row r="28" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="I28" s="30"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="5"/>
+      <c r="X28" s="5"/>
+      <c r="Y28" s="5"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="5"/>
+      <c r="AB28" s="5"/>
+      <c r="AC28" s="5"/>
+      <c r="AD28" s="5"/>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+      <c r="AH28" s="5"/>
+      <c r="AI28" s="5"/>
+      <c r="AJ28" s="5"/>
+      <c r="AK28" s="5"/>
+      <c r="AL28" s="5"/>
+      <c r="AM28" s="5"/>
+      <c r="AN28" s="1"/>
+      <c r="AO28" s="15"/>
+      <c r="AP28" s="15"/>
+      <c r="AQ28" s="15"/>
+      <c r="AR28" s="15"/>
+      <c r="AS28" s="1"/>
+      <c r="AT28" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="AU28" s="15"/>
+      <c r="AV28" s="26"/>
+      <c r="AW28" s="1"/>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="AZ28" s="15"/>
+      <c r="BA28" s="15"/>
+      <c r="BB28" s="15"/>
+      <c r="BC28" s="15"/>
+      <c r="BD28" s="15"/>
+      <c r="BE28" s="16"/>
+      <c r="BF28" s="15"/>
+      <c r="BG28" s="15"/>
+      <c r="BH28" s="15"/>
+      <c r="BI28" s="15"/>
+      <c r="BJ28" s="15"/>
+      <c r="BK28" s="15"/>
+      <c r="BL28" s="15"/>
+      <c r="BM28" s="15"/>
+      <c r="BN28" s="15"/>
+      <c r="BO28" s="15"/>
+      <c r="BP28" s="15"/>
+      <c r="BQ28" s="15"/>
+      <c r="BR28" s="15"/>
+      <c r="BS28" s="15"/>
+      <c r="BT28" s="15"/>
+      <c r="BU28" s="15"/>
+      <c r="BV28" s="15"/>
+      <c r="BW28" s="15"/>
+      <c r="BX28" s="15"/>
+      <c r="BY28" s="15"/>
+      <c r="BZ28" s="15"/>
+      <c r="CA28" s="15"/>
+      <c r="CB28" s="15"/>
+      <c r="CC28" s="15"/>
+      <c r="CD28" s="15"/>
+      <c r="CE28" s="15"/>
+      <c r="CF28" s="15"/>
+      <c r="CG28" s="15"/>
+      <c r="CH28" s="15"/>
+      <c r="CI28" s="15"/>
+      <c r="CJ28" s="15"/>
+      <c r="CK28" s="15"/>
+      <c r="CL28" s="15"/>
+      <c r="CM28" s="15"/>
+      <c r="CN28" s="1"/>
+      <c r="CO28" s="16"/>
+      <c r="CP28" s="16"/>
+      <c r="CQ28" s="16"/>
+      <c r="CR28" s="16"/>
+      <c r="CS28" s="16"/>
+      <c r="CT28" s="16"/>
+      <c r="CU28" s="16"/>
+      <c r="CV28" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW28" s="16"/>
+    </row>
+    <row r="29" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="I29" s="30"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="5"/>
+      <c r="X29" s="5"/>
+      <c r="Y29" s="5"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="5"/>
+      <c r="AB29" s="5"/>
+      <c r="AC29" s="5"/>
+      <c r="AD29" s="5"/>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+      <c r="AH29" s="5"/>
+      <c r="AI29" s="5"/>
+      <c r="AJ29" s="5"/>
+      <c r="AK29" s="5"/>
+      <c r="AL29" s="5"/>
+      <c r="AM29" s="5"/>
+      <c r="AN29" s="1"/>
+      <c r="AO29" s="15"/>
+      <c r="AP29" s="15"/>
+      <c r="AQ29" s="15"/>
+      <c r="AR29" s="15"/>
+      <c r="AS29" s="1"/>
+      <c r="AT29" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="AU29" s="15"/>
+      <c r="AV29" s="26"/>
+      <c r="AW29" s="1"/>
+      <c r="AX29" s="1"/>
+      <c r="AY29" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="AZ29" s="15"/>
+      <c r="BA29" s="15"/>
+      <c r="BB29" s="15"/>
+      <c r="BC29" s="15"/>
+      <c r="BD29" s="15"/>
+      <c r="BE29" s="16"/>
+      <c r="BF29" s="15"/>
+      <c r="BG29" s="15"/>
+      <c r="BH29" s="15"/>
+      <c r="BI29" s="15"/>
+      <c r="BJ29" s="15"/>
+      <c r="BK29" s="15"/>
+      <c r="BL29" s="15"/>
+      <c r="BM29" s="15"/>
+      <c r="BN29" s="15"/>
+      <c r="BO29" s="15"/>
+      <c r="BP29" s="15"/>
+      <c r="BQ29" s="15"/>
+      <c r="BR29" s="15"/>
+      <c r="BS29" s="15"/>
+      <c r="BT29" s="15"/>
+      <c r="BU29" s="15"/>
+      <c r="BV29" s="15"/>
+      <c r="BW29" s="15"/>
+      <c r="BX29" s="15"/>
+      <c r="BY29" s="15"/>
+      <c r="BZ29" s="15"/>
+      <c r="CA29" s="15"/>
+      <c r="CB29" s="15"/>
+      <c r="CC29" s="15"/>
+      <c r="CD29" s="15"/>
+      <c r="CE29" s="15"/>
+      <c r="CF29" s="15"/>
+      <c r="CG29" s="15"/>
+      <c r="CH29" s="15"/>
+      <c r="CI29" s="15"/>
+      <c r="CJ29" s="15"/>
+      <c r="CK29" s="15"/>
+      <c r="CL29" s="15"/>
+      <c r="CM29" s="15"/>
+      <c r="CN29" s="1"/>
+      <c r="CO29" s="16"/>
+      <c r="CP29" s="16"/>
+      <c r="CQ29" s="16"/>
+      <c r="CR29" s="16"/>
+      <c r="CS29" s="16"/>
+      <c r="CT29" s="16"/>
+      <c r="CU29" s="16"/>
+      <c r="CV29" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW29" s="16"/>
+    </row>
+    <row r="30" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="I30" s="30"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="W30" s="5"/>
+      <c r="X30" s="5"/>
+      <c r="Y30" s="5"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="5"/>
+      <c r="AB30" s="5"/>
+      <c r="AC30" s="5"/>
+      <c r="AD30" s="5"/>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+      <c r="AH30" s="5"/>
+      <c r="AI30" s="5"/>
+      <c r="AJ30" s="5"/>
+      <c r="AK30" s="5"/>
+      <c r="AL30" s="5"/>
+      <c r="AM30" s="5"/>
+      <c r="AN30" s="1"/>
+      <c r="AO30" s="15"/>
+      <c r="AP30" s="15"/>
+      <c r="AQ30" s="15"/>
+      <c r="AR30" s="15"/>
+      <c r="AS30" s="1"/>
+      <c r="AT30" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="AU30" s="15"/>
+      <c r="AV30" s="26"/>
+      <c r="AW30" s="1"/>
+      <c r="AX30" s="1"/>
+      <c r="AY30" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="AZ30" s="15"/>
+      <c r="BA30" s="15"/>
+      <c r="BB30" s="15"/>
+      <c r="BC30" s="15"/>
+      <c r="BD30" s="15"/>
+      <c r="BE30" s="16"/>
+      <c r="BF30" s="15"/>
+      <c r="BG30" s="15"/>
+      <c r="BH30" s="15"/>
+      <c r="BI30" s="15"/>
+      <c r="BJ30" s="15"/>
+      <c r="BK30" s="15"/>
+      <c r="BL30" s="15"/>
+      <c r="BM30" s="15"/>
+      <c r="BN30" s="15"/>
+      <c r="BO30" s="15"/>
+      <c r="BP30" s="15"/>
+      <c r="BQ30" s="15"/>
+      <c r="BR30" s="15"/>
+      <c r="BS30" s="15"/>
+      <c r="BT30" s="15"/>
+      <c r="BU30" s="15"/>
+      <c r="BV30" s="15"/>
+      <c r="BW30" s="15"/>
+      <c r="BX30" s="15"/>
+      <c r="BY30" s="15"/>
+      <c r="BZ30" s="15"/>
+      <c r="CA30" s="15"/>
+      <c r="CB30" s="15"/>
+      <c r="CC30" s="15"/>
+      <c r="CD30" s="15"/>
+      <c r="CE30" s="15"/>
+      <c r="CF30" s="15"/>
+      <c r="CG30" s="15"/>
+      <c r="CH30" s="15"/>
+      <c r="CI30" s="15"/>
+      <c r="CJ30" s="15"/>
+      <c r="CK30" s="15"/>
+      <c r="CL30" s="15"/>
+      <c r="CM30" s="15"/>
+      <c r="CN30" s="1"/>
+      <c r="CO30" s="16"/>
+      <c r="CP30" s="16"/>
+      <c r="CQ30" s="16"/>
+      <c r="CR30" s="16"/>
+      <c r="CS30" s="16"/>
+      <c r="CT30" s="16"/>
+      <c r="CU30" s="16"/>
+      <c r="CV30" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW30" s="16"/>
+    </row>
+    <row r="31" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="I31" s="30"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="U31" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="V31" s="1"/>
+      <c r="W31" s="5"/>
+      <c r="X31" s="5"/>
+      <c r="Y31" s="5"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="5"/>
+      <c r="AB31" s="5"/>
+      <c r="AC31" s="5"/>
+      <c r="AD31" s="5"/>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+      <c r="AH31" s="5"/>
+      <c r="AI31" s="5"/>
+      <c r="AJ31" s="5"/>
+      <c r="AK31" s="5"/>
+      <c r="AL31" s="5"/>
+      <c r="AM31" s="5"/>
+      <c r="AN31" s="1"/>
+      <c r="AO31" s="15"/>
+      <c r="AP31" s="15"/>
+      <c r="AQ31" s="15"/>
+      <c r="AR31" s="15"/>
+      <c r="AS31" s="1"/>
+      <c r="AT31" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="AU31" s="15"/>
+      <c r="AV31" s="26"/>
+      <c r="AW31" s="1"/>
+      <c r="AX31" s="1"/>
+      <c r="AY31" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="AZ31" s="15"/>
+      <c r="BA31" s="15"/>
+      <c r="BB31" s="15"/>
+      <c r="BC31" s="15"/>
+      <c r="BD31" s="15"/>
+      <c r="BE31" s="16"/>
+      <c r="BF31" s="15"/>
+      <c r="BG31" s="15"/>
+      <c r="BH31" s="15"/>
+      <c r="BI31" s="15"/>
+      <c r="BJ31" s="15"/>
+      <c r="BK31" s="15"/>
+      <c r="BL31" s="15"/>
+      <c r="BM31" s="15"/>
+      <c r="BN31" s="15"/>
+      <c r="BO31" s="15"/>
+      <c r="BP31" s="15"/>
+      <c r="BQ31" s="15"/>
+      <c r="BR31" s="15"/>
+      <c r="BS31" s="15"/>
+      <c r="BT31" s="15"/>
+      <c r="BU31" s="15"/>
+      <c r="BV31" s="15"/>
+      <c r="BW31" s="15"/>
+      <c r="BX31" s="15"/>
+      <c r="BY31" s="15"/>
+      <c r="BZ31" s="15"/>
+      <c r="CA31" s="15"/>
+      <c r="CB31" s="15"/>
+      <c r="CC31" s="15"/>
+      <c r="CD31" s="15"/>
+      <c r="CE31" s="15"/>
+      <c r="CF31" s="15"/>
+      <c r="CG31" s="15"/>
+      <c r="CH31" s="15"/>
+      <c r="CI31" s="15"/>
+      <c r="CJ31" s="15"/>
+      <c r="CK31" s="15"/>
+      <c r="CL31" s="15"/>
+      <c r="CM31" s="15"/>
+      <c r="CN31" s="1"/>
+      <c r="CO31" s="16"/>
+      <c r="CP31" s="16"/>
+      <c r="CQ31" s="16"/>
+      <c r="CR31" s="16"/>
+      <c r="CS31" s="16"/>
+      <c r="CT31" s="16"/>
+      <c r="CU31" s="16"/>
+      <c r="CV31" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW31" s="16"/>
+    </row>
+    <row r="32" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="I32" s="30"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="5"/>
+      <c r="AH32" s="5"/>
+      <c r="AI32" s="5"/>
+      <c r="AJ32" s="5"/>
+      <c r="AK32" s="5"/>
+      <c r="AL32" s="5"/>
+      <c r="AM32" s="5"/>
+      <c r="AN32" s="1"/>
+      <c r="AO32" s="15"/>
+      <c r="AP32" s="15"/>
+      <c r="AQ32" s="15"/>
+      <c r="AR32" s="15"/>
+      <c r="AS32" s="1"/>
+      <c r="AT32" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="AU32" s="15"/>
+      <c r="AV32" s="1"/>
+      <c r="AW32" s="1"/>
+      <c r="AX32" s="1"/>
+      <c r="AY32" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="AZ32" s="15"/>
+      <c r="BA32" s="15"/>
+      <c r="BB32" s="15"/>
+      <c r="BC32" s="15"/>
+      <c r="BD32" s="15"/>
+      <c r="BE32" s="16"/>
+      <c r="BF32" s="15"/>
+      <c r="BG32" s="15"/>
+      <c r="BH32" s="15"/>
+      <c r="BI32" s="15"/>
+      <c r="BJ32" s="15"/>
+      <c r="BK32" s="15"/>
+      <c r="BL32" s="15"/>
+      <c r="BM32" s="15"/>
+      <c r="BN32" s="15"/>
+      <c r="BO32" s="15"/>
+      <c r="BP32" s="15"/>
+      <c r="BQ32" s="15"/>
+      <c r="BR32" s="15"/>
+      <c r="BS32" s="15"/>
+      <c r="BT32" s="15"/>
+      <c r="BU32" s="15"/>
+      <c r="BV32" s="15"/>
+      <c r="BW32" s="15"/>
+      <c r="BX32" s="15"/>
+      <c r="BY32" s="15"/>
+      <c r="BZ32" s="15"/>
+      <c r="CA32" s="15"/>
+      <c r="CB32" s="15"/>
+      <c r="CC32" s="15"/>
+      <c r="CD32" s="15"/>
+      <c r="CE32" s="15"/>
+      <c r="CF32" s="15"/>
+      <c r="CG32" s="15"/>
+      <c r="CH32" s="15"/>
+      <c r="CI32" s="15"/>
+      <c r="CJ32" s="15"/>
+      <c r="CK32" s="15"/>
+      <c r="CL32" s="15"/>
+      <c r="CM32" s="15"/>
+      <c r="CN32" s="1"/>
+      <c r="CO32" s="16"/>
+      <c r="CP32" s="16"/>
+      <c r="CQ32" s="16"/>
+      <c r="CR32" s="16"/>
+      <c r="CS32" s="16"/>
+      <c r="CT32" s="16"/>
+      <c r="CU32" s="16"/>
+      <c r="CV32" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="CW32" s="16"/>
+    </row>
+    <row r="33" spans="1:101" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="J33" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="K33" s="1"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="5"/>
+      <c r="AH33" s="5"/>
+      <c r="AI33" s="5"/>
+      <c r="AJ33" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="AK33" s="5"/>
+      <c r="AL33" s="5"/>
+      <c r="AM33" s="5"/>
+      <c r="AN33" s="1"/>
+      <c r="AO33" s="15"/>
+      <c r="AP33" s="15"/>
+      <c r="AQ33" s="15"/>
+      <c r="AR33" s="15"/>
+      <c r="AS33" s="15"/>
+      <c r="AT33" s="15" t="s">
+        <v>259</v>
+      </c>
+      <c r="AU33" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="AV33" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW33" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="AX33" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="AY33" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="AZ33" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="BA33" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="BB33" s="15"/>
+      <c r="BC33" s="15"/>
+      <c r="BD33" s="15"/>
+      <c r="BE33" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="BF33" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="BG33" s="15"/>
+      <c r="BH33" s="15"/>
+      <c r="BI33" s="15"/>
+      <c r="BJ33" s="15"/>
+      <c r="BK33" s="15"/>
+      <c r="BL33" s="15"/>
+      <c r="BM33" s="15"/>
+      <c r="BN33" s="15"/>
+      <c r="BO33" s="15"/>
+      <c r="BP33" s="15"/>
+      <c r="BQ33" s="15"/>
+      <c r="BR33" s="15"/>
+      <c r="BS33" s="15"/>
+      <c r="BT33" s="15"/>
+      <c r="BU33" s="15"/>
+      <c r="BV33" s="15"/>
+      <c r="BW33" s="15"/>
+      <c r="BX33" s="15"/>
+      <c r="BY33" s="15"/>
+      <c r="BZ33" s="15"/>
+      <c r="CA33" s="15"/>
+      <c r="CB33" s="16" t="s">
+        <v>276</v>
+      </c>
+      <c r="CC33" s="15"/>
+      <c r="CD33" s="15"/>
+      <c r="CE33" s="15"/>
+      <c r="CF33" s="15"/>
+      <c r="CG33" s="15"/>
+      <c r="CH33" s="15"/>
+      <c r="CI33" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="CJ33" s="15">
+        <v>6</v>
+      </c>
+      <c r="CK33" s="15" t="s">
+        <v>269</v>
+      </c>
+      <c r="CL33" s="15">
+        <v>10</v>
+      </c>
+      <c r="CM33" s="15" t="s">
+        <v>273</v>
+      </c>
+      <c r="CN33" s="1"/>
+      <c r="CO33" s="16"/>
+      <c r="CP33" s="16"/>
+      <c r="CQ33" s="16"/>
+      <c r="CR33" s="16"/>
+      <c r="CS33" s="16"/>
+      <c r="CT33" s="16"/>
+      <c r="CU33" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="CV33" s="16"/>
+      <c r="CW33" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="Q2" r:id="rId1" display="nehatest100@gmail.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-    <hyperlink ref="W10" r:id="rId2" xr:uid="{9E455840-DC38-468E-816E-C20661A2FB36}"/>
-    <hyperlink ref="W11:W16" r:id="rId3" display="ayadav@zarca.com" xr:uid="{CE6B9826-BFAB-41F0-B871-4C1950B5E4BF}"/>
+    <hyperlink ref="W10" r:id="rId2" display="ayadav@zarca.com" xr:uid="{9E455840-DC38-468E-816E-C20661A2FB36}"/>
+    <hyperlink ref="W11:W16" r:id="rId3" display="ayadav@zarca.com" xr:uid="{84B4F6F0-61CD-43DE-8B70-EB09A9D93DC7}"/>
+    <hyperlink ref="W14" r:id="rId4" xr:uid="{8C71C607-2682-4605-B2F2-128FAE06F1D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
errors occured because of keys and sogo excel
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
+++ b/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="527">
   <si>
     <t>Environment</t>
   </si>
@@ -1729,6 +1729,9 @@
   </si>
   <si>
     <t>header and footer 74</t>
+  </si>
+  <si>
+    <t>Dp poll</t>
   </si>
 </sst>
 </file>
@@ -2435,8 +2438,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CW65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5181,7 +5184,9 @@
       <c r="E20" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>526</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="30"/>
@@ -6964,7 +6969,9 @@
       <c r="CU33" s="16" t="s">
         <v>262</v>
       </c>
-      <c r="CV33" s="16"/>
+      <c r="CV33" s="1" t="s">
+        <v>367</v>
+      </c>
       <c r="CW33" s="16"/>
     </row>
     <row r="34" spans="1:101" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -6992,8 +6999,8 @@
       <c r="H34" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="I34" s="29" t="s">
-        <v>265</v>
+      <c r="I34" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -7047,49 +7054,56 @@
       </c>
       <c r="AZ34" s="1"/>
       <c r="BA34" s="1"/>
-      <c r="BB34" s="1"/>
-      <c r="BC34" s="1"/>
-      <c r="BD34" s="1"/>
-      <c r="BE34" s="1"/>
-      <c r="BF34" s="1"/>
-      <c r="BG34" s="1"/>
-      <c r="BH34" s="1"/>
-      <c r="BI34" s="1"/>
-      <c r="BJ34" s="1"/>
-      <c r="BK34" s="1"/>
-      <c r="BL34" s="1"/>
-      <c r="BM34" s="1"/>
-      <c r="BN34" s="1"/>
-      <c r="BO34" s="1"/>
-      <c r="BP34" s="1"/>
-      <c r="BQ34" s="1"/>
-      <c r="BR34" s="1"/>
-      <c r="BS34" s="1"/>
-      <c r="BT34" s="1"/>
-      <c r="BU34" s="1"/>
-      <c r="BV34" s="1"/>
-      <c r="BW34" s="1"/>
-      <c r="BX34" s="1"/>
-      <c r="BY34" s="1"/>
-      <c r="BZ34" s="1"/>
-      <c r="CA34" s="1"/>
-      <c r="CB34" s="1"/>
-      <c r="CC34" s="1"/>
-      <c r="CD34" s="1"/>
-      <c r="CE34" s="1"/>
-      <c r="CF34" s="1"/>
-      <c r="CG34" s="1"/>
-      <c r="CH34" s="1"/>
-      <c r="CI34" s="1"/>
-      <c r="CJ34" s="1"/>
-      <c r="CK34" s="1"/>
-      <c r="CL34" s="1"/>
-      <c r="CM34" s="1"/>
+      <c r="BB34" s="15"/>
+      <c r="BC34" s="15"/>
+      <c r="BD34" s="15"/>
+      <c r="BE34" s="16"/>
+      <c r="BF34" s="15"/>
+      <c r="BG34" s="15"/>
+      <c r="BH34" s="15"/>
+      <c r="BI34" s="15"/>
+      <c r="BJ34" s="15"/>
+      <c r="BK34" s="15"/>
+      <c r="BL34" s="15"/>
+      <c r="BM34" s="15"/>
+      <c r="BN34" s="15"/>
+      <c r="BO34" s="15"/>
+      <c r="BP34" s="15"/>
+      <c r="BQ34" s="15"/>
+      <c r="BR34" s="15"/>
+      <c r="BS34" s="15"/>
+      <c r="BT34" s="15"/>
+      <c r="BU34" s="15"/>
+      <c r="BV34" s="15"/>
+      <c r="BW34" s="15"/>
+      <c r="BX34" s="15"/>
+      <c r="BY34" s="15"/>
+      <c r="BZ34" s="15"/>
+      <c r="CA34" s="15"/>
+      <c r="CB34" s="16"/>
+      <c r="CC34" s="15"/>
+      <c r="CD34" s="15"/>
+      <c r="CE34" s="15"/>
+      <c r="CF34" s="15"/>
+      <c r="CG34" s="15"/>
+      <c r="CH34" s="15"/>
+      <c r="CI34" s="15"/>
+      <c r="CJ34" s="15"/>
+      <c r="CK34" s="15"/>
+      <c r="CL34" s="15"/>
+      <c r="CM34" s="15"/>
       <c r="CN34" s="1"/>
-      <c r="CO34" s="1" t="s">
+      <c r="CO34" s="16"/>
+      <c r="CP34" s="16"/>
+      <c r="CQ34" s="16"/>
+      <c r="CR34" s="16"/>
+      <c r="CS34" s="16"/>
+      <c r="CT34" s="16"/>
+      <c r="CU34" s="16"/>
+      <c r="CV34" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP34" s="1"/>
+      <c r="CW34" s="16"/>
     </row>
     <row r="35" spans="1:101" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
@@ -7116,8 +7130,8 @@
       <c r="H35" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="I35" s="29" t="s">
-        <v>265</v>
+      <c r="I35" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -7171,49 +7185,56 @@
       <c r="BA35" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="BB35" s="1"/>
-      <c r="BC35" s="1"/>
-      <c r="BD35" s="1"/>
-      <c r="BE35" s="1"/>
-      <c r="BF35" s="1"/>
-      <c r="BG35" s="1"/>
-      <c r="BH35" s="1"/>
-      <c r="BI35" s="1"/>
-      <c r="BJ35" s="1"/>
-      <c r="BK35" s="1"/>
-      <c r="BL35" s="1"/>
-      <c r="BM35" s="1"/>
-      <c r="BN35" s="1"/>
-      <c r="BO35" s="1"/>
-      <c r="BP35" s="1"/>
-      <c r="BQ35" s="1"/>
-      <c r="BR35" s="1"/>
-      <c r="BS35" s="1"/>
-      <c r="BT35" s="1"/>
-      <c r="BU35" s="1"/>
-      <c r="BV35" s="1"/>
-      <c r="BW35" s="1"/>
-      <c r="BX35" s="1"/>
-      <c r="BY35" s="1"/>
-      <c r="BZ35" s="1"/>
-      <c r="CA35" s="1"/>
-      <c r="CB35" s="1"/>
-      <c r="CC35" s="1"/>
-      <c r="CD35" s="1"/>
-      <c r="CE35" s="1"/>
-      <c r="CF35" s="1"/>
-      <c r="CG35" s="1"/>
-      <c r="CH35" s="1"/>
-      <c r="CI35" s="1"/>
-      <c r="CJ35" s="1"/>
-      <c r="CK35" s="1"/>
-      <c r="CL35" s="1"/>
-      <c r="CM35" s="1"/>
+      <c r="BB35" s="15"/>
+      <c r="BC35" s="15"/>
+      <c r="BD35" s="15"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="15"/>
+      <c r="BG35" s="15"/>
+      <c r="BH35" s="15"/>
+      <c r="BI35" s="15"/>
+      <c r="BJ35" s="15"/>
+      <c r="BK35" s="15"/>
+      <c r="BL35" s="15"/>
+      <c r="BM35" s="15"/>
+      <c r="BN35" s="15"/>
+      <c r="BO35" s="15"/>
+      <c r="BP35" s="15"/>
+      <c r="BQ35" s="15"/>
+      <c r="BR35" s="15"/>
+      <c r="BS35" s="15"/>
+      <c r="BT35" s="15"/>
+      <c r="BU35" s="15"/>
+      <c r="BV35" s="15"/>
+      <c r="BW35" s="15"/>
+      <c r="BX35" s="15"/>
+      <c r="BY35" s="15"/>
+      <c r="BZ35" s="15"/>
+      <c r="CA35" s="15"/>
+      <c r="CB35" s="16"/>
+      <c r="CC35" s="15"/>
+      <c r="CD35" s="15"/>
+      <c r="CE35" s="15"/>
+      <c r="CF35" s="15"/>
+      <c r="CG35" s="15"/>
+      <c r="CH35" s="15"/>
+      <c r="CI35" s="15"/>
+      <c r="CJ35" s="15"/>
+      <c r="CK35" s="15"/>
+      <c r="CL35" s="15"/>
+      <c r="CM35" s="15"/>
       <c r="CN35" s="1"/>
-      <c r="CO35" s="1" t="s">
+      <c r="CO35" s="16"/>
+      <c r="CP35" s="16"/>
+      <c r="CQ35" s="16"/>
+      <c r="CR35" s="16"/>
+      <c r="CS35" s="16"/>
+      <c r="CT35" s="16"/>
+      <c r="CU35" s="16"/>
+      <c r="CV35" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP35" s="1"/>
+      <c r="CW35" s="16"/>
     </row>
     <row r="36" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
@@ -7240,8 +7261,8 @@
       <c r="H36" s="32" t="s">
         <v>386</v>
       </c>
-      <c r="I36" s="29" t="s">
-        <v>265</v>
+      <c r="I36" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -7291,49 +7312,56 @@
       </c>
       <c r="AZ36" s="1"/>
       <c r="BA36" s="1"/>
-      <c r="BB36" s="1"/>
-      <c r="BC36" s="1"/>
-      <c r="BD36" s="1"/>
-      <c r="BE36" s="1"/>
-      <c r="BF36" s="1"/>
-      <c r="BG36" s="1"/>
-      <c r="BH36" s="1"/>
-      <c r="BI36" s="1"/>
-      <c r="BJ36" s="1"/>
-      <c r="BK36" s="1"/>
-      <c r="BL36" s="1"/>
-      <c r="BM36" s="1"/>
-      <c r="BN36" s="1"/>
-      <c r="BO36" s="1"/>
-      <c r="BP36" s="1"/>
-      <c r="BQ36" s="1"/>
-      <c r="BR36" s="1"/>
-      <c r="BS36" s="1"/>
-      <c r="BT36" s="1"/>
-      <c r="BU36" s="1"/>
-      <c r="BV36" s="1"/>
-      <c r="BW36" s="1"/>
-      <c r="BX36" s="1"/>
-      <c r="BY36" s="1"/>
-      <c r="BZ36" s="1"/>
-      <c r="CA36" s="1"/>
-      <c r="CB36" s="1"/>
-      <c r="CC36" s="1"/>
-      <c r="CD36" s="1"/>
-      <c r="CE36" s="1"/>
-      <c r="CF36" s="1"/>
-      <c r="CG36" s="1"/>
-      <c r="CH36" s="1"/>
-      <c r="CI36" s="1"/>
-      <c r="CJ36" s="1"/>
-      <c r="CK36" s="1"/>
-      <c r="CL36" s="1"/>
-      <c r="CM36" s="1"/>
+      <c r="BB36" s="15"/>
+      <c r="BC36" s="15"/>
+      <c r="BD36" s="15"/>
+      <c r="BE36" s="16"/>
+      <c r="BF36" s="15"/>
+      <c r="BG36" s="15"/>
+      <c r="BH36" s="15"/>
+      <c r="BI36" s="15"/>
+      <c r="BJ36" s="15"/>
+      <c r="BK36" s="15"/>
+      <c r="BL36" s="15"/>
+      <c r="BM36" s="15"/>
+      <c r="BN36" s="15"/>
+      <c r="BO36" s="15"/>
+      <c r="BP36" s="15"/>
+      <c r="BQ36" s="15"/>
+      <c r="BR36" s="15"/>
+      <c r="BS36" s="15"/>
+      <c r="BT36" s="15"/>
+      <c r="BU36" s="15"/>
+      <c r="BV36" s="15"/>
+      <c r="BW36" s="15"/>
+      <c r="BX36" s="15"/>
+      <c r="BY36" s="15"/>
+      <c r="BZ36" s="15"/>
+      <c r="CA36" s="15"/>
+      <c r="CB36" s="16"/>
+      <c r="CC36" s="15"/>
+      <c r="CD36" s="15"/>
+      <c r="CE36" s="15"/>
+      <c r="CF36" s="15"/>
+      <c r="CG36" s="15"/>
+      <c r="CH36" s="15"/>
+      <c r="CI36" s="15"/>
+      <c r="CJ36" s="15"/>
+      <c r="CK36" s="15"/>
+      <c r="CL36" s="15"/>
+      <c r="CM36" s="15"/>
       <c r="CN36" s="1"/>
-      <c r="CO36" s="1" t="s">
+      <c r="CO36" s="16"/>
+      <c r="CP36" s="16"/>
+      <c r="CQ36" s="16"/>
+      <c r="CR36" s="16"/>
+      <c r="CS36" s="16"/>
+      <c r="CT36" s="16"/>
+      <c r="CU36" s="16"/>
+      <c r="CV36" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP36" s="1"/>
+      <c r="CW36" s="16"/>
     </row>
     <row r="37" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
@@ -7360,8 +7388,8 @@
       <c r="H37" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I37" s="29" t="s">
-        <v>265</v>
+      <c r="I37" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -7411,49 +7439,56 @@
       </c>
       <c r="AZ37" s="1"/>
       <c r="BA37" s="1"/>
-      <c r="BB37" s="1"/>
-      <c r="BC37" s="1"/>
-      <c r="BD37" s="1"/>
-      <c r="BE37" s="1"/>
-      <c r="BF37" s="1"/>
-      <c r="BG37" s="1"/>
-      <c r="BH37" s="1"/>
-      <c r="BI37" s="1"/>
-      <c r="BJ37" s="1"/>
-      <c r="BK37" s="1"/>
-      <c r="BL37" s="1"/>
-      <c r="BM37" s="1"/>
-      <c r="BN37" s="1"/>
-      <c r="BO37" s="1"/>
-      <c r="BP37" s="1"/>
-      <c r="BQ37" s="1"/>
-      <c r="BR37" s="1"/>
-      <c r="BS37" s="1"/>
-      <c r="BT37" s="1"/>
-      <c r="BU37" s="1"/>
-      <c r="BV37" s="1"/>
-      <c r="BW37" s="1"/>
-      <c r="BX37" s="1"/>
-      <c r="BY37" s="1"/>
-      <c r="BZ37" s="1"/>
-      <c r="CA37" s="1"/>
-      <c r="CB37" s="1"/>
-      <c r="CC37" s="1"/>
-      <c r="CD37" s="1"/>
-      <c r="CE37" s="1"/>
-      <c r="CF37" s="1"/>
-      <c r="CG37" s="1"/>
-      <c r="CH37" s="1"/>
-      <c r="CI37" s="1"/>
-      <c r="CJ37" s="1"/>
-      <c r="CK37" s="1"/>
-      <c r="CL37" s="1"/>
-      <c r="CM37" s="1"/>
+      <c r="BB37" s="15"/>
+      <c r="BC37" s="15"/>
+      <c r="BD37" s="15"/>
+      <c r="BE37" s="16"/>
+      <c r="BF37" s="15"/>
+      <c r="BG37" s="15"/>
+      <c r="BH37" s="15"/>
+      <c r="BI37" s="15"/>
+      <c r="BJ37" s="15"/>
+      <c r="BK37" s="15"/>
+      <c r="BL37" s="15"/>
+      <c r="BM37" s="15"/>
+      <c r="BN37" s="15"/>
+      <c r="BO37" s="15"/>
+      <c r="BP37" s="15"/>
+      <c r="BQ37" s="15"/>
+      <c r="BR37" s="15"/>
+      <c r="BS37" s="15"/>
+      <c r="BT37" s="15"/>
+      <c r="BU37" s="15"/>
+      <c r="BV37" s="15"/>
+      <c r="BW37" s="15"/>
+      <c r="BX37" s="15"/>
+      <c r="BY37" s="15"/>
+      <c r="BZ37" s="15"/>
+      <c r="CA37" s="15"/>
+      <c r="CB37" s="16"/>
+      <c r="CC37" s="15"/>
+      <c r="CD37" s="15"/>
+      <c r="CE37" s="15"/>
+      <c r="CF37" s="15"/>
+      <c r="CG37" s="15"/>
+      <c r="CH37" s="15"/>
+      <c r="CI37" s="15"/>
+      <c r="CJ37" s="15"/>
+      <c r="CK37" s="15"/>
+      <c r="CL37" s="15"/>
+      <c r="CM37" s="15"/>
       <c r="CN37" s="1"/>
-      <c r="CO37" s="1" t="s">
+      <c r="CO37" s="16"/>
+      <c r="CP37" s="16"/>
+      <c r="CQ37" s="16"/>
+      <c r="CR37" s="16"/>
+      <c r="CS37" s="16"/>
+      <c r="CT37" s="16"/>
+      <c r="CU37" s="16"/>
+      <c r="CV37" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP37" s="1"/>
+      <c r="CW37" s="16"/>
     </row>
     <row r="38" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
@@ -7480,8 +7515,8 @@
       <c r="H38" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="I38" s="29" t="s">
-        <v>265</v>
+      <c r="I38" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -7531,49 +7566,56 @@
       </c>
       <c r="AZ38" s="1"/>
       <c r="BA38" s="1"/>
-      <c r="BB38" s="1"/>
-      <c r="BC38" s="1"/>
-      <c r="BD38" s="1"/>
-      <c r="BE38" s="1"/>
-      <c r="BF38" s="1"/>
-      <c r="BG38" s="1"/>
-      <c r="BH38" s="1"/>
-      <c r="BI38" s="1"/>
-      <c r="BJ38" s="1"/>
-      <c r="BK38" s="1"/>
-      <c r="BL38" s="1"/>
-      <c r="BM38" s="1"/>
-      <c r="BN38" s="1"/>
-      <c r="BO38" s="1"/>
-      <c r="BP38" s="1"/>
-      <c r="BQ38" s="1"/>
-      <c r="BR38" s="1"/>
-      <c r="BS38" s="1"/>
-      <c r="BT38" s="1"/>
-      <c r="BU38" s="1"/>
-      <c r="BV38" s="1"/>
-      <c r="BW38" s="1"/>
-      <c r="BX38" s="1"/>
-      <c r="BY38" s="1"/>
-      <c r="BZ38" s="1"/>
-      <c r="CA38" s="1"/>
-      <c r="CB38" s="1"/>
-      <c r="CC38" s="1"/>
-      <c r="CD38" s="1"/>
-      <c r="CE38" s="1"/>
-      <c r="CF38" s="1"/>
-      <c r="CG38" s="1"/>
-      <c r="CH38" s="1"/>
-      <c r="CI38" s="1"/>
-      <c r="CJ38" s="1"/>
-      <c r="CK38" s="1"/>
-      <c r="CL38" s="1"/>
-      <c r="CM38" s="1"/>
+      <c r="BB38" s="15"/>
+      <c r="BC38" s="15"/>
+      <c r="BD38" s="15"/>
+      <c r="BE38" s="16"/>
+      <c r="BF38" s="15"/>
+      <c r="BG38" s="15"/>
+      <c r="BH38" s="15"/>
+      <c r="BI38" s="15"/>
+      <c r="BJ38" s="15"/>
+      <c r="BK38" s="15"/>
+      <c r="BL38" s="15"/>
+      <c r="BM38" s="15"/>
+      <c r="BN38" s="15"/>
+      <c r="BO38" s="15"/>
+      <c r="BP38" s="15"/>
+      <c r="BQ38" s="15"/>
+      <c r="BR38" s="15"/>
+      <c r="BS38" s="15"/>
+      <c r="BT38" s="15"/>
+      <c r="BU38" s="15"/>
+      <c r="BV38" s="15"/>
+      <c r="BW38" s="15"/>
+      <c r="BX38" s="15"/>
+      <c r="BY38" s="15"/>
+      <c r="BZ38" s="15"/>
+      <c r="CA38" s="15"/>
+      <c r="CB38" s="16"/>
+      <c r="CC38" s="15"/>
+      <c r="CD38" s="15"/>
+      <c r="CE38" s="15"/>
+      <c r="CF38" s="15"/>
+      <c r="CG38" s="15"/>
+      <c r="CH38" s="15"/>
+      <c r="CI38" s="15"/>
+      <c r="CJ38" s="15"/>
+      <c r="CK38" s="15"/>
+      <c r="CL38" s="15"/>
+      <c r="CM38" s="15"/>
       <c r="CN38" s="1"/>
-      <c r="CO38" s="1" t="s">
+      <c r="CO38" s="16"/>
+      <c r="CP38" s="16"/>
+      <c r="CQ38" s="16"/>
+      <c r="CR38" s="16"/>
+      <c r="CS38" s="16"/>
+      <c r="CT38" s="16"/>
+      <c r="CU38" s="16"/>
+      <c r="CV38" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP38" s="1"/>
+      <c r="CW38" s="16"/>
     </row>
     <row r="39" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -7600,8 +7642,8 @@
       <c r="H39" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="I39" s="29" t="s">
-        <v>265</v>
+      <c r="I39" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -7651,49 +7693,56 @@
       </c>
       <c r="AZ39" s="1"/>
       <c r="BA39" s="1"/>
-      <c r="BB39" s="1"/>
-      <c r="BC39" s="1"/>
-      <c r="BD39" s="1"/>
-      <c r="BE39" s="1"/>
-      <c r="BF39" s="1"/>
-      <c r="BG39" s="1"/>
-      <c r="BH39" s="1"/>
-      <c r="BI39" s="1"/>
-      <c r="BJ39" s="1"/>
-      <c r="BK39" s="1"/>
-      <c r="BL39" s="1"/>
-      <c r="BM39" s="1"/>
-      <c r="BN39" s="1"/>
-      <c r="BO39" s="1"/>
-      <c r="BP39" s="1"/>
-      <c r="BQ39" s="1"/>
-      <c r="BR39" s="1"/>
-      <c r="BS39" s="1"/>
-      <c r="BT39" s="1"/>
-      <c r="BU39" s="1"/>
-      <c r="BV39" s="1"/>
-      <c r="BW39" s="1"/>
-      <c r="BX39" s="1"/>
-      <c r="BY39" s="1"/>
-      <c r="BZ39" s="1"/>
-      <c r="CA39" s="1"/>
-      <c r="CB39" s="1"/>
-      <c r="CC39" s="1"/>
-      <c r="CD39" s="1"/>
-      <c r="CE39" s="1"/>
-      <c r="CF39" s="1"/>
-      <c r="CG39" s="1"/>
-      <c r="CH39" s="1"/>
-      <c r="CI39" s="1"/>
-      <c r="CJ39" s="1"/>
-      <c r="CK39" s="1"/>
-      <c r="CL39" s="1"/>
-      <c r="CM39" s="1"/>
+      <c r="BB39" s="15"/>
+      <c r="BC39" s="15"/>
+      <c r="BD39" s="15"/>
+      <c r="BE39" s="16"/>
+      <c r="BF39" s="15"/>
+      <c r="BG39" s="15"/>
+      <c r="BH39" s="15"/>
+      <c r="BI39" s="15"/>
+      <c r="BJ39" s="15"/>
+      <c r="BK39" s="15"/>
+      <c r="BL39" s="15"/>
+      <c r="BM39" s="15"/>
+      <c r="BN39" s="15"/>
+      <c r="BO39" s="15"/>
+      <c r="BP39" s="15"/>
+      <c r="BQ39" s="15"/>
+      <c r="BR39" s="15"/>
+      <c r="BS39" s="15"/>
+      <c r="BT39" s="15"/>
+      <c r="BU39" s="15"/>
+      <c r="BV39" s="15"/>
+      <c r="BW39" s="15"/>
+      <c r="BX39" s="15"/>
+      <c r="BY39" s="15"/>
+      <c r="BZ39" s="15"/>
+      <c r="CA39" s="15"/>
+      <c r="CB39" s="16"/>
+      <c r="CC39" s="15"/>
+      <c r="CD39" s="15"/>
+      <c r="CE39" s="15"/>
+      <c r="CF39" s="15"/>
+      <c r="CG39" s="15"/>
+      <c r="CH39" s="15"/>
+      <c r="CI39" s="15"/>
+      <c r="CJ39" s="15"/>
+      <c r="CK39" s="15"/>
+      <c r="CL39" s="15"/>
+      <c r="CM39" s="15"/>
       <c r="CN39" s="1"/>
-      <c r="CO39" s="1" t="s">
+      <c r="CO39" s="16"/>
+      <c r="CP39" s="16"/>
+      <c r="CQ39" s="16"/>
+      <c r="CR39" s="16"/>
+      <c r="CS39" s="16"/>
+      <c r="CT39" s="16"/>
+      <c r="CU39" s="16"/>
+      <c r="CV39" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP39" s="1"/>
+      <c r="CW39" s="16"/>
     </row>
     <row r="40" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
@@ -7720,8 +7769,8 @@
       <c r="H40" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="I40" s="29" t="s">
-        <v>265</v>
+      <c r="I40" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -7771,49 +7820,56 @@
       </c>
       <c r="AZ40" s="1"/>
       <c r="BA40" s="1"/>
-      <c r="BB40" s="1"/>
-      <c r="BC40" s="1"/>
-      <c r="BD40" s="1"/>
-      <c r="BE40" s="1"/>
-      <c r="BF40" s="1"/>
-      <c r="BG40" s="1"/>
-      <c r="BH40" s="1"/>
-      <c r="BI40" s="1"/>
-      <c r="BJ40" s="1"/>
-      <c r="BK40" s="1"/>
-      <c r="BL40" s="1"/>
-      <c r="BM40" s="1"/>
-      <c r="BN40" s="1"/>
-      <c r="BO40" s="1"/>
-      <c r="BP40" s="1"/>
-      <c r="BQ40" s="1"/>
-      <c r="BR40" s="1"/>
-      <c r="BS40" s="1"/>
-      <c r="BT40" s="1"/>
-      <c r="BU40" s="1"/>
-      <c r="BV40" s="1"/>
-      <c r="BW40" s="1"/>
-      <c r="BX40" s="1"/>
-      <c r="BY40" s="1"/>
-      <c r="BZ40" s="1"/>
-      <c r="CA40" s="1"/>
-      <c r="CB40" s="1"/>
-      <c r="CC40" s="1"/>
-      <c r="CD40" s="1"/>
-      <c r="CE40" s="1"/>
-      <c r="CF40" s="1"/>
-      <c r="CG40" s="1"/>
-      <c r="CH40" s="1"/>
-      <c r="CI40" s="1"/>
-      <c r="CJ40" s="1"/>
-      <c r="CK40" s="1"/>
-      <c r="CL40" s="1"/>
-      <c r="CM40" s="1"/>
+      <c r="BB40" s="15"/>
+      <c r="BC40" s="15"/>
+      <c r="BD40" s="15"/>
+      <c r="BE40" s="16"/>
+      <c r="BF40" s="15"/>
+      <c r="BG40" s="15"/>
+      <c r="BH40" s="15"/>
+      <c r="BI40" s="15"/>
+      <c r="BJ40" s="15"/>
+      <c r="BK40" s="15"/>
+      <c r="BL40" s="15"/>
+      <c r="BM40" s="15"/>
+      <c r="BN40" s="15"/>
+      <c r="BO40" s="15"/>
+      <c r="BP40" s="15"/>
+      <c r="BQ40" s="15"/>
+      <c r="BR40" s="15"/>
+      <c r="BS40" s="15"/>
+      <c r="BT40" s="15"/>
+      <c r="BU40" s="15"/>
+      <c r="BV40" s="15"/>
+      <c r="BW40" s="15"/>
+      <c r="BX40" s="15"/>
+      <c r="BY40" s="15"/>
+      <c r="BZ40" s="15"/>
+      <c r="CA40" s="15"/>
+      <c r="CB40" s="16"/>
+      <c r="CC40" s="15"/>
+      <c r="CD40" s="15"/>
+      <c r="CE40" s="15"/>
+      <c r="CF40" s="15"/>
+      <c r="CG40" s="15"/>
+      <c r="CH40" s="15"/>
+      <c r="CI40" s="15"/>
+      <c r="CJ40" s="15"/>
+      <c r="CK40" s="15"/>
+      <c r="CL40" s="15"/>
+      <c r="CM40" s="15"/>
       <c r="CN40" s="1"/>
-      <c r="CO40" s="1" t="s">
+      <c r="CO40" s="16"/>
+      <c r="CP40" s="16"/>
+      <c r="CQ40" s="16"/>
+      <c r="CR40" s="16"/>
+      <c r="CS40" s="16"/>
+      <c r="CT40" s="16"/>
+      <c r="CU40" s="16"/>
+      <c r="CV40" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP40" s="1"/>
+      <c r="CW40" s="16"/>
     </row>
     <row r="41" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
@@ -7840,8 +7896,8 @@
       <c r="H41" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I41" s="29" t="s">
-        <v>265</v>
+      <c r="I41" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -7891,49 +7947,56 @@
       </c>
       <c r="AZ41" s="1"/>
       <c r="BA41" s="1"/>
-      <c r="BB41" s="1"/>
-      <c r="BC41" s="1"/>
-      <c r="BD41" s="1"/>
-      <c r="BE41" s="1"/>
-      <c r="BF41" s="1"/>
-      <c r="BG41" s="1"/>
-      <c r="BH41" s="1"/>
-      <c r="BI41" s="1"/>
-      <c r="BJ41" s="1"/>
-      <c r="BK41" s="1"/>
-      <c r="BL41" s="1"/>
-      <c r="BM41" s="1"/>
-      <c r="BN41" s="1"/>
-      <c r="BO41" s="1"/>
-      <c r="BP41" s="1"/>
-      <c r="BQ41" s="1"/>
-      <c r="BR41" s="1"/>
-      <c r="BS41" s="1"/>
-      <c r="BT41" s="1"/>
-      <c r="BU41" s="1"/>
-      <c r="BV41" s="1"/>
-      <c r="BW41" s="1"/>
-      <c r="BX41" s="1"/>
-      <c r="BY41" s="1"/>
-      <c r="BZ41" s="1"/>
-      <c r="CA41" s="1"/>
-      <c r="CB41" s="1"/>
-      <c r="CC41" s="1"/>
-      <c r="CD41" s="1"/>
-      <c r="CE41" s="1"/>
-      <c r="CF41" s="1"/>
-      <c r="CG41" s="1"/>
-      <c r="CH41" s="1"/>
-      <c r="CI41" s="1"/>
-      <c r="CJ41" s="1"/>
-      <c r="CK41" s="1"/>
-      <c r="CL41" s="1"/>
-      <c r="CM41" s="1"/>
+      <c r="BB41" s="15"/>
+      <c r="BC41" s="15"/>
+      <c r="BD41" s="15"/>
+      <c r="BE41" s="16"/>
+      <c r="BF41" s="15"/>
+      <c r="BG41" s="15"/>
+      <c r="BH41" s="15"/>
+      <c r="BI41" s="15"/>
+      <c r="BJ41" s="15"/>
+      <c r="BK41" s="15"/>
+      <c r="BL41" s="15"/>
+      <c r="BM41" s="15"/>
+      <c r="BN41" s="15"/>
+      <c r="BO41" s="15"/>
+      <c r="BP41" s="15"/>
+      <c r="BQ41" s="15"/>
+      <c r="BR41" s="15"/>
+      <c r="BS41" s="15"/>
+      <c r="BT41" s="15"/>
+      <c r="BU41" s="15"/>
+      <c r="BV41" s="15"/>
+      <c r="BW41" s="15"/>
+      <c r="BX41" s="15"/>
+      <c r="BY41" s="15"/>
+      <c r="BZ41" s="15"/>
+      <c r="CA41" s="15"/>
+      <c r="CB41" s="16"/>
+      <c r="CC41" s="15"/>
+      <c r="CD41" s="15"/>
+      <c r="CE41" s="15"/>
+      <c r="CF41" s="15"/>
+      <c r="CG41" s="15"/>
+      <c r="CH41" s="15"/>
+      <c r="CI41" s="15"/>
+      <c r="CJ41" s="15"/>
+      <c r="CK41" s="15"/>
+      <c r="CL41" s="15"/>
+      <c r="CM41" s="15"/>
       <c r="CN41" s="1"/>
-      <c r="CO41" s="1" t="s">
+      <c r="CO41" s="16"/>
+      <c r="CP41" s="16"/>
+      <c r="CQ41" s="16"/>
+      <c r="CR41" s="16"/>
+      <c r="CS41" s="16"/>
+      <c r="CT41" s="16"/>
+      <c r="CU41" s="16"/>
+      <c r="CV41" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP41" s="1"/>
+      <c r="CW41" s="16"/>
     </row>
     <row r="42" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -7960,8 +8023,8 @@
       <c r="H42" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="I42" s="29" t="s">
-        <v>265</v>
+      <c r="I42" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -8011,49 +8074,56 @@
       </c>
       <c r="AZ42" s="1"/>
       <c r="BA42" s="1"/>
-      <c r="BB42" s="1"/>
-      <c r="BC42" s="1"/>
-      <c r="BD42" s="1"/>
-      <c r="BE42" s="1"/>
-      <c r="BF42" s="1"/>
-      <c r="BG42" s="1"/>
-      <c r="BH42" s="1"/>
-      <c r="BI42" s="1"/>
-      <c r="BJ42" s="1"/>
-      <c r="BK42" s="1"/>
-      <c r="BL42" s="1"/>
-      <c r="BM42" s="1"/>
-      <c r="BN42" s="1"/>
-      <c r="BO42" s="1"/>
-      <c r="BP42" s="1"/>
-      <c r="BQ42" s="1"/>
-      <c r="BR42" s="1"/>
-      <c r="BS42" s="1"/>
-      <c r="BT42" s="1"/>
-      <c r="BU42" s="1"/>
-      <c r="BV42" s="1"/>
-      <c r="BW42" s="1"/>
-      <c r="BX42" s="1"/>
-      <c r="BY42" s="1"/>
-      <c r="BZ42" s="1"/>
-      <c r="CA42" s="1"/>
-      <c r="CB42" s="1"/>
-      <c r="CC42" s="1"/>
-      <c r="CD42" s="1"/>
-      <c r="CE42" s="1"/>
-      <c r="CF42" s="1"/>
-      <c r="CG42" s="1"/>
-      <c r="CH42" s="1"/>
-      <c r="CI42" s="1"/>
-      <c r="CJ42" s="1"/>
-      <c r="CK42" s="1"/>
-      <c r="CL42" s="1"/>
-      <c r="CM42" s="1"/>
+      <c r="BB42" s="15"/>
+      <c r="BC42" s="15"/>
+      <c r="BD42" s="15"/>
+      <c r="BE42" s="16"/>
+      <c r="BF42" s="15"/>
+      <c r="BG42" s="15"/>
+      <c r="BH42" s="15"/>
+      <c r="BI42" s="15"/>
+      <c r="BJ42" s="15"/>
+      <c r="BK42" s="15"/>
+      <c r="BL42" s="15"/>
+      <c r="BM42" s="15"/>
+      <c r="BN42" s="15"/>
+      <c r="BO42" s="15"/>
+      <c r="BP42" s="15"/>
+      <c r="BQ42" s="15"/>
+      <c r="BR42" s="15"/>
+      <c r="BS42" s="15"/>
+      <c r="BT42" s="15"/>
+      <c r="BU42" s="15"/>
+      <c r="BV42" s="15"/>
+      <c r="BW42" s="15"/>
+      <c r="BX42" s="15"/>
+      <c r="BY42" s="15"/>
+      <c r="BZ42" s="15"/>
+      <c r="CA42" s="15"/>
+      <c r="CB42" s="16"/>
+      <c r="CC42" s="15"/>
+      <c r="CD42" s="15"/>
+      <c r="CE42" s="15"/>
+      <c r="CF42" s="15"/>
+      <c r="CG42" s="15"/>
+      <c r="CH42" s="15"/>
+      <c r="CI42" s="15"/>
+      <c r="CJ42" s="15"/>
+      <c r="CK42" s="15"/>
+      <c r="CL42" s="15"/>
+      <c r="CM42" s="15"/>
       <c r="CN42" s="1"/>
-      <c r="CO42" s="1" t="s">
+      <c r="CO42" s="16"/>
+      <c r="CP42" s="16"/>
+      <c r="CQ42" s="16"/>
+      <c r="CR42" s="16"/>
+      <c r="CS42" s="16"/>
+      <c r="CT42" s="16"/>
+      <c r="CU42" s="16"/>
+      <c r="CV42" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP42" s="1"/>
+      <c r="CW42" s="16"/>
     </row>
     <row r="43" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
@@ -8080,8 +8150,8 @@
       <c r="H43" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="I43" s="29" t="s">
-        <v>265</v>
+      <c r="I43" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -8131,49 +8201,56 @@
       </c>
       <c r="AZ43" s="1"/>
       <c r="BA43" s="1"/>
-      <c r="BB43" s="1"/>
-      <c r="BC43" s="1"/>
-      <c r="BD43" s="1"/>
-      <c r="BE43" s="1"/>
-      <c r="BF43" s="1"/>
-      <c r="BG43" s="1"/>
-      <c r="BH43" s="1"/>
-      <c r="BI43" s="1"/>
-      <c r="BJ43" s="1"/>
-      <c r="BK43" s="1"/>
-      <c r="BL43" s="1"/>
-      <c r="BM43" s="1"/>
-      <c r="BN43" s="1"/>
-      <c r="BO43" s="1"/>
-      <c r="BP43" s="1"/>
-      <c r="BQ43" s="1"/>
-      <c r="BR43" s="1"/>
-      <c r="BS43" s="1"/>
-      <c r="BT43" s="1"/>
-      <c r="BU43" s="1"/>
-      <c r="BV43" s="1"/>
-      <c r="BW43" s="1"/>
-      <c r="BX43" s="1"/>
-      <c r="BY43" s="1"/>
-      <c r="BZ43" s="1"/>
-      <c r="CA43" s="1"/>
-      <c r="CB43" s="1"/>
-      <c r="CC43" s="1"/>
-      <c r="CD43" s="1"/>
-      <c r="CE43" s="1"/>
-      <c r="CF43" s="1"/>
-      <c r="CG43" s="1"/>
-      <c r="CH43" s="1"/>
-      <c r="CI43" s="1"/>
-      <c r="CJ43" s="1"/>
-      <c r="CK43" s="1"/>
-      <c r="CL43" s="1"/>
-      <c r="CM43" s="1"/>
+      <c r="BB43" s="15"/>
+      <c r="BC43" s="15"/>
+      <c r="BD43" s="15"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="15"/>
+      <c r="BG43" s="15"/>
+      <c r="BH43" s="15"/>
+      <c r="BI43" s="15"/>
+      <c r="BJ43" s="15"/>
+      <c r="BK43" s="15"/>
+      <c r="BL43" s="15"/>
+      <c r="BM43" s="15"/>
+      <c r="BN43" s="15"/>
+      <c r="BO43" s="15"/>
+      <c r="BP43" s="15"/>
+      <c r="BQ43" s="15"/>
+      <c r="BR43" s="15"/>
+      <c r="BS43" s="15"/>
+      <c r="BT43" s="15"/>
+      <c r="BU43" s="15"/>
+      <c r="BV43" s="15"/>
+      <c r="BW43" s="15"/>
+      <c r="BX43" s="15"/>
+      <c r="BY43" s="15"/>
+      <c r="BZ43" s="15"/>
+      <c r="CA43" s="15"/>
+      <c r="CB43" s="16"/>
+      <c r="CC43" s="15"/>
+      <c r="CD43" s="15"/>
+      <c r="CE43" s="15"/>
+      <c r="CF43" s="15"/>
+      <c r="CG43" s="15"/>
+      <c r="CH43" s="15"/>
+      <c r="CI43" s="15"/>
+      <c r="CJ43" s="15"/>
+      <c r="CK43" s="15"/>
+      <c r="CL43" s="15"/>
+      <c r="CM43" s="15"/>
       <c r="CN43" s="1"/>
-      <c r="CO43" s="1" t="s">
+      <c r="CO43" s="16"/>
+      <c r="CP43" s="16"/>
+      <c r="CQ43" s="16"/>
+      <c r="CR43" s="16"/>
+      <c r="CS43" s="16"/>
+      <c r="CT43" s="16"/>
+      <c r="CU43" s="16"/>
+      <c r="CV43" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP43" s="1"/>
+      <c r="CW43" s="16"/>
     </row>
     <row r="44" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
@@ -8198,8 +8275,8 @@
         <v>425</v>
       </c>
       <c r="H44" s="1"/>
-      <c r="I44" s="29" t="s">
-        <v>265</v>
+      <c r="I44" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
@@ -8249,49 +8326,56 @@
       </c>
       <c r="AZ44" s="1"/>
       <c r="BA44" s="1"/>
-      <c r="BB44" s="1"/>
-      <c r="BC44" s="1"/>
-      <c r="BD44" s="1"/>
-      <c r="BE44" s="1"/>
-      <c r="BF44" s="1"/>
-      <c r="BG44" s="1"/>
-      <c r="BH44" s="1"/>
-      <c r="BI44" s="1"/>
-      <c r="BJ44" s="1"/>
-      <c r="BK44" s="1"/>
-      <c r="BL44" s="1"/>
-      <c r="BM44" s="1"/>
-      <c r="BN44" s="1"/>
-      <c r="BO44" s="1"/>
-      <c r="BP44" s="1"/>
-      <c r="BQ44" s="1"/>
-      <c r="BR44" s="1"/>
-      <c r="BS44" s="1"/>
-      <c r="BT44" s="1"/>
-      <c r="BU44" s="1"/>
-      <c r="BV44" s="1"/>
-      <c r="BW44" s="1"/>
-      <c r="BX44" s="1"/>
-      <c r="BY44" s="1"/>
-      <c r="BZ44" s="1"/>
-      <c r="CA44" s="1"/>
-      <c r="CB44" s="1"/>
-      <c r="CC44" s="1"/>
-      <c r="CD44" s="1"/>
-      <c r="CE44" s="1"/>
-      <c r="CF44" s="1"/>
-      <c r="CG44" s="1"/>
-      <c r="CH44" s="1"/>
-      <c r="CI44" s="1"/>
-      <c r="CJ44" s="1"/>
-      <c r="CK44" s="1"/>
-      <c r="CL44" s="1"/>
-      <c r="CM44" s="1"/>
+      <c r="BB44" s="15"/>
+      <c r="BC44" s="15"/>
+      <c r="BD44" s="15"/>
+      <c r="BE44" s="16"/>
+      <c r="BF44" s="15"/>
+      <c r="BG44" s="15"/>
+      <c r="BH44" s="15"/>
+      <c r="BI44" s="15"/>
+      <c r="BJ44" s="15"/>
+      <c r="BK44" s="15"/>
+      <c r="BL44" s="15"/>
+      <c r="BM44" s="15"/>
+      <c r="BN44" s="15"/>
+      <c r="BO44" s="15"/>
+      <c r="BP44" s="15"/>
+      <c r="BQ44" s="15"/>
+      <c r="BR44" s="15"/>
+      <c r="BS44" s="15"/>
+      <c r="BT44" s="15"/>
+      <c r="BU44" s="15"/>
+      <c r="BV44" s="15"/>
+      <c r="BW44" s="15"/>
+      <c r="BX44" s="15"/>
+      <c r="BY44" s="15"/>
+      <c r="BZ44" s="15"/>
+      <c r="CA44" s="15"/>
+      <c r="CB44" s="16"/>
+      <c r="CC44" s="15"/>
+      <c r="CD44" s="15"/>
+      <c r="CE44" s="15"/>
+      <c r="CF44" s="15"/>
+      <c r="CG44" s="15"/>
+      <c r="CH44" s="15"/>
+      <c r="CI44" s="15"/>
+      <c r="CJ44" s="15"/>
+      <c r="CK44" s="15"/>
+      <c r="CL44" s="15"/>
+      <c r="CM44" s="15"/>
       <c r="CN44" s="1"/>
-      <c r="CO44" s="1" t="s">
+      <c r="CO44" s="16"/>
+      <c r="CP44" s="16"/>
+      <c r="CQ44" s="16"/>
+      <c r="CR44" s="16"/>
+      <c r="CS44" s="16"/>
+      <c r="CT44" s="16"/>
+      <c r="CU44" s="16"/>
+      <c r="CV44" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP44" s="1"/>
+      <c r="CW44" s="16"/>
     </row>
     <row r="45" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
@@ -8316,8 +8400,8 @@
         <v>429</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="29" t="s">
-        <v>265</v>
+      <c r="I45" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
@@ -8367,49 +8451,56 @@
       </c>
       <c r="AZ45" s="1"/>
       <c r="BA45" s="1"/>
-      <c r="BB45" s="1"/>
-      <c r="BC45" s="1"/>
-      <c r="BD45" s="1"/>
-      <c r="BE45" s="1"/>
-      <c r="BF45" s="1"/>
-      <c r="BG45" s="1"/>
-      <c r="BH45" s="1"/>
-      <c r="BI45" s="1"/>
-      <c r="BJ45" s="1"/>
-      <c r="BK45" s="1"/>
-      <c r="BL45" s="1"/>
-      <c r="BM45" s="1"/>
-      <c r="BN45" s="1"/>
-      <c r="BO45" s="1"/>
-      <c r="BP45" s="1"/>
-      <c r="BQ45" s="1"/>
-      <c r="BR45" s="1"/>
-      <c r="BS45" s="1"/>
-      <c r="BT45" s="1"/>
-      <c r="BU45" s="1"/>
-      <c r="BV45" s="1"/>
-      <c r="BW45" s="1"/>
-      <c r="BX45" s="1"/>
-      <c r="BY45" s="1"/>
-      <c r="BZ45" s="1"/>
-      <c r="CA45" s="1"/>
-      <c r="CB45" s="1"/>
-      <c r="CC45" s="1"/>
-      <c r="CD45" s="1"/>
-      <c r="CE45" s="1"/>
-      <c r="CF45" s="1"/>
-      <c r="CG45" s="1"/>
-      <c r="CH45" s="1"/>
-      <c r="CI45" s="1"/>
-      <c r="CJ45" s="1"/>
-      <c r="CK45" s="1"/>
-      <c r="CL45" s="1"/>
-      <c r="CM45" s="1"/>
+      <c r="BB45" s="15"/>
+      <c r="BC45" s="15"/>
+      <c r="BD45" s="15"/>
+      <c r="BE45" s="16"/>
+      <c r="BF45" s="15"/>
+      <c r="BG45" s="15"/>
+      <c r="BH45" s="15"/>
+      <c r="BI45" s="15"/>
+      <c r="BJ45" s="15"/>
+      <c r="BK45" s="15"/>
+      <c r="BL45" s="15"/>
+      <c r="BM45" s="15"/>
+      <c r="BN45" s="15"/>
+      <c r="BO45" s="15"/>
+      <c r="BP45" s="15"/>
+      <c r="BQ45" s="15"/>
+      <c r="BR45" s="15"/>
+      <c r="BS45" s="15"/>
+      <c r="BT45" s="15"/>
+      <c r="BU45" s="15"/>
+      <c r="BV45" s="15"/>
+      <c r="BW45" s="15"/>
+      <c r="BX45" s="15"/>
+      <c r="BY45" s="15"/>
+      <c r="BZ45" s="15"/>
+      <c r="CA45" s="15"/>
+      <c r="CB45" s="16"/>
+      <c r="CC45" s="15"/>
+      <c r="CD45" s="15"/>
+      <c r="CE45" s="15"/>
+      <c r="CF45" s="15"/>
+      <c r="CG45" s="15"/>
+      <c r="CH45" s="15"/>
+      <c r="CI45" s="15"/>
+      <c r="CJ45" s="15"/>
+      <c r="CK45" s="15"/>
+      <c r="CL45" s="15"/>
+      <c r="CM45" s="15"/>
       <c r="CN45" s="1"/>
-      <c r="CO45" s="1" t="s">
+      <c r="CO45" s="16"/>
+      <c r="CP45" s="16"/>
+      <c r="CQ45" s="16"/>
+      <c r="CR45" s="16"/>
+      <c r="CS45" s="16"/>
+      <c r="CT45" s="16"/>
+      <c r="CU45" s="16"/>
+      <c r="CV45" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP45" s="1"/>
+      <c r="CW45" s="16"/>
     </row>
     <row r="46" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
@@ -8434,8 +8525,8 @@
         <v>433</v>
       </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="29" t="s">
-        <v>265</v>
+      <c r="I46" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
@@ -8485,49 +8576,56 @@
       </c>
       <c r="AZ46" s="1"/>
       <c r="BA46" s="1"/>
-      <c r="BB46" s="1"/>
-      <c r="BC46" s="1"/>
-      <c r="BD46" s="1"/>
-      <c r="BE46" s="1"/>
-      <c r="BF46" s="1"/>
-      <c r="BG46" s="1"/>
-      <c r="BH46" s="1"/>
-      <c r="BI46" s="1"/>
-      <c r="BJ46" s="1"/>
-      <c r="BK46" s="1"/>
-      <c r="BL46" s="1"/>
-      <c r="BM46" s="1"/>
-      <c r="BN46" s="1"/>
-      <c r="BO46" s="1"/>
-      <c r="BP46" s="1"/>
-      <c r="BQ46" s="1"/>
-      <c r="BR46" s="1"/>
-      <c r="BS46" s="1"/>
-      <c r="BT46" s="1"/>
-      <c r="BU46" s="1"/>
-      <c r="BV46" s="1"/>
-      <c r="BW46" s="1"/>
-      <c r="BX46" s="1"/>
-      <c r="BY46" s="1"/>
-      <c r="BZ46" s="1"/>
-      <c r="CA46" s="1"/>
-      <c r="CB46" s="1"/>
-      <c r="CC46" s="1"/>
-      <c r="CD46" s="1"/>
-      <c r="CE46" s="1"/>
-      <c r="CF46" s="1"/>
-      <c r="CG46" s="1"/>
-      <c r="CH46" s="1"/>
-      <c r="CI46" s="1"/>
-      <c r="CJ46" s="1"/>
-      <c r="CK46" s="1"/>
-      <c r="CL46" s="1"/>
-      <c r="CM46" s="1"/>
+      <c r="BB46" s="15"/>
+      <c r="BC46" s="15"/>
+      <c r="BD46" s="15"/>
+      <c r="BE46" s="16"/>
+      <c r="BF46" s="15"/>
+      <c r="BG46" s="15"/>
+      <c r="BH46" s="15"/>
+      <c r="BI46" s="15"/>
+      <c r="BJ46" s="15"/>
+      <c r="BK46" s="15"/>
+      <c r="BL46" s="15"/>
+      <c r="BM46" s="15"/>
+      <c r="BN46" s="15"/>
+      <c r="BO46" s="15"/>
+      <c r="BP46" s="15"/>
+      <c r="BQ46" s="15"/>
+      <c r="BR46" s="15"/>
+      <c r="BS46" s="15"/>
+      <c r="BT46" s="15"/>
+      <c r="BU46" s="15"/>
+      <c r="BV46" s="15"/>
+      <c r="BW46" s="15"/>
+      <c r="BX46" s="15"/>
+      <c r="BY46" s="15"/>
+      <c r="BZ46" s="15"/>
+      <c r="CA46" s="15"/>
+      <c r="CB46" s="16"/>
+      <c r="CC46" s="15"/>
+      <c r="CD46" s="15"/>
+      <c r="CE46" s="15"/>
+      <c r="CF46" s="15"/>
+      <c r="CG46" s="15"/>
+      <c r="CH46" s="15"/>
+      <c r="CI46" s="15"/>
+      <c r="CJ46" s="15"/>
+      <c r="CK46" s="15"/>
+      <c r="CL46" s="15"/>
+      <c r="CM46" s="15"/>
       <c r="CN46" s="1"/>
-      <c r="CO46" s="1" t="s">
+      <c r="CO46" s="16"/>
+      <c r="CP46" s="16"/>
+      <c r="CQ46" s="16"/>
+      <c r="CR46" s="16"/>
+      <c r="CS46" s="16"/>
+      <c r="CT46" s="16"/>
+      <c r="CU46" s="16"/>
+      <c r="CV46" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP46" s="1"/>
+      <c r="CW46" s="16"/>
     </row>
     <row r="47" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
@@ -8552,8 +8650,8 @@
         <v>437</v>
       </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="29" t="s">
-        <v>265</v>
+      <c r="I47" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
@@ -8603,49 +8701,56 @@
       </c>
       <c r="AZ47" s="1"/>
       <c r="BA47" s="1"/>
-      <c r="BB47" s="1"/>
-      <c r="BC47" s="1"/>
-      <c r="BD47" s="1"/>
-      <c r="BE47" s="1"/>
-      <c r="BF47" s="1"/>
-      <c r="BG47" s="1"/>
-      <c r="BH47" s="1"/>
-      <c r="BI47" s="1"/>
-      <c r="BJ47" s="1"/>
-      <c r="BK47" s="1"/>
-      <c r="BL47" s="1"/>
-      <c r="BM47" s="1"/>
-      <c r="BN47" s="1"/>
-      <c r="BO47" s="1"/>
-      <c r="BP47" s="1"/>
-      <c r="BQ47" s="1"/>
-      <c r="BR47" s="1"/>
-      <c r="BS47" s="1"/>
-      <c r="BT47" s="1"/>
-      <c r="BU47" s="1"/>
-      <c r="BV47" s="1"/>
-      <c r="BW47" s="1"/>
-      <c r="BX47" s="1"/>
-      <c r="BY47" s="1"/>
-      <c r="BZ47" s="1"/>
-      <c r="CA47" s="1"/>
-      <c r="CB47" s="1"/>
-      <c r="CC47" s="1"/>
-      <c r="CD47" s="1"/>
-      <c r="CE47" s="1"/>
-      <c r="CF47" s="1"/>
-      <c r="CG47" s="1"/>
-      <c r="CH47" s="1"/>
-      <c r="CI47" s="1"/>
-      <c r="CJ47" s="1"/>
-      <c r="CK47" s="1"/>
-      <c r="CL47" s="1"/>
-      <c r="CM47" s="1"/>
+      <c r="BB47" s="15"/>
+      <c r="BC47" s="15"/>
+      <c r="BD47" s="15"/>
+      <c r="BE47" s="16"/>
+      <c r="BF47" s="15"/>
+      <c r="BG47" s="15"/>
+      <c r="BH47" s="15"/>
+      <c r="BI47" s="15"/>
+      <c r="BJ47" s="15"/>
+      <c r="BK47" s="15"/>
+      <c r="BL47" s="15"/>
+      <c r="BM47" s="15"/>
+      <c r="BN47" s="15"/>
+      <c r="BO47" s="15"/>
+      <c r="BP47" s="15"/>
+      <c r="BQ47" s="15"/>
+      <c r="BR47" s="15"/>
+      <c r="BS47" s="15"/>
+      <c r="BT47" s="15"/>
+      <c r="BU47" s="15"/>
+      <c r="BV47" s="15"/>
+      <c r="BW47" s="15"/>
+      <c r="BX47" s="15"/>
+      <c r="BY47" s="15"/>
+      <c r="BZ47" s="15"/>
+      <c r="CA47" s="15"/>
+      <c r="CB47" s="16"/>
+      <c r="CC47" s="15"/>
+      <c r="CD47" s="15"/>
+      <c r="CE47" s="15"/>
+      <c r="CF47" s="15"/>
+      <c r="CG47" s="15"/>
+      <c r="CH47" s="15"/>
+      <c r="CI47" s="15"/>
+      <c r="CJ47" s="15"/>
+      <c r="CK47" s="15"/>
+      <c r="CL47" s="15"/>
+      <c r="CM47" s="15"/>
       <c r="CN47" s="1"/>
-      <c r="CO47" s="1" t="s">
+      <c r="CO47" s="16"/>
+      <c r="CP47" s="16"/>
+      <c r="CQ47" s="16"/>
+      <c r="CR47" s="16"/>
+      <c r="CS47" s="16"/>
+      <c r="CT47" s="16"/>
+      <c r="CU47" s="16"/>
+      <c r="CV47" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP47" s="1"/>
+      <c r="CW47" s="16"/>
     </row>
     <row r="48" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -8672,8 +8777,8 @@
       <c r="H48" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="I48" s="29" t="s">
-        <v>265</v>
+      <c r="I48" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
@@ -8723,51 +8828,58 @@
       </c>
       <c r="AZ48" s="1"/>
       <c r="BA48" s="1"/>
-      <c r="BB48" s="1"/>
-      <c r="BC48" s="1"/>
-      <c r="BD48" s="1"/>
-      <c r="BE48" s="1"/>
-      <c r="BF48" s="1"/>
-      <c r="BG48" s="1"/>
-      <c r="BH48" s="1"/>
-      <c r="BI48" s="1"/>
-      <c r="BJ48" s="1"/>
-      <c r="BK48" s="1"/>
-      <c r="BL48" s="1"/>
-      <c r="BM48" s="1"/>
-      <c r="BN48" s="1"/>
-      <c r="BO48" s="1"/>
-      <c r="BP48" s="1"/>
-      <c r="BQ48" s="1"/>
-      <c r="BR48" s="1"/>
-      <c r="BS48" s="1"/>
-      <c r="BT48" s="1"/>
-      <c r="BU48" s="1"/>
-      <c r="BV48" s="1"/>
-      <c r="BW48" s="1"/>
-      <c r="BX48" s="1"/>
-      <c r="BY48" s="1"/>
-      <c r="BZ48" s="1"/>
-      <c r="CA48" s="1"/>
-      <c r="CB48" s="1"/>
-      <c r="CC48" s="1"/>
-      <c r="CD48" s="1"/>
-      <c r="CE48" s="1"/>
-      <c r="CF48" s="1"/>
-      <c r="CG48" s="1"/>
-      <c r="CH48" s="1"/>
-      <c r="CI48" s="1"/>
-      <c r="CJ48" s="1"/>
-      <c r="CK48" s="1"/>
-      <c r="CL48" s="1"/>
-      <c r="CM48" s="1"/>
+      <c r="BB48" s="15"/>
+      <c r="BC48" s="15"/>
+      <c r="BD48" s="15"/>
+      <c r="BE48" s="16"/>
+      <c r="BF48" s="15"/>
+      <c r="BG48" s="15"/>
+      <c r="BH48" s="15"/>
+      <c r="BI48" s="15"/>
+      <c r="BJ48" s="15"/>
+      <c r="BK48" s="15"/>
+      <c r="BL48" s="15"/>
+      <c r="BM48" s="15"/>
+      <c r="BN48" s="15"/>
+      <c r="BO48" s="15"/>
+      <c r="BP48" s="15"/>
+      <c r="BQ48" s="15"/>
+      <c r="BR48" s="15"/>
+      <c r="BS48" s="15"/>
+      <c r="BT48" s="15"/>
+      <c r="BU48" s="15"/>
+      <c r="BV48" s="15"/>
+      <c r="BW48" s="15"/>
+      <c r="BX48" s="15"/>
+      <c r="BY48" s="15"/>
+      <c r="BZ48" s="15"/>
+      <c r="CA48" s="15"/>
+      <c r="CB48" s="16"/>
+      <c r="CC48" s="15"/>
+      <c r="CD48" s="15"/>
+      <c r="CE48" s="15"/>
+      <c r="CF48" s="15"/>
+      <c r="CG48" s="15"/>
+      <c r="CH48" s="15"/>
+      <c r="CI48" s="15"/>
+      <c r="CJ48" s="15"/>
+      <c r="CK48" s="15"/>
+      <c r="CL48" s="15"/>
+      <c r="CM48" s="15"/>
       <c r="CN48" s="1"/>
-      <c r="CO48" s="1" t="s">
+      <c r="CO48" s="16"/>
+      <c r="CP48" s="16"/>
+      <c r="CQ48" s="16"/>
+      <c r="CR48" s="16"/>
+      <c r="CS48" s="16"/>
+      <c r="CT48" s="16"/>
+      <c r="CU48" s="16"/>
+      <c r="CV48" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP48" s="1"/>
+      <c r="CW48" s="16"/>
     </row>
-    <row r="49" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>444</v>
       </c>
@@ -8792,8 +8904,8 @@
       <c r="H49" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I49" s="29" t="s">
-        <v>265</v>
+      <c r="I49" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
@@ -8843,51 +8955,58 @@
       </c>
       <c r="AZ49" s="1"/>
       <c r="BA49" s="1"/>
-      <c r="BB49" s="1"/>
-      <c r="BC49" s="1"/>
-      <c r="BD49" s="1"/>
-      <c r="BE49" s="1"/>
-      <c r="BF49" s="1"/>
-      <c r="BG49" s="1"/>
-      <c r="BH49" s="1"/>
-      <c r="BI49" s="1"/>
-      <c r="BJ49" s="1"/>
-      <c r="BK49" s="1"/>
-      <c r="BL49" s="1"/>
-      <c r="BM49" s="1"/>
-      <c r="BN49" s="1"/>
-      <c r="BO49" s="1"/>
-      <c r="BP49" s="1"/>
-      <c r="BQ49" s="1"/>
-      <c r="BR49" s="1"/>
-      <c r="BS49" s="1"/>
-      <c r="BT49" s="1"/>
-      <c r="BU49" s="1"/>
-      <c r="BV49" s="1"/>
-      <c r="BW49" s="1"/>
-      <c r="BX49" s="1"/>
-      <c r="BY49" s="1"/>
-      <c r="BZ49" s="1"/>
-      <c r="CA49" s="1"/>
-      <c r="CB49" s="1"/>
-      <c r="CC49" s="1"/>
-      <c r="CD49" s="1"/>
-      <c r="CE49" s="1"/>
-      <c r="CF49" s="1"/>
-      <c r="CG49" s="1"/>
-      <c r="CH49" s="1"/>
-      <c r="CI49" s="1"/>
-      <c r="CJ49" s="1"/>
-      <c r="CK49" s="1"/>
-      <c r="CL49" s="1"/>
-      <c r="CM49" s="1"/>
+      <c r="BB49" s="15"/>
+      <c r="BC49" s="15"/>
+      <c r="BD49" s="15"/>
+      <c r="BE49" s="16"/>
+      <c r="BF49" s="15"/>
+      <c r="BG49" s="15"/>
+      <c r="BH49" s="15"/>
+      <c r="BI49" s="15"/>
+      <c r="BJ49" s="15"/>
+      <c r="BK49" s="15"/>
+      <c r="BL49" s="15"/>
+      <c r="BM49" s="15"/>
+      <c r="BN49" s="15"/>
+      <c r="BO49" s="15"/>
+      <c r="BP49" s="15"/>
+      <c r="BQ49" s="15"/>
+      <c r="BR49" s="15"/>
+      <c r="BS49" s="15"/>
+      <c r="BT49" s="15"/>
+      <c r="BU49" s="15"/>
+      <c r="BV49" s="15"/>
+      <c r="BW49" s="15"/>
+      <c r="BX49" s="15"/>
+      <c r="BY49" s="15"/>
+      <c r="BZ49" s="15"/>
+      <c r="CA49" s="15"/>
+      <c r="CB49" s="16"/>
+      <c r="CC49" s="15"/>
+      <c r="CD49" s="15"/>
+      <c r="CE49" s="15"/>
+      <c r="CF49" s="15"/>
+      <c r="CG49" s="15"/>
+      <c r="CH49" s="15"/>
+      <c r="CI49" s="15"/>
+      <c r="CJ49" s="15"/>
+      <c r="CK49" s="15"/>
+      <c r="CL49" s="15"/>
+      <c r="CM49" s="15"/>
       <c r="CN49" s="1"/>
-      <c r="CO49" s="1" t="s">
+      <c r="CO49" s="16"/>
+      <c r="CP49" s="16"/>
+      <c r="CQ49" s="16"/>
+      <c r="CR49" s="16"/>
+      <c r="CS49" s="16"/>
+      <c r="CT49" s="16"/>
+      <c r="CU49" s="16"/>
+      <c r="CV49" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP49" s="1"/>
+      <c r="CW49" s="16"/>
     </row>
-    <row r="50" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>449</v>
       </c>
@@ -8912,8 +9031,8 @@
       <c r="H50" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="I50" s="29" t="s">
-        <v>265</v>
+      <c r="I50" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
@@ -8963,51 +9082,58 @@
       </c>
       <c r="AZ50" s="1"/>
       <c r="BA50" s="1"/>
-      <c r="BB50" s="1"/>
-      <c r="BC50" s="1"/>
-      <c r="BD50" s="1"/>
-      <c r="BE50" s="1"/>
-      <c r="BF50" s="1"/>
-      <c r="BG50" s="1"/>
-      <c r="BH50" s="1"/>
-      <c r="BI50" s="1"/>
-      <c r="BJ50" s="1"/>
-      <c r="BK50" s="1"/>
-      <c r="BL50" s="1"/>
-      <c r="BM50" s="1"/>
-      <c r="BN50" s="1"/>
-      <c r="BO50" s="1"/>
-      <c r="BP50" s="1"/>
-      <c r="BQ50" s="1"/>
-      <c r="BR50" s="1"/>
-      <c r="BS50" s="1"/>
-      <c r="BT50" s="1"/>
-      <c r="BU50" s="1"/>
-      <c r="BV50" s="1"/>
-      <c r="BW50" s="1"/>
-      <c r="BX50" s="1"/>
-      <c r="BY50" s="1"/>
-      <c r="BZ50" s="1"/>
-      <c r="CA50" s="1"/>
-      <c r="CB50" s="1"/>
-      <c r="CC50" s="1"/>
-      <c r="CD50" s="1"/>
-      <c r="CE50" s="1"/>
-      <c r="CF50" s="1"/>
-      <c r="CG50" s="1"/>
-      <c r="CH50" s="1"/>
-      <c r="CI50" s="1"/>
-      <c r="CJ50" s="1"/>
-      <c r="CK50" s="1"/>
-      <c r="CL50" s="1"/>
-      <c r="CM50" s="1"/>
+      <c r="BB50" s="15"/>
+      <c r="BC50" s="15"/>
+      <c r="BD50" s="15"/>
+      <c r="BE50" s="16"/>
+      <c r="BF50" s="15"/>
+      <c r="BG50" s="15"/>
+      <c r="BH50" s="15"/>
+      <c r="BI50" s="15"/>
+      <c r="BJ50" s="15"/>
+      <c r="BK50" s="15"/>
+      <c r="BL50" s="15"/>
+      <c r="BM50" s="15"/>
+      <c r="BN50" s="15"/>
+      <c r="BO50" s="15"/>
+      <c r="BP50" s="15"/>
+      <c r="BQ50" s="15"/>
+      <c r="BR50" s="15"/>
+      <c r="BS50" s="15"/>
+      <c r="BT50" s="15"/>
+      <c r="BU50" s="15"/>
+      <c r="BV50" s="15"/>
+      <c r="BW50" s="15"/>
+      <c r="BX50" s="15"/>
+      <c r="BY50" s="15"/>
+      <c r="BZ50" s="15"/>
+      <c r="CA50" s="15"/>
+      <c r="CB50" s="16"/>
+      <c r="CC50" s="15"/>
+      <c r="CD50" s="15"/>
+      <c r="CE50" s="15"/>
+      <c r="CF50" s="15"/>
+      <c r="CG50" s="15"/>
+      <c r="CH50" s="15"/>
+      <c r="CI50" s="15"/>
+      <c r="CJ50" s="15"/>
+      <c r="CK50" s="15"/>
+      <c r="CL50" s="15"/>
+      <c r="CM50" s="15"/>
       <c r="CN50" s="1"/>
-      <c r="CO50" s="1" t="s">
+      <c r="CO50" s="16"/>
+      <c r="CP50" s="16"/>
+      <c r="CQ50" s="16"/>
+      <c r="CR50" s="16"/>
+      <c r="CS50" s="16"/>
+      <c r="CT50" s="16"/>
+      <c r="CU50" s="16"/>
+      <c r="CV50" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP50" s="1"/>
+      <c r="CW50" s="16"/>
     </row>
-    <row r="51" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>454</v>
       </c>
@@ -9032,8 +9158,8 @@
       <c r="H51" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I51" s="29" t="s">
-        <v>265</v>
+      <c r="I51" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
@@ -9083,51 +9209,58 @@
       </c>
       <c r="AZ51" s="1"/>
       <c r="BA51" s="1"/>
-      <c r="BB51" s="1"/>
-      <c r="BC51" s="1"/>
-      <c r="BD51" s="1"/>
-      <c r="BE51" s="1"/>
-      <c r="BF51" s="1"/>
-      <c r="BG51" s="1"/>
-      <c r="BH51" s="1"/>
-      <c r="BI51" s="1"/>
-      <c r="BJ51" s="1"/>
-      <c r="BK51" s="1"/>
-      <c r="BL51" s="1"/>
-      <c r="BM51" s="1"/>
-      <c r="BN51" s="1"/>
-      <c r="BO51" s="1"/>
-      <c r="BP51" s="1"/>
-      <c r="BQ51" s="1"/>
-      <c r="BR51" s="1"/>
-      <c r="BS51" s="1"/>
-      <c r="BT51" s="1"/>
-      <c r="BU51" s="1"/>
-      <c r="BV51" s="1"/>
-      <c r="BW51" s="1"/>
-      <c r="BX51" s="1"/>
-      <c r="BY51" s="1"/>
-      <c r="BZ51" s="1"/>
-      <c r="CA51" s="1"/>
-      <c r="CB51" s="1"/>
-      <c r="CC51" s="1"/>
-      <c r="CD51" s="1"/>
-      <c r="CE51" s="1"/>
-      <c r="CF51" s="1"/>
-      <c r="CG51" s="1"/>
-      <c r="CH51" s="1"/>
-      <c r="CI51" s="1"/>
-      <c r="CJ51" s="1"/>
-      <c r="CK51" s="1"/>
-      <c r="CL51" s="1"/>
-      <c r="CM51" s="1"/>
+      <c r="BB51" s="15"/>
+      <c r="BC51" s="15"/>
+      <c r="BD51" s="15"/>
+      <c r="BE51" s="16"/>
+      <c r="BF51" s="15"/>
+      <c r="BG51" s="15"/>
+      <c r="BH51" s="15"/>
+      <c r="BI51" s="15"/>
+      <c r="BJ51" s="15"/>
+      <c r="BK51" s="15"/>
+      <c r="BL51" s="15"/>
+      <c r="BM51" s="15"/>
+      <c r="BN51" s="15"/>
+      <c r="BO51" s="15"/>
+      <c r="BP51" s="15"/>
+      <c r="BQ51" s="15"/>
+      <c r="BR51" s="15"/>
+      <c r="BS51" s="15"/>
+      <c r="BT51" s="15"/>
+      <c r="BU51" s="15"/>
+      <c r="BV51" s="15"/>
+      <c r="BW51" s="15"/>
+      <c r="BX51" s="15"/>
+      <c r="BY51" s="15"/>
+      <c r="BZ51" s="15"/>
+      <c r="CA51" s="15"/>
+      <c r="CB51" s="16"/>
+      <c r="CC51" s="15"/>
+      <c r="CD51" s="15"/>
+      <c r="CE51" s="15"/>
+      <c r="CF51" s="15"/>
+      <c r="CG51" s="15"/>
+      <c r="CH51" s="15"/>
+      <c r="CI51" s="15"/>
+      <c r="CJ51" s="15"/>
+      <c r="CK51" s="15"/>
+      <c r="CL51" s="15"/>
+      <c r="CM51" s="15"/>
       <c r="CN51" s="1"/>
-      <c r="CO51" s="1" t="s">
+      <c r="CO51" s="16"/>
+      <c r="CP51" s="16"/>
+      <c r="CQ51" s="16"/>
+      <c r="CR51" s="16"/>
+      <c r="CS51" s="16"/>
+      <c r="CT51" s="16"/>
+      <c r="CU51" s="16"/>
+      <c r="CV51" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP51" s="1"/>
+      <c r="CW51" s="16"/>
     </row>
-    <row r="52" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>459</v>
       </c>
@@ -9150,8 +9283,8 @@
         <v>461</v>
       </c>
       <c r="H52" s="1"/>
-      <c r="I52" s="29" t="s">
-        <v>265</v>
+      <c r="I52" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
@@ -9201,51 +9334,58 @@
       </c>
       <c r="AZ52" s="1"/>
       <c r="BA52" s="1"/>
-      <c r="BB52" s="1"/>
-      <c r="BC52" s="1"/>
-      <c r="BD52" s="1"/>
-      <c r="BE52" s="1"/>
-      <c r="BF52" s="1"/>
-      <c r="BG52" s="1"/>
-      <c r="BH52" s="1"/>
-      <c r="BI52" s="1"/>
-      <c r="BJ52" s="1"/>
-      <c r="BK52" s="1"/>
-      <c r="BL52" s="1"/>
-      <c r="BM52" s="1"/>
-      <c r="BN52" s="1"/>
-      <c r="BO52" s="1"/>
-      <c r="BP52" s="1"/>
-      <c r="BQ52" s="1"/>
-      <c r="BR52" s="1"/>
-      <c r="BS52" s="1"/>
-      <c r="BT52" s="1"/>
-      <c r="BU52" s="1"/>
-      <c r="BV52" s="1"/>
-      <c r="BW52" s="1"/>
-      <c r="BX52" s="1"/>
-      <c r="BY52" s="1"/>
-      <c r="BZ52" s="1"/>
-      <c r="CA52" s="1"/>
-      <c r="CB52" s="1"/>
-      <c r="CC52" s="1"/>
-      <c r="CD52" s="1"/>
-      <c r="CE52" s="1"/>
-      <c r="CF52" s="1"/>
-      <c r="CG52" s="1"/>
-      <c r="CH52" s="1"/>
-      <c r="CI52" s="1"/>
-      <c r="CJ52" s="1"/>
-      <c r="CK52" s="1"/>
-      <c r="CL52" s="1"/>
-      <c r="CM52" s="1"/>
+      <c r="BB52" s="15"/>
+      <c r="BC52" s="15"/>
+      <c r="BD52" s="15"/>
+      <c r="BE52" s="16"/>
+      <c r="BF52" s="15"/>
+      <c r="BG52" s="15"/>
+      <c r="BH52" s="15"/>
+      <c r="BI52" s="15"/>
+      <c r="BJ52" s="15"/>
+      <c r="BK52" s="15"/>
+      <c r="BL52" s="15"/>
+      <c r="BM52" s="15"/>
+      <c r="BN52" s="15"/>
+      <c r="BO52" s="15"/>
+      <c r="BP52" s="15"/>
+      <c r="BQ52" s="15"/>
+      <c r="BR52" s="15"/>
+      <c r="BS52" s="15"/>
+      <c r="BT52" s="15"/>
+      <c r="BU52" s="15"/>
+      <c r="BV52" s="15"/>
+      <c r="BW52" s="15"/>
+      <c r="BX52" s="15"/>
+      <c r="BY52" s="15"/>
+      <c r="BZ52" s="15"/>
+      <c r="CA52" s="15"/>
+      <c r="CB52" s="16"/>
+      <c r="CC52" s="15"/>
+      <c r="CD52" s="15"/>
+      <c r="CE52" s="15"/>
+      <c r="CF52" s="15"/>
+      <c r="CG52" s="15"/>
+      <c r="CH52" s="15"/>
+      <c r="CI52" s="15"/>
+      <c r="CJ52" s="15"/>
+      <c r="CK52" s="15"/>
+      <c r="CL52" s="15"/>
+      <c r="CM52" s="15"/>
       <c r="CN52" s="1"/>
-      <c r="CO52" s="1" t="s">
+      <c r="CO52" s="16"/>
+      <c r="CP52" s="16"/>
+      <c r="CQ52" s="16"/>
+      <c r="CR52" s="16"/>
+      <c r="CS52" s="16"/>
+      <c r="CT52" s="16"/>
+      <c r="CU52" s="16"/>
+      <c r="CV52" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP52" s="1"/>
+      <c r="CW52" s="16"/>
     </row>
-    <row r="53" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>463</v>
       </c>
@@ -9268,8 +9408,8 @@
         <v>465</v>
       </c>
       <c r="H53" s="1"/>
-      <c r="I53" s="29" t="s">
-        <v>265</v>
+      <c r="I53" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
@@ -9319,51 +9459,58 @@
       </c>
       <c r="AZ53" s="1"/>
       <c r="BA53" s="1"/>
-      <c r="BB53" s="1"/>
-      <c r="BC53" s="1"/>
-      <c r="BD53" s="1"/>
-      <c r="BE53" s="1"/>
-      <c r="BF53" s="1"/>
-      <c r="BG53" s="1"/>
-      <c r="BH53" s="1"/>
-      <c r="BI53" s="1"/>
-      <c r="BJ53" s="1"/>
-      <c r="BK53" s="1"/>
-      <c r="BL53" s="1"/>
-      <c r="BM53" s="1"/>
-      <c r="BN53" s="1"/>
-      <c r="BO53" s="1"/>
-      <c r="BP53" s="1"/>
-      <c r="BQ53" s="1"/>
-      <c r="BR53" s="1"/>
-      <c r="BS53" s="1"/>
-      <c r="BT53" s="1"/>
-      <c r="BU53" s="1"/>
-      <c r="BV53" s="1"/>
-      <c r="BW53" s="1"/>
-      <c r="BX53" s="1"/>
-      <c r="BY53" s="1"/>
-      <c r="BZ53" s="1"/>
-      <c r="CA53" s="1"/>
-      <c r="CB53" s="1"/>
-      <c r="CC53" s="1"/>
-      <c r="CD53" s="1"/>
-      <c r="CE53" s="1"/>
-      <c r="CF53" s="1"/>
-      <c r="CG53" s="1"/>
-      <c r="CH53" s="1"/>
-      <c r="CI53" s="1"/>
-      <c r="CJ53" s="1"/>
-      <c r="CK53" s="1"/>
-      <c r="CL53" s="1"/>
-      <c r="CM53" s="1"/>
+      <c r="BB53" s="15"/>
+      <c r="BC53" s="15"/>
+      <c r="BD53" s="15"/>
+      <c r="BE53" s="16"/>
+      <c r="BF53" s="15"/>
+      <c r="BG53" s="15"/>
+      <c r="BH53" s="15"/>
+      <c r="BI53" s="15"/>
+      <c r="BJ53" s="15"/>
+      <c r="BK53" s="15"/>
+      <c r="BL53" s="15"/>
+      <c r="BM53" s="15"/>
+      <c r="BN53" s="15"/>
+      <c r="BO53" s="15"/>
+      <c r="BP53" s="15"/>
+      <c r="BQ53" s="15"/>
+      <c r="BR53" s="15"/>
+      <c r="BS53" s="15"/>
+      <c r="BT53" s="15"/>
+      <c r="BU53" s="15"/>
+      <c r="BV53" s="15"/>
+      <c r="BW53" s="15"/>
+      <c r="BX53" s="15"/>
+      <c r="BY53" s="15"/>
+      <c r="BZ53" s="15"/>
+      <c r="CA53" s="15"/>
+      <c r="CB53" s="16"/>
+      <c r="CC53" s="15"/>
+      <c r="CD53" s="15"/>
+      <c r="CE53" s="15"/>
+      <c r="CF53" s="15"/>
+      <c r="CG53" s="15"/>
+      <c r="CH53" s="15"/>
+      <c r="CI53" s="15"/>
+      <c r="CJ53" s="15"/>
+      <c r="CK53" s="15"/>
+      <c r="CL53" s="15"/>
+      <c r="CM53" s="15"/>
       <c r="CN53" s="1"/>
-      <c r="CO53" s="1" t="s">
+      <c r="CO53" s="16"/>
+      <c r="CP53" s="16"/>
+      <c r="CQ53" s="16"/>
+      <c r="CR53" s="16"/>
+      <c r="CS53" s="16"/>
+      <c r="CT53" s="16"/>
+      <c r="CU53" s="16"/>
+      <c r="CV53" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP53" s="1"/>
+      <c r="CW53" s="16"/>
     </row>
-    <row r="54" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>467</v>
       </c>
@@ -9388,8 +9535,8 @@
       <c r="H54" s="1" t="s">
         <v>470</v>
       </c>
-      <c r="I54" s="29" t="s">
-        <v>265</v>
+      <c r="I54" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
@@ -9439,51 +9586,58 @@
       </c>
       <c r="AZ54" s="1"/>
       <c r="BA54" s="1"/>
-      <c r="BB54" s="1"/>
-      <c r="BC54" s="1"/>
-      <c r="BD54" s="1"/>
-      <c r="BE54" s="1"/>
-      <c r="BF54" s="1"/>
-      <c r="BG54" s="1"/>
-      <c r="BH54" s="1"/>
-      <c r="BI54" s="1"/>
-      <c r="BJ54" s="1"/>
-      <c r="BK54" s="1"/>
-      <c r="BL54" s="1"/>
-      <c r="BM54" s="1"/>
-      <c r="BN54" s="1"/>
-      <c r="BO54" s="1"/>
-      <c r="BP54" s="1"/>
-      <c r="BQ54" s="1"/>
-      <c r="BR54" s="1"/>
-      <c r="BS54" s="1"/>
-      <c r="BT54" s="1"/>
-      <c r="BU54" s="1"/>
-      <c r="BV54" s="1"/>
-      <c r="BW54" s="1"/>
-      <c r="BX54" s="1"/>
-      <c r="BY54" s="1"/>
-      <c r="BZ54" s="1"/>
-      <c r="CA54" s="1"/>
-      <c r="CB54" s="1"/>
-      <c r="CC54" s="1"/>
-      <c r="CD54" s="1"/>
-      <c r="CE54" s="1"/>
-      <c r="CF54" s="1"/>
-      <c r="CG54" s="1"/>
-      <c r="CH54" s="1"/>
-      <c r="CI54" s="1"/>
-      <c r="CJ54" s="1"/>
-      <c r="CK54" s="1"/>
-      <c r="CL54" s="1"/>
-      <c r="CM54" s="1"/>
+      <c r="BB54" s="15"/>
+      <c r="BC54" s="15"/>
+      <c r="BD54" s="15"/>
+      <c r="BE54" s="16"/>
+      <c r="BF54" s="15"/>
+      <c r="BG54" s="15"/>
+      <c r="BH54" s="15"/>
+      <c r="BI54" s="15"/>
+      <c r="BJ54" s="15"/>
+      <c r="BK54" s="15"/>
+      <c r="BL54" s="15"/>
+      <c r="BM54" s="15"/>
+      <c r="BN54" s="15"/>
+      <c r="BO54" s="15"/>
+      <c r="BP54" s="15"/>
+      <c r="BQ54" s="15"/>
+      <c r="BR54" s="15"/>
+      <c r="BS54" s="15"/>
+      <c r="BT54" s="15"/>
+      <c r="BU54" s="15"/>
+      <c r="BV54" s="15"/>
+      <c r="BW54" s="15"/>
+      <c r="BX54" s="15"/>
+      <c r="BY54" s="15"/>
+      <c r="BZ54" s="15"/>
+      <c r="CA54" s="15"/>
+      <c r="CB54" s="16"/>
+      <c r="CC54" s="15"/>
+      <c r="CD54" s="15"/>
+      <c r="CE54" s="15"/>
+      <c r="CF54" s="15"/>
+      <c r="CG54" s="15"/>
+      <c r="CH54" s="15"/>
+      <c r="CI54" s="15"/>
+      <c r="CJ54" s="15"/>
+      <c r="CK54" s="15"/>
+      <c r="CL54" s="15"/>
+      <c r="CM54" s="15"/>
       <c r="CN54" s="1"/>
-      <c r="CO54" s="1" t="s">
+      <c r="CO54" s="16"/>
+      <c r="CP54" s="16"/>
+      <c r="CQ54" s="16"/>
+      <c r="CR54" s="16"/>
+      <c r="CS54" s="16"/>
+      <c r="CT54" s="16"/>
+      <c r="CU54" s="16"/>
+      <c r="CV54" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP54" s="1"/>
+      <c r="CW54" s="16"/>
     </row>
-    <row r="55" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>472</v>
       </c>
@@ -9508,8 +9662,8 @@
       <c r="H55" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="I55" s="29" t="s">
-        <v>265</v>
+      <c r="I55" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
@@ -9559,51 +9713,58 @@
       </c>
       <c r="AZ55" s="1"/>
       <c r="BA55" s="1"/>
-      <c r="BB55" s="1"/>
-      <c r="BC55" s="1"/>
-      <c r="BD55" s="1"/>
-      <c r="BE55" s="1"/>
-      <c r="BF55" s="1"/>
-      <c r="BG55" s="1"/>
-      <c r="BH55" s="1"/>
-      <c r="BI55" s="1"/>
-      <c r="BJ55" s="1"/>
-      <c r="BK55" s="1"/>
-      <c r="BL55" s="1"/>
-      <c r="BM55" s="1"/>
-      <c r="BN55" s="1"/>
-      <c r="BO55" s="1"/>
-      <c r="BP55" s="1"/>
-      <c r="BQ55" s="1"/>
-      <c r="BR55" s="1"/>
-      <c r="BS55" s="1"/>
-      <c r="BT55" s="1"/>
-      <c r="BU55" s="1"/>
-      <c r="BV55" s="1"/>
-      <c r="BW55" s="1"/>
-      <c r="BX55" s="1"/>
-      <c r="BY55" s="1"/>
-      <c r="BZ55" s="1"/>
-      <c r="CA55" s="1"/>
-      <c r="CB55" s="1"/>
-      <c r="CC55" s="1"/>
-      <c r="CD55" s="1"/>
-      <c r="CE55" s="1"/>
-      <c r="CF55" s="1"/>
-      <c r="CG55" s="1"/>
-      <c r="CH55" s="1"/>
-      <c r="CI55" s="1"/>
-      <c r="CJ55" s="1"/>
-      <c r="CK55" s="1"/>
-      <c r="CL55" s="1"/>
-      <c r="CM55" s="1"/>
+      <c r="BB55" s="15"/>
+      <c r="BC55" s="15"/>
+      <c r="BD55" s="15"/>
+      <c r="BE55" s="16"/>
+      <c r="BF55" s="15"/>
+      <c r="BG55" s="15"/>
+      <c r="BH55" s="15"/>
+      <c r="BI55" s="15"/>
+      <c r="BJ55" s="15"/>
+      <c r="BK55" s="15"/>
+      <c r="BL55" s="15"/>
+      <c r="BM55" s="15"/>
+      <c r="BN55" s="15"/>
+      <c r="BO55" s="15"/>
+      <c r="BP55" s="15"/>
+      <c r="BQ55" s="15"/>
+      <c r="BR55" s="15"/>
+      <c r="BS55" s="15"/>
+      <c r="BT55" s="15"/>
+      <c r="BU55" s="15"/>
+      <c r="BV55" s="15"/>
+      <c r="BW55" s="15"/>
+      <c r="BX55" s="15"/>
+      <c r="BY55" s="15"/>
+      <c r="BZ55" s="15"/>
+      <c r="CA55" s="15"/>
+      <c r="CB55" s="16"/>
+      <c r="CC55" s="15"/>
+      <c r="CD55" s="15"/>
+      <c r="CE55" s="15"/>
+      <c r="CF55" s="15"/>
+      <c r="CG55" s="15"/>
+      <c r="CH55" s="15"/>
+      <c r="CI55" s="15"/>
+      <c r="CJ55" s="15"/>
+      <c r="CK55" s="15"/>
+      <c r="CL55" s="15"/>
+      <c r="CM55" s="15"/>
       <c r="CN55" s="1"/>
-      <c r="CO55" s="1" t="s">
+      <c r="CO55" s="16"/>
+      <c r="CP55" s="16"/>
+      <c r="CQ55" s="16"/>
+      <c r="CR55" s="16"/>
+      <c r="CS55" s="16"/>
+      <c r="CT55" s="16"/>
+      <c r="CU55" s="16"/>
+      <c r="CV55" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP55" s="1"/>
+      <c r="CW55" s="16"/>
     </row>
-    <row r="56" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>477</v>
       </c>
@@ -9626,8 +9787,8 @@
         <v>479</v>
       </c>
       <c r="H56" s="1"/>
-      <c r="I56" s="29" t="s">
-        <v>265</v>
+      <c r="I56" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
@@ -9679,51 +9840,58 @@
       </c>
       <c r="AZ56" s="1"/>
       <c r="BA56" s="1"/>
-      <c r="BB56" s="1"/>
-      <c r="BC56" s="1"/>
-      <c r="BD56" s="1"/>
-      <c r="BE56" s="1"/>
-      <c r="BF56" s="1"/>
-      <c r="BG56" s="1"/>
-      <c r="BH56" s="1"/>
-      <c r="BI56" s="1"/>
-      <c r="BJ56" s="1"/>
-      <c r="BK56" s="1"/>
-      <c r="BL56" s="1"/>
-      <c r="BM56" s="1"/>
-      <c r="BN56" s="1"/>
-      <c r="BO56" s="1"/>
-      <c r="BP56" s="1"/>
-      <c r="BQ56" s="1"/>
-      <c r="BR56" s="1"/>
-      <c r="BS56" s="1"/>
-      <c r="BT56" s="1"/>
-      <c r="BU56" s="1"/>
-      <c r="BV56" s="1"/>
-      <c r="BW56" s="1"/>
-      <c r="BX56" s="1"/>
-      <c r="BY56" s="1"/>
-      <c r="BZ56" s="1"/>
-      <c r="CA56" s="1"/>
-      <c r="CB56" s="1"/>
-      <c r="CC56" s="1"/>
-      <c r="CD56" s="1"/>
-      <c r="CE56" s="1"/>
-      <c r="CF56" s="1"/>
-      <c r="CG56" s="1"/>
-      <c r="CH56" s="1"/>
-      <c r="CI56" s="1"/>
-      <c r="CJ56" s="1"/>
-      <c r="CK56" s="1"/>
-      <c r="CL56" s="1"/>
-      <c r="CM56" s="1"/>
+      <c r="BB56" s="15"/>
+      <c r="BC56" s="15"/>
+      <c r="BD56" s="15"/>
+      <c r="BE56" s="16"/>
+      <c r="BF56" s="15"/>
+      <c r="BG56" s="15"/>
+      <c r="BH56" s="15"/>
+      <c r="BI56" s="15"/>
+      <c r="BJ56" s="15"/>
+      <c r="BK56" s="15"/>
+      <c r="BL56" s="15"/>
+      <c r="BM56" s="15"/>
+      <c r="BN56" s="15"/>
+      <c r="BO56" s="15"/>
+      <c r="BP56" s="15"/>
+      <c r="BQ56" s="15"/>
+      <c r="BR56" s="15"/>
+      <c r="BS56" s="15"/>
+      <c r="BT56" s="15"/>
+      <c r="BU56" s="15"/>
+      <c r="BV56" s="15"/>
+      <c r="BW56" s="15"/>
+      <c r="BX56" s="15"/>
+      <c r="BY56" s="15"/>
+      <c r="BZ56" s="15"/>
+      <c r="CA56" s="15"/>
+      <c r="CB56" s="16"/>
+      <c r="CC56" s="15"/>
+      <c r="CD56" s="15"/>
+      <c r="CE56" s="15"/>
+      <c r="CF56" s="15"/>
+      <c r="CG56" s="15"/>
+      <c r="CH56" s="15"/>
+      <c r="CI56" s="15"/>
+      <c r="CJ56" s="15"/>
+      <c r="CK56" s="15"/>
+      <c r="CL56" s="15"/>
+      <c r="CM56" s="15"/>
       <c r="CN56" s="1"/>
-      <c r="CO56" s="1" t="s">
+      <c r="CO56" s="16"/>
+      <c r="CP56" s="16"/>
+      <c r="CQ56" s="16"/>
+      <c r="CR56" s="16"/>
+      <c r="CS56" s="16"/>
+      <c r="CT56" s="16"/>
+      <c r="CU56" s="16"/>
+      <c r="CV56" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP56" s="1"/>
+      <c r="CW56" s="16"/>
     </row>
-    <row r="57" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>482</v>
       </c>
@@ -9746,8 +9914,8 @@
         <v>484</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="I57" s="29" t="s">
-        <v>265</v>
+      <c r="I57" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
@@ -9799,51 +9967,58 @@
       </c>
       <c r="AZ57" s="1"/>
       <c r="BA57" s="1"/>
-      <c r="BB57" s="1"/>
-      <c r="BC57" s="1"/>
-      <c r="BD57" s="1"/>
-      <c r="BE57" s="1"/>
-      <c r="BF57" s="1"/>
-      <c r="BG57" s="1"/>
-      <c r="BH57" s="1"/>
-      <c r="BI57" s="1"/>
-      <c r="BJ57" s="1"/>
-      <c r="BK57" s="1"/>
-      <c r="BL57" s="1"/>
-      <c r="BM57" s="1"/>
-      <c r="BN57" s="1"/>
-      <c r="BO57" s="1"/>
-      <c r="BP57" s="1"/>
-      <c r="BQ57" s="1"/>
-      <c r="BR57" s="1"/>
-      <c r="BS57" s="1"/>
-      <c r="BT57" s="1"/>
-      <c r="BU57" s="1"/>
-      <c r="BV57" s="1"/>
-      <c r="BW57" s="1"/>
-      <c r="BX57" s="1"/>
-      <c r="BY57" s="1"/>
-      <c r="BZ57" s="1"/>
-      <c r="CA57" s="1"/>
-      <c r="CB57" s="1"/>
-      <c r="CC57" s="1"/>
-      <c r="CD57" s="1"/>
-      <c r="CE57" s="1"/>
-      <c r="CF57" s="1"/>
-      <c r="CG57" s="1"/>
-      <c r="CH57" s="1"/>
-      <c r="CI57" s="1"/>
-      <c r="CJ57" s="1"/>
-      <c r="CK57" s="1"/>
-      <c r="CL57" s="1"/>
-      <c r="CM57" s="1"/>
+      <c r="BB57" s="15"/>
+      <c r="BC57" s="15"/>
+      <c r="BD57" s="15"/>
+      <c r="BE57" s="16"/>
+      <c r="BF57" s="15"/>
+      <c r="BG57" s="15"/>
+      <c r="BH57" s="15"/>
+      <c r="BI57" s="15"/>
+      <c r="BJ57" s="15"/>
+      <c r="BK57" s="15"/>
+      <c r="BL57" s="15"/>
+      <c r="BM57" s="15"/>
+      <c r="BN57" s="15"/>
+      <c r="BO57" s="15"/>
+      <c r="BP57" s="15"/>
+      <c r="BQ57" s="15"/>
+      <c r="BR57" s="15"/>
+      <c r="BS57" s="15"/>
+      <c r="BT57" s="15"/>
+      <c r="BU57" s="15"/>
+      <c r="BV57" s="15"/>
+      <c r="BW57" s="15"/>
+      <c r="BX57" s="15"/>
+      <c r="BY57" s="15"/>
+      <c r="BZ57" s="15"/>
+      <c r="CA57" s="15"/>
+      <c r="CB57" s="16"/>
+      <c r="CC57" s="15"/>
+      <c r="CD57" s="15"/>
+      <c r="CE57" s="15"/>
+      <c r="CF57" s="15"/>
+      <c r="CG57" s="15"/>
+      <c r="CH57" s="15"/>
+      <c r="CI57" s="15"/>
+      <c r="CJ57" s="15"/>
+      <c r="CK57" s="15"/>
+      <c r="CL57" s="15"/>
+      <c r="CM57" s="15"/>
       <c r="CN57" s="1"/>
-      <c r="CO57" s="1" t="s">
+      <c r="CO57" s="16"/>
+      <c r="CP57" s="16"/>
+      <c r="CQ57" s="16"/>
+      <c r="CR57" s="16"/>
+      <c r="CS57" s="16"/>
+      <c r="CT57" s="16"/>
+      <c r="CU57" s="16"/>
+      <c r="CV57" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP57" s="1"/>
+      <c r="CW57" s="16"/>
     </row>
-    <row r="58" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>486</v>
       </c>
@@ -9868,8 +10043,8 @@
       <c r="H58" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="I58" s="29" t="s">
-        <v>265</v>
+      <c r="I58" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
@@ -9921,51 +10096,58 @@
         <v>491</v>
       </c>
       <c r="BA58" s="1"/>
-      <c r="BB58" s="1"/>
-      <c r="BC58" s="1"/>
-      <c r="BD58" s="1"/>
-      <c r="BE58" s="1"/>
-      <c r="BF58" s="1"/>
-      <c r="BG58" s="1"/>
-      <c r="BH58" s="1"/>
-      <c r="BI58" s="1"/>
-      <c r="BJ58" s="1"/>
-      <c r="BK58" s="1"/>
-      <c r="BL58" s="1"/>
-      <c r="BM58" s="1"/>
-      <c r="BN58" s="1"/>
-      <c r="BO58" s="1"/>
-      <c r="BP58" s="1"/>
-      <c r="BQ58" s="1"/>
-      <c r="BR58" s="1"/>
-      <c r="BS58" s="1"/>
-      <c r="BT58" s="1"/>
-      <c r="BU58" s="1"/>
-      <c r="BV58" s="1"/>
-      <c r="BW58" s="1"/>
-      <c r="BX58" s="1"/>
-      <c r="BY58" s="1"/>
-      <c r="BZ58" s="1"/>
-      <c r="CA58" s="1"/>
-      <c r="CB58" s="1"/>
-      <c r="CC58" s="1"/>
-      <c r="CD58" s="1"/>
-      <c r="CE58" s="1"/>
-      <c r="CF58" s="1"/>
-      <c r="CG58" s="1"/>
-      <c r="CH58" s="1"/>
-      <c r="CI58" s="1"/>
-      <c r="CJ58" s="1"/>
-      <c r="CK58" s="1"/>
-      <c r="CL58" s="1"/>
-      <c r="CM58" s="1"/>
+      <c r="BB58" s="15"/>
+      <c r="BC58" s="15"/>
+      <c r="BD58" s="15"/>
+      <c r="BE58" s="16"/>
+      <c r="BF58" s="15"/>
+      <c r="BG58" s="15"/>
+      <c r="BH58" s="15"/>
+      <c r="BI58" s="15"/>
+      <c r="BJ58" s="15"/>
+      <c r="BK58" s="15"/>
+      <c r="BL58" s="15"/>
+      <c r="BM58" s="15"/>
+      <c r="BN58" s="15"/>
+      <c r="BO58" s="15"/>
+      <c r="BP58" s="15"/>
+      <c r="BQ58" s="15"/>
+      <c r="BR58" s="15"/>
+      <c r="BS58" s="15"/>
+      <c r="BT58" s="15"/>
+      <c r="BU58" s="15"/>
+      <c r="BV58" s="15"/>
+      <c r="BW58" s="15"/>
+      <c r="BX58" s="15"/>
+      <c r="BY58" s="15"/>
+      <c r="BZ58" s="15"/>
+      <c r="CA58" s="15"/>
+      <c r="CB58" s="16"/>
+      <c r="CC58" s="15"/>
+      <c r="CD58" s="15"/>
+      <c r="CE58" s="15"/>
+      <c r="CF58" s="15"/>
+      <c r="CG58" s="15"/>
+      <c r="CH58" s="15"/>
+      <c r="CI58" s="15"/>
+      <c r="CJ58" s="15"/>
+      <c r="CK58" s="15"/>
+      <c r="CL58" s="15"/>
+      <c r="CM58" s="15"/>
       <c r="CN58" s="1"/>
-      <c r="CO58" s="1" t="s">
+      <c r="CO58" s="16"/>
+      <c r="CP58" s="16"/>
+      <c r="CQ58" s="16"/>
+      <c r="CR58" s="16"/>
+      <c r="CS58" s="16"/>
+      <c r="CT58" s="16"/>
+      <c r="CU58" s="16"/>
+      <c r="CV58" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP58" s="1"/>
+      <c r="CW58" s="16"/>
     </row>
-    <row r="59" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>492</v>
       </c>
@@ -9990,8 +10172,8 @@
       <c r="H59" s="1" t="s">
         <v>489</v>
       </c>
-      <c r="I59" s="29" t="s">
-        <v>265</v>
+      <c r="I59" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
@@ -10043,51 +10225,58 @@
         <v>491</v>
       </c>
       <c r="BA59" s="1"/>
-      <c r="BB59" s="1"/>
-      <c r="BC59" s="1"/>
-      <c r="BD59" s="1"/>
-      <c r="BE59" s="1"/>
-      <c r="BF59" s="1"/>
-      <c r="BG59" s="1"/>
-      <c r="BH59" s="1"/>
-      <c r="BI59" s="1"/>
-      <c r="BJ59" s="1"/>
-      <c r="BK59" s="1"/>
-      <c r="BL59" s="1"/>
-      <c r="BM59" s="1"/>
-      <c r="BN59" s="1"/>
-      <c r="BO59" s="1"/>
-      <c r="BP59" s="1"/>
-      <c r="BQ59" s="1"/>
-      <c r="BR59" s="1"/>
-      <c r="BS59" s="1"/>
-      <c r="BT59" s="1"/>
-      <c r="BU59" s="1"/>
-      <c r="BV59" s="1"/>
-      <c r="BW59" s="1"/>
-      <c r="BX59" s="1"/>
-      <c r="BY59" s="1"/>
-      <c r="BZ59" s="1"/>
-      <c r="CA59" s="1"/>
-      <c r="CB59" s="1"/>
-      <c r="CC59" s="1"/>
-      <c r="CD59" s="1"/>
-      <c r="CE59" s="1"/>
-      <c r="CF59" s="1"/>
-      <c r="CG59" s="1"/>
-      <c r="CH59" s="1"/>
-      <c r="CI59" s="1"/>
-      <c r="CJ59" s="1"/>
-      <c r="CK59" s="1"/>
-      <c r="CL59" s="1"/>
-      <c r="CM59" s="1"/>
+      <c r="BB59" s="15"/>
+      <c r="BC59" s="15"/>
+      <c r="BD59" s="15"/>
+      <c r="BE59" s="16"/>
+      <c r="BF59" s="15"/>
+      <c r="BG59" s="15"/>
+      <c r="BH59" s="15"/>
+      <c r="BI59" s="15"/>
+      <c r="BJ59" s="15"/>
+      <c r="BK59" s="15"/>
+      <c r="BL59" s="15"/>
+      <c r="BM59" s="15"/>
+      <c r="BN59" s="15"/>
+      <c r="BO59" s="15"/>
+      <c r="BP59" s="15"/>
+      <c r="BQ59" s="15"/>
+      <c r="BR59" s="15"/>
+      <c r="BS59" s="15"/>
+      <c r="BT59" s="15"/>
+      <c r="BU59" s="15"/>
+      <c r="BV59" s="15"/>
+      <c r="BW59" s="15"/>
+      <c r="BX59" s="15"/>
+      <c r="BY59" s="15"/>
+      <c r="BZ59" s="15"/>
+      <c r="CA59" s="15"/>
+      <c r="CB59" s="16"/>
+      <c r="CC59" s="15"/>
+      <c r="CD59" s="15"/>
+      <c r="CE59" s="15"/>
+      <c r="CF59" s="15"/>
+      <c r="CG59" s="15"/>
+      <c r="CH59" s="15"/>
+      <c r="CI59" s="15"/>
+      <c r="CJ59" s="15"/>
+      <c r="CK59" s="15"/>
+      <c r="CL59" s="15"/>
+      <c r="CM59" s="15"/>
       <c r="CN59" s="1"/>
-      <c r="CO59" s="1" t="s">
+      <c r="CO59" s="16"/>
+      <c r="CP59" s="16"/>
+      <c r="CQ59" s="16"/>
+      <c r="CR59" s="16"/>
+      <c r="CS59" s="16"/>
+      <c r="CT59" s="16"/>
+      <c r="CU59" s="16"/>
+      <c r="CV59" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP59" s="1"/>
+      <c r="CW59" s="16"/>
     </row>
-    <row r="60" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>496</v>
       </c>
@@ -10112,8 +10301,8 @@
       <c r="H60" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="I60" s="29" t="s">
-        <v>265</v>
+      <c r="I60" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
@@ -10165,51 +10354,58 @@
       </c>
       <c r="AZ60" s="1"/>
       <c r="BA60" s="1"/>
-      <c r="BB60" s="1"/>
-      <c r="BC60" s="1"/>
-      <c r="BD60" s="1"/>
-      <c r="BE60" s="1"/>
-      <c r="BF60" s="1"/>
-      <c r="BG60" s="1"/>
-      <c r="BH60" s="1"/>
-      <c r="BI60" s="1"/>
-      <c r="BJ60" s="1"/>
-      <c r="BK60" s="1"/>
-      <c r="BL60" s="1"/>
-      <c r="BM60" s="1"/>
-      <c r="BN60" s="1"/>
-      <c r="BO60" s="1"/>
-      <c r="BP60" s="1"/>
-      <c r="BQ60" s="1"/>
-      <c r="BR60" s="1"/>
-      <c r="BS60" s="1"/>
-      <c r="BT60" s="1"/>
-      <c r="BU60" s="1"/>
-      <c r="BV60" s="1"/>
-      <c r="BW60" s="1"/>
-      <c r="BX60" s="1"/>
-      <c r="BY60" s="1"/>
-      <c r="BZ60" s="1"/>
-      <c r="CA60" s="1"/>
-      <c r="CB60" s="1"/>
-      <c r="CC60" s="1"/>
-      <c r="CD60" s="1"/>
-      <c r="CE60" s="1"/>
-      <c r="CF60" s="1"/>
-      <c r="CG60" s="1"/>
-      <c r="CH60" s="1"/>
-      <c r="CI60" s="1"/>
-      <c r="CJ60" s="1"/>
-      <c r="CK60" s="1"/>
-      <c r="CL60" s="1"/>
-      <c r="CM60" s="1"/>
+      <c r="BB60" s="15"/>
+      <c r="BC60" s="15"/>
+      <c r="BD60" s="15"/>
+      <c r="BE60" s="16"/>
+      <c r="BF60" s="15"/>
+      <c r="BG60" s="15"/>
+      <c r="BH60" s="15"/>
+      <c r="BI60" s="15"/>
+      <c r="BJ60" s="15"/>
+      <c r="BK60" s="15"/>
+      <c r="BL60" s="15"/>
+      <c r="BM60" s="15"/>
+      <c r="BN60" s="15"/>
+      <c r="BO60" s="15"/>
+      <c r="BP60" s="15"/>
+      <c r="BQ60" s="15"/>
+      <c r="BR60" s="15"/>
+      <c r="BS60" s="15"/>
+      <c r="BT60" s="15"/>
+      <c r="BU60" s="15"/>
+      <c r="BV60" s="15"/>
+      <c r="BW60" s="15"/>
+      <c r="BX60" s="15"/>
+      <c r="BY60" s="15"/>
+      <c r="BZ60" s="15"/>
+      <c r="CA60" s="15"/>
+      <c r="CB60" s="16"/>
+      <c r="CC60" s="15"/>
+      <c r="CD60" s="15"/>
+      <c r="CE60" s="15"/>
+      <c r="CF60" s="15"/>
+      <c r="CG60" s="15"/>
+      <c r="CH60" s="15"/>
+      <c r="CI60" s="15"/>
+      <c r="CJ60" s="15"/>
+      <c r="CK60" s="15"/>
+      <c r="CL60" s="15"/>
+      <c r="CM60" s="15"/>
       <c r="CN60" s="1"/>
-      <c r="CO60" s="1" t="s">
+      <c r="CO60" s="16"/>
+      <c r="CP60" s="16"/>
+      <c r="CQ60" s="16"/>
+      <c r="CR60" s="16"/>
+      <c r="CS60" s="16"/>
+      <c r="CT60" s="16"/>
+      <c r="CU60" s="16"/>
+      <c r="CV60" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP60" s="1"/>
+      <c r="CW60" s="16"/>
     </row>
-    <row r="61" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>501</v>
       </c>
@@ -10234,8 +10430,8 @@
       <c r="H61" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="I61" s="29" t="s">
-        <v>265</v>
+      <c r="I61" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
@@ -10287,51 +10483,58 @@
       </c>
       <c r="AZ61" s="1"/>
       <c r="BA61" s="1"/>
-      <c r="BB61" s="1"/>
-      <c r="BC61" s="1"/>
-      <c r="BD61" s="1"/>
-      <c r="BE61" s="1"/>
-      <c r="BF61" s="1"/>
-      <c r="BG61" s="1"/>
-      <c r="BH61" s="1"/>
-      <c r="BI61" s="1"/>
-      <c r="BJ61" s="1"/>
-      <c r="BK61" s="1"/>
-      <c r="BL61" s="1"/>
-      <c r="BM61" s="1"/>
-      <c r="BN61" s="1"/>
-      <c r="BO61" s="1"/>
-      <c r="BP61" s="1"/>
-      <c r="BQ61" s="1"/>
-      <c r="BR61" s="1"/>
-      <c r="BS61" s="1"/>
-      <c r="BT61" s="1"/>
-      <c r="BU61" s="1"/>
-      <c r="BV61" s="1"/>
-      <c r="BW61" s="1"/>
-      <c r="BX61" s="1"/>
-      <c r="BY61" s="1"/>
-      <c r="BZ61" s="1"/>
-      <c r="CA61" s="1"/>
-      <c r="CB61" s="1"/>
-      <c r="CC61" s="1"/>
-      <c r="CD61" s="1"/>
-      <c r="CE61" s="1"/>
-      <c r="CF61" s="1"/>
-      <c r="CG61" s="1"/>
-      <c r="CH61" s="1"/>
-      <c r="CI61" s="1"/>
-      <c r="CJ61" s="1"/>
-      <c r="CK61" s="1"/>
-      <c r="CL61" s="1"/>
-      <c r="CM61" s="1"/>
+      <c r="BB61" s="15"/>
+      <c r="BC61" s="15"/>
+      <c r="BD61" s="15"/>
+      <c r="BE61" s="16"/>
+      <c r="BF61" s="15"/>
+      <c r="BG61" s="15"/>
+      <c r="BH61" s="15"/>
+      <c r="BI61" s="15"/>
+      <c r="BJ61" s="15"/>
+      <c r="BK61" s="15"/>
+      <c r="BL61" s="15"/>
+      <c r="BM61" s="15"/>
+      <c r="BN61" s="15"/>
+      <c r="BO61" s="15"/>
+      <c r="BP61" s="15"/>
+      <c r="BQ61" s="15"/>
+      <c r="BR61" s="15"/>
+      <c r="BS61" s="15"/>
+      <c r="BT61" s="15"/>
+      <c r="BU61" s="15"/>
+      <c r="BV61" s="15"/>
+      <c r="BW61" s="15"/>
+      <c r="BX61" s="15"/>
+      <c r="BY61" s="15"/>
+      <c r="BZ61" s="15"/>
+      <c r="CA61" s="15"/>
+      <c r="CB61" s="16"/>
+      <c r="CC61" s="15"/>
+      <c r="CD61" s="15"/>
+      <c r="CE61" s="15"/>
+      <c r="CF61" s="15"/>
+      <c r="CG61" s="15"/>
+      <c r="CH61" s="15"/>
+      <c r="CI61" s="15"/>
+      <c r="CJ61" s="15"/>
+      <c r="CK61" s="15"/>
+      <c r="CL61" s="15"/>
+      <c r="CM61" s="15"/>
       <c r="CN61" s="1"/>
-      <c r="CO61" s="1" t="s">
+      <c r="CO61" s="16"/>
+      <c r="CP61" s="16"/>
+      <c r="CQ61" s="16"/>
+      <c r="CR61" s="16"/>
+      <c r="CS61" s="16"/>
+      <c r="CT61" s="16"/>
+      <c r="CU61" s="16"/>
+      <c r="CV61" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP61" s="1"/>
+      <c r="CW61" s="16"/>
     </row>
-    <row r="62" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>505</v>
       </c>
@@ -10356,8 +10559,8 @@
       <c r="H62" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="I62" s="29" t="s">
-        <v>265</v>
+      <c r="I62" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
@@ -10409,51 +10612,58 @@
       <c r="BA62" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="BB62" s="1"/>
-      <c r="BC62" s="1"/>
-      <c r="BD62" s="1"/>
-      <c r="BE62" s="1"/>
-      <c r="BF62" s="1"/>
-      <c r="BG62" s="1"/>
-      <c r="BH62" s="1"/>
-      <c r="BI62" s="1"/>
-      <c r="BJ62" s="1"/>
-      <c r="BK62" s="1"/>
-      <c r="BL62" s="1"/>
-      <c r="BM62" s="1"/>
-      <c r="BN62" s="1"/>
-      <c r="BO62" s="1"/>
-      <c r="BP62" s="1"/>
-      <c r="BQ62" s="1"/>
-      <c r="BR62" s="1"/>
-      <c r="BS62" s="1"/>
-      <c r="BT62" s="1"/>
-      <c r="BU62" s="1"/>
-      <c r="BV62" s="1"/>
-      <c r="BW62" s="1"/>
-      <c r="BX62" s="1"/>
-      <c r="BY62" s="1"/>
-      <c r="BZ62" s="1"/>
-      <c r="CA62" s="1"/>
-      <c r="CB62" s="1"/>
-      <c r="CC62" s="1"/>
-      <c r="CD62" s="1"/>
-      <c r="CE62" s="1"/>
-      <c r="CF62" s="1"/>
-      <c r="CG62" s="1"/>
-      <c r="CH62" s="1"/>
-      <c r="CI62" s="1"/>
-      <c r="CJ62" s="1"/>
-      <c r="CK62" s="1"/>
-      <c r="CL62" s="1"/>
-      <c r="CM62" s="1"/>
+      <c r="BB62" s="15"/>
+      <c r="BC62" s="15"/>
+      <c r="BD62" s="15"/>
+      <c r="BE62" s="16"/>
+      <c r="BF62" s="15"/>
+      <c r="BG62" s="15"/>
+      <c r="BH62" s="15"/>
+      <c r="BI62" s="15"/>
+      <c r="BJ62" s="15"/>
+      <c r="BK62" s="15"/>
+      <c r="BL62" s="15"/>
+      <c r="BM62" s="15"/>
+      <c r="BN62" s="15"/>
+      <c r="BO62" s="15"/>
+      <c r="BP62" s="15"/>
+      <c r="BQ62" s="15"/>
+      <c r="BR62" s="15"/>
+      <c r="BS62" s="15"/>
+      <c r="BT62" s="15"/>
+      <c r="BU62" s="15"/>
+      <c r="BV62" s="15"/>
+      <c r="BW62" s="15"/>
+      <c r="BX62" s="15"/>
+      <c r="BY62" s="15"/>
+      <c r="BZ62" s="15"/>
+      <c r="CA62" s="15"/>
+      <c r="CB62" s="16"/>
+      <c r="CC62" s="15"/>
+      <c r="CD62" s="15"/>
+      <c r="CE62" s="15"/>
+      <c r="CF62" s="15"/>
+      <c r="CG62" s="15"/>
+      <c r="CH62" s="15"/>
+      <c r="CI62" s="15"/>
+      <c r="CJ62" s="15"/>
+      <c r="CK62" s="15"/>
+      <c r="CL62" s="15"/>
+      <c r="CM62" s="15"/>
       <c r="CN62" s="1"/>
-      <c r="CO62" s="1" t="s">
+      <c r="CO62" s="16"/>
+      <c r="CP62" s="16"/>
+      <c r="CQ62" s="16"/>
+      <c r="CR62" s="16"/>
+      <c r="CS62" s="16"/>
+      <c r="CT62" s="16"/>
+      <c r="CU62" s="16"/>
+      <c r="CV62" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP62" s="1"/>
+      <c r="CW62" s="16"/>
     </row>
-    <row r="63" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>511</v>
       </c>
@@ -10478,8 +10688,8 @@
       <c r="H63" s="1" t="s">
         <v>514</v>
       </c>
-      <c r="I63" s="29" t="s">
-        <v>265</v>
+      <c r="I63" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
@@ -10531,51 +10741,58 @@
       <c r="BA63" s="1" t="s">
         <v>510</v>
       </c>
-      <c r="BB63" s="1"/>
-      <c r="BC63" s="1"/>
-      <c r="BD63" s="1"/>
-      <c r="BE63" s="1"/>
-      <c r="BF63" s="1"/>
-      <c r="BG63" s="1"/>
-      <c r="BH63" s="1"/>
-      <c r="BI63" s="1"/>
-      <c r="BJ63" s="1"/>
-      <c r="BK63" s="1"/>
-      <c r="BL63" s="1"/>
-      <c r="BM63" s="1"/>
-      <c r="BN63" s="1"/>
-      <c r="BO63" s="1"/>
-      <c r="BP63" s="1"/>
-      <c r="BQ63" s="1"/>
-      <c r="BR63" s="1"/>
-      <c r="BS63" s="1"/>
-      <c r="BT63" s="1"/>
-      <c r="BU63" s="1"/>
-      <c r="BV63" s="1"/>
-      <c r="BW63" s="1"/>
-      <c r="BX63" s="1"/>
-      <c r="BY63" s="1"/>
-      <c r="BZ63" s="1"/>
-      <c r="CA63" s="1"/>
-      <c r="CB63" s="1"/>
-      <c r="CC63" s="1"/>
-      <c r="CD63" s="1"/>
-      <c r="CE63" s="1"/>
-      <c r="CF63" s="1"/>
-      <c r="CG63" s="1"/>
-      <c r="CH63" s="1"/>
-      <c r="CI63" s="1"/>
-      <c r="CJ63" s="1"/>
-      <c r="CK63" s="1"/>
-      <c r="CL63" s="1"/>
-      <c r="CM63" s="1"/>
+      <c r="BB63" s="15"/>
+      <c r="BC63" s="15"/>
+      <c r="BD63" s="15"/>
+      <c r="BE63" s="16"/>
+      <c r="BF63" s="15"/>
+      <c r="BG63" s="15"/>
+      <c r="BH63" s="15"/>
+      <c r="BI63" s="15"/>
+      <c r="BJ63" s="15"/>
+      <c r="BK63" s="15"/>
+      <c r="BL63" s="15"/>
+      <c r="BM63" s="15"/>
+      <c r="BN63" s="15"/>
+      <c r="BO63" s="15"/>
+      <c r="BP63" s="15"/>
+      <c r="BQ63" s="15"/>
+      <c r="BR63" s="15"/>
+      <c r="BS63" s="15"/>
+      <c r="BT63" s="15"/>
+      <c r="BU63" s="15"/>
+      <c r="BV63" s="15"/>
+      <c r="BW63" s="15"/>
+      <c r="BX63" s="15"/>
+      <c r="BY63" s="15"/>
+      <c r="BZ63" s="15"/>
+      <c r="CA63" s="15"/>
+      <c r="CB63" s="16"/>
+      <c r="CC63" s="15"/>
+      <c r="CD63" s="15"/>
+      <c r="CE63" s="15"/>
+      <c r="CF63" s="15"/>
+      <c r="CG63" s="15"/>
+      <c r="CH63" s="15"/>
+      <c r="CI63" s="15"/>
+      <c r="CJ63" s="15"/>
+      <c r="CK63" s="15"/>
+      <c r="CL63" s="15"/>
+      <c r="CM63" s="15"/>
       <c r="CN63" s="1"/>
-      <c r="CO63" s="1" t="s">
+      <c r="CO63" s="16"/>
+      <c r="CP63" s="16"/>
+      <c r="CQ63" s="16"/>
+      <c r="CR63" s="16"/>
+      <c r="CS63" s="16"/>
+      <c r="CT63" s="16"/>
+      <c r="CU63" s="16"/>
+      <c r="CV63" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP63" s="1"/>
+      <c r="CW63" s="16"/>
     </row>
-    <row r="64" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>516</v>
       </c>
@@ -10600,8 +10817,8 @@
       <c r="H64" s="1" t="s">
         <v>519</v>
       </c>
-      <c r="I64" s="29" t="s">
-        <v>265</v>
+      <c r="I64" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -10653,51 +10870,58 @@
       <c r="BA64" s="1">
         <v>28</v>
       </c>
-      <c r="BB64" s="1"/>
-      <c r="BC64" s="1"/>
-      <c r="BD64" s="1"/>
-      <c r="BE64" s="1"/>
-      <c r="BF64" s="1"/>
-      <c r="BG64" s="1"/>
-      <c r="BH64" s="1"/>
-      <c r="BI64" s="1"/>
-      <c r="BJ64" s="1"/>
-      <c r="BK64" s="1"/>
-      <c r="BL64" s="1"/>
-      <c r="BM64" s="1"/>
-      <c r="BN64" s="1"/>
-      <c r="BO64" s="1"/>
-      <c r="BP64" s="1"/>
-      <c r="BQ64" s="1"/>
-      <c r="BR64" s="1"/>
-      <c r="BS64" s="1"/>
-      <c r="BT64" s="1"/>
-      <c r="BU64" s="1"/>
-      <c r="BV64" s="1"/>
-      <c r="BW64" s="1"/>
-      <c r="BX64" s="1"/>
-      <c r="BY64" s="1"/>
-      <c r="BZ64" s="1"/>
-      <c r="CA64" s="1"/>
-      <c r="CB64" s="1"/>
-      <c r="CC64" s="1"/>
-      <c r="CD64" s="1"/>
-      <c r="CE64" s="1"/>
-      <c r="CF64" s="1"/>
-      <c r="CG64" s="1"/>
-      <c r="CH64" s="1"/>
-      <c r="CI64" s="1"/>
-      <c r="CJ64" s="1"/>
-      <c r="CK64" s="1"/>
-      <c r="CL64" s="1"/>
-      <c r="CM64" s="1"/>
+      <c r="BB64" s="15"/>
+      <c r="BC64" s="15"/>
+      <c r="BD64" s="15"/>
+      <c r="BE64" s="16"/>
+      <c r="BF64" s="15"/>
+      <c r="BG64" s="15"/>
+      <c r="BH64" s="15"/>
+      <c r="BI64" s="15"/>
+      <c r="BJ64" s="15"/>
+      <c r="BK64" s="15"/>
+      <c r="BL64" s="15"/>
+      <c r="BM64" s="15"/>
+      <c r="BN64" s="15"/>
+      <c r="BO64" s="15"/>
+      <c r="BP64" s="15"/>
+      <c r="BQ64" s="15"/>
+      <c r="BR64" s="15"/>
+      <c r="BS64" s="15"/>
+      <c r="BT64" s="15"/>
+      <c r="BU64" s="15"/>
+      <c r="BV64" s="15"/>
+      <c r="BW64" s="15"/>
+      <c r="BX64" s="15"/>
+      <c r="BY64" s="15"/>
+      <c r="BZ64" s="15"/>
+      <c r="CA64" s="15"/>
+      <c r="CB64" s="16"/>
+      <c r="CC64" s="15"/>
+      <c r="CD64" s="15"/>
+      <c r="CE64" s="15"/>
+      <c r="CF64" s="15"/>
+      <c r="CG64" s="15"/>
+      <c r="CH64" s="15"/>
+      <c r="CI64" s="15"/>
+      <c r="CJ64" s="15"/>
+      <c r="CK64" s="15"/>
+      <c r="CL64" s="15"/>
+      <c r="CM64" s="15"/>
       <c r="CN64" s="1"/>
-      <c r="CO64" s="1" t="s">
+      <c r="CO64" s="16"/>
+      <c r="CP64" s="16"/>
+      <c r="CQ64" s="16"/>
+      <c r="CR64" s="16"/>
+      <c r="CS64" s="16"/>
+      <c r="CT64" s="16"/>
+      <c r="CU64" s="16"/>
+      <c r="CV64" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP64" s="1"/>
+      <c r="CW64" s="16"/>
     </row>
-    <row r="65" spans="1:94" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>521</v>
       </c>
@@ -10722,8 +10946,8 @@
       <c r="H65" s="1" t="s">
         <v>524</v>
       </c>
-      <c r="I65" s="29" t="s">
-        <v>265</v>
+      <c r="I65" s="30" t="s">
+        <v>185</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -10775,49 +10999,56 @@
       <c r="BA65" s="1">
         <v>28</v>
       </c>
-      <c r="BB65" s="1"/>
-      <c r="BC65" s="1"/>
-      <c r="BD65" s="1"/>
-      <c r="BE65" s="1"/>
-      <c r="BF65" s="1"/>
-      <c r="BG65" s="1"/>
-      <c r="BH65" s="1"/>
-      <c r="BI65" s="1"/>
-      <c r="BJ65" s="1"/>
-      <c r="BK65" s="1"/>
-      <c r="BL65" s="1"/>
-      <c r="BM65" s="1"/>
-      <c r="BN65" s="1"/>
-      <c r="BO65" s="1"/>
-      <c r="BP65" s="1"/>
-      <c r="BQ65" s="1"/>
-      <c r="BR65" s="1"/>
-      <c r="BS65" s="1"/>
-      <c r="BT65" s="1"/>
-      <c r="BU65" s="1"/>
-      <c r="BV65" s="1"/>
-      <c r="BW65" s="1"/>
-      <c r="BX65" s="1"/>
-      <c r="BY65" s="1"/>
-      <c r="BZ65" s="1"/>
-      <c r="CA65" s="1"/>
-      <c r="CB65" s="1"/>
-      <c r="CC65" s="1"/>
-      <c r="CD65" s="1"/>
-      <c r="CE65" s="1"/>
-      <c r="CF65" s="1"/>
-      <c r="CG65" s="1"/>
-      <c r="CH65" s="1"/>
-      <c r="CI65" s="1"/>
-      <c r="CJ65" s="1"/>
-      <c r="CK65" s="1"/>
-      <c r="CL65" s="1"/>
-      <c r="CM65" s="1"/>
+      <c r="BB65" s="15"/>
+      <c r="BC65" s="15"/>
+      <c r="BD65" s="15"/>
+      <c r="BE65" s="16"/>
+      <c r="BF65" s="15"/>
+      <c r="BG65" s="15"/>
+      <c r="BH65" s="15"/>
+      <c r="BI65" s="15"/>
+      <c r="BJ65" s="15"/>
+      <c r="BK65" s="15"/>
+      <c r="BL65" s="15"/>
+      <c r="BM65" s="15"/>
+      <c r="BN65" s="15"/>
+      <c r="BO65" s="15"/>
+      <c r="BP65" s="15"/>
+      <c r="BQ65" s="15"/>
+      <c r="BR65" s="15"/>
+      <c r="BS65" s="15"/>
+      <c r="BT65" s="15"/>
+      <c r="BU65" s="15"/>
+      <c r="BV65" s="15"/>
+      <c r="BW65" s="15"/>
+      <c r="BX65" s="15"/>
+      <c r="BY65" s="15"/>
+      <c r="BZ65" s="15"/>
+      <c r="CA65" s="15"/>
+      <c r="CB65" s="16"/>
+      <c r="CC65" s="15"/>
+      <c r="CD65" s="15"/>
+      <c r="CE65" s="15"/>
+      <c r="CF65" s="15"/>
+      <c r="CG65" s="15"/>
+      <c r="CH65" s="15"/>
+      <c r="CI65" s="15"/>
+      <c r="CJ65" s="15"/>
+      <c r="CK65" s="15"/>
+      <c r="CL65" s="15"/>
+      <c r="CM65" s="15"/>
       <c r="CN65" s="1"/>
-      <c r="CO65" s="1" t="s">
+      <c r="CO65" s="16"/>
+      <c r="CP65" s="16"/>
+      <c r="CQ65" s="16"/>
+      <c r="CR65" s="16"/>
+      <c r="CS65" s="16"/>
+      <c r="CT65" s="16"/>
+      <c r="CU65" s="16"/>
+      <c r="CV65" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="CP65" s="1"/>
+      <c r="CW65" s="16"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
Salesforce DP added and updated logo changes on login page
</commit_message>
<xml_diff>
--- a/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
+++ b/Engage/Sogo-Smoke/src/main/resources/excelfiles/Sogo_Smoke.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0746D836-64ED-4C54-BE30-ED52E37582C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCBCDE2-C01B-402F-966F-646BF89813D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1275" uniqueCount="572">
   <si>
     <t>Environment</t>
   </si>
@@ -1815,13 +1815,67 @@
   <si>
     <t>PASS</t>
   </si>
+  <si>
+    <t>Smoke_TC101</t>
+  </si>
+  <si>
+    <t>USER9</t>
+  </si>
+  <si>
+    <t>RMSFandD</t>
+  </si>
+  <si>
+    <t>sogo_nayan_ent</t>
+  </si>
+  <si>
+    <t>Maxrunner@1234</t>
+  </si>
+  <si>
+    <t>salesforceFields</t>
+  </si>
+  <si>
+    <t>Contact ID,Account ID,Full Name,Mobile Phone,Email</t>
+  </si>
+  <si>
+    <t>Email,Id,AccountId,Name,MobilePhone</t>
+  </si>
+  <si>
+    <t>Smoke_TC102</t>
+  </si>
+  <si>
+    <t>Lead ID,Full Name,Mobile Phone,Email</t>
+  </si>
+  <si>
+    <t>Email,Id,Name,MobilePhone</t>
+  </si>
+  <si>
+    <t>Smoke_TC103</t>
+  </si>
+  <si>
+    <t>Account ID,Account Name,Account Phone,Email</t>
+  </si>
+  <si>
+    <t>Id,Name,Phone,Email__c</t>
+  </si>
+  <si>
+    <t>Create contact list via salesforce by using Contact object</t>
+  </si>
+  <si>
+    <t>Create contact list via salesforce by using Lead object</t>
+  </si>
+  <si>
+    <t>Create contact list via salesforce by using Account object</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="10">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1873,6 +1927,41 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color indexed="8"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <u val="single"/>
+      <color indexed="12"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -1884,7 +1973,7 @@
       <color indexed="12"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1926,6 +2015,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="17"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="13"/>
       </patternFill>
     </fill>
     <fill>
@@ -2034,7 +2183,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -2085,10 +2234,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" xfId="0" applyFill="true" applyFont="true"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2466,10 +2629,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2620,6 +2783,20 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>557</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>558</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
@@ -2628,6 +2805,7 @@
     <hyperlink ref="C8" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
     <hyperlink ref="C9" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
     <hyperlink ref="C10" r:id="rId5" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="C11" r:id="rId6" xr:uid="{E92E2B5B-B269-498D-B490-AE6E9447F3EE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2636,10 +2814,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:DB68"/>
+  <dimension ref="A1:DC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2664,7 +2842,7 @@
     <col min="18" max="18" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:106">
+    <row r="1" spans="1:107">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -2981,10 +3159,13 @@
         <v>540</v>
       </c>
       <c r="DB1" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="DC1" s="9" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="2" spans="1:106">
+    <row r="2" spans="1:107">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -3007,7 +3188,7 @@
       <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J2" s="4"/>
@@ -3107,10 +3288,11 @@
       <c r="CX2" s="1"/>
       <c r="CY2" s="1"/>
       <c r="CZ2" s="1"/>
-      <c r="DA2" s="1"/>
-      <c r="DB2" s="1"/>
+      <c r="DA2" s="47"/>
+      <c r="DB2" s="47"/>
+      <c r="DC2" s="1"/>
     </row>
-    <row r="3" spans="1:106">
+    <row r="3" spans="1:107">
       <c r="A3" s="1" t="s">
         <v>27</v>
       </c>
@@ -3133,7 +3315,7 @@
       <c r="H3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="48" t="s">
+      <c r="I3" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J3" s="14"/>
@@ -3311,10 +3493,11 @@
       <c r="CX3" s="1"/>
       <c r="CY3" s="1"/>
       <c r="CZ3" s="1"/>
-      <c r="DA3" s="1"/>
-      <c r="DB3" s="1"/>
+      <c r="DA3" s="47"/>
+      <c r="DB3" s="47"/>
+      <c r="DC3" s="1"/>
     </row>
-    <row r="4" spans="1:106">
+    <row r="4" spans="1:107">
       <c r="A4" s="1" t="s">
         <v>178</v>
       </c>
@@ -3337,7 +3520,7 @@
       <c r="H4" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I4" s="48" t="s">
+      <c r="I4" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J4" s="14"/>
@@ -3449,10 +3632,11 @@
       <c r="CX4" s="1"/>
       <c r="CY4" s="1"/>
       <c r="CZ4" s="1"/>
-      <c r="DA4" s="1"/>
-      <c r="DB4" s="1"/>
+      <c r="DA4" s="47"/>
+      <c r="DB4" s="47"/>
+      <c r="DC4" s="1"/>
     </row>
-    <row r="5" spans="1:106">
+    <row r="5" spans="1:107">
       <c r="A5" s="1" t="s">
         <v>179</v>
       </c>
@@ -3475,7 +3659,7 @@
       <c r="H5" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I5" s="48" t="s">
+      <c r="I5" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J5" s="14" t="s">
@@ -3589,10 +3773,11 @@
       <c r="CX5" s="1"/>
       <c r="CY5" s="1"/>
       <c r="CZ5" s="1"/>
-      <c r="DA5" s="1"/>
-      <c r="DB5" s="1"/>
+      <c r="DA5" s="47"/>
+      <c r="DB5" s="47"/>
+      <c r="DC5" s="1"/>
     </row>
-    <row r="6" spans="1:106">
+    <row r="6" spans="1:107">
       <c r="A6" s="1" t="s">
         <v>180</v>
       </c>
@@ -3615,7 +3800,7 @@
       <c r="H6" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I6" s="48" t="s">
+      <c r="I6" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J6" s="14" t="s">
@@ -3719,10 +3904,11 @@
       <c r="CX6" s="1"/>
       <c r="CY6" s="1"/>
       <c r="CZ6" s="1"/>
-      <c r="DA6" s="1"/>
-      <c r="DB6" s="1"/>
+      <c r="DA6" s="47"/>
+      <c r="DB6" s="47"/>
+      <c r="DC6" s="1"/>
     </row>
-    <row r="7" spans="1:106">
+    <row r="7" spans="1:107">
       <c r="A7" s="1" t="s">
         <v>181</v>
       </c>
@@ -3745,7 +3931,7 @@
       <c r="H7" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="I7" s="48" t="s">
+      <c r="I7" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J7" s="14"/>
@@ -3849,10 +4035,11 @@
       <c r="CX7" s="1"/>
       <c r="CY7" s="1"/>
       <c r="CZ7" s="1"/>
-      <c r="DA7" s="1"/>
-      <c r="DB7" s="1"/>
+      <c r="DA7" s="47"/>
+      <c r="DB7" s="47"/>
+      <c r="DC7" s="1"/>
     </row>
-    <row r="8" spans="1:106">
+    <row r="8" spans="1:107">
       <c r="A8" s="1" t="s">
         <v>182</v>
       </c>
@@ -3875,7 +4062,7 @@
       <c r="H8" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="I8" s="48" t="s">
+      <c r="I8" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J8" s="17" t="s">
@@ -3981,10 +4168,11 @@
       <c r="CX8" s="1"/>
       <c r="CY8" s="1"/>
       <c r="CZ8" s="1"/>
-      <c r="DA8" s="1"/>
-      <c r="DB8" s="1"/>
+      <c r="DA8" s="47"/>
+      <c r="DB8" s="47"/>
+      <c r="DC8" s="1"/>
     </row>
-    <row r="9" spans="1:106">
+    <row r="9" spans="1:107">
       <c r="A9" s="1" t="s">
         <v>157</v>
       </c>
@@ -4007,7 +4195,7 @@
       <c r="H9" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="I9" s="48" t="s">
+      <c r="I9" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J9" s="1"/>
@@ -4117,10 +4305,11 @@
       <c r="CX9" s="1"/>
       <c r="CY9" s="1"/>
       <c r="CZ9" s="1"/>
-      <c r="DA9" s="1"/>
-      <c r="DB9" s="1"/>
+      <c r="DA9" s="47"/>
+      <c r="DB9" s="47"/>
+      <c r="DC9" s="1"/>
     </row>
-    <row r="10" spans="1:106">
+    <row r="10" spans="1:107">
       <c r="A10" s="1" t="s">
         <v>214</v>
       </c>
@@ -4143,7 +4332,7 @@
         <v>187</v>
       </c>
       <c r="H10" s="20"/>
-      <c r="I10" s="48" t="s">
+      <c r="I10" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J10" s="21" t="s">
@@ -4255,10 +4444,11 @@
       <c r="CX10" s="1"/>
       <c r="CY10" s="1"/>
       <c r="CZ10" s="1"/>
-      <c r="DA10" s="1"/>
-      <c r="DB10" s="1"/>
+      <c r="DA10" s="47"/>
+      <c r="DB10" s="47"/>
+      <c r="DC10" s="1"/>
     </row>
-    <row r="11" spans="1:106">
+    <row r="11" spans="1:107">
       <c r="A11" s="1" t="s">
         <v>215</v>
       </c>
@@ -4281,7 +4471,7 @@
         <v>192</v>
       </c>
       <c r="H11" s="20"/>
-      <c r="I11" s="48" t="s">
+      <c r="I11" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J11" s="21" t="s">
@@ -4389,10 +4579,11 @@
       <c r="CX11" s="1"/>
       <c r="CY11" s="1"/>
       <c r="CZ11" s="1"/>
-      <c r="DA11" s="1"/>
-      <c r="DB11" s="1"/>
+      <c r="DA11" s="47"/>
+      <c r="DB11" s="47"/>
+      <c r="DC11" s="1"/>
     </row>
-    <row r="12" spans="1:106">
+    <row r="12" spans="1:107">
       <c r="A12" s="1" t="s">
         <v>216</v>
       </c>
@@ -4415,7 +4606,7 @@
         <v>195</v>
       </c>
       <c r="H12" s="20"/>
-      <c r="I12" s="48" t="s">
+      <c r="I12" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J12" s="21"/>
@@ -4521,10 +4712,11 @@
       <c r="CX12" s="1"/>
       <c r="CY12" s="1"/>
       <c r="CZ12" s="1"/>
-      <c r="DA12" s="1"/>
-      <c r="DB12" s="1"/>
+      <c r="DA12" s="47"/>
+      <c r="DB12" s="47"/>
+      <c r="DC12" s="1"/>
     </row>
-    <row r="13" spans="1:106">
+    <row r="13" spans="1:107">
       <c r="A13" s="1" t="s">
         <v>217</v>
       </c>
@@ -4547,7 +4739,7 @@
         <v>198</v>
       </c>
       <c r="H13" s="20"/>
-      <c r="I13" s="48" t="s">
+      <c r="I13" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J13" s="21"/>
@@ -4653,10 +4845,11 @@
       <c r="CX13" s="1"/>
       <c r="CY13" s="1"/>
       <c r="CZ13" s="1"/>
-      <c r="DA13" s="1"/>
-      <c r="DB13" s="1"/>
+      <c r="DA13" s="47"/>
+      <c r="DB13" s="47"/>
+      <c r="DC13" s="1"/>
     </row>
-    <row r="14" spans="1:106">
+    <row r="14" spans="1:107">
       <c r="A14" s="1" t="s">
         <v>218</v>
       </c>
@@ -4679,7 +4872,7 @@
         <v>201</v>
       </c>
       <c r="H14" s="20"/>
-      <c r="I14" s="48" t="s">
+      <c r="I14" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J14" s="21"/>
@@ -4785,10 +4978,11 @@
       <c r="CX14" s="1"/>
       <c r="CY14" s="1"/>
       <c r="CZ14" s="1"/>
-      <c r="DA14" s="1"/>
-      <c r="DB14" s="1"/>
+      <c r="DA14" s="47"/>
+      <c r="DB14" s="47"/>
+      <c r="DC14" s="1"/>
     </row>
-    <row r="15" spans="1:106">
+    <row r="15" spans="1:107">
       <c r="A15" s="1" t="s">
         <v>219</v>
       </c>
@@ -4811,7 +5005,7 @@
         <v>204</v>
       </c>
       <c r="H15" s="20"/>
-      <c r="I15" s="48" t="s">
+      <c r="I15" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J15" s="21" t="s">
@@ -4937,10 +5131,11 @@
       <c r="CX15" s="1"/>
       <c r="CY15" s="1"/>
       <c r="CZ15" s="1"/>
-      <c r="DA15" s="1"/>
-      <c r="DB15" s="1"/>
+      <c r="DA15" s="47"/>
+      <c r="DB15" s="47"/>
+      <c r="DC15" s="1"/>
     </row>
-    <row r="16" spans="1:106">
+    <row r="16" spans="1:107">
       <c r="A16" s="1" t="s">
         <v>223</v>
       </c>
@@ -4963,7 +5158,7 @@
         <v>225</v>
       </c>
       <c r="H16" s="20"/>
-      <c r="I16" s="48" t="s">
+      <c r="I16" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J16" s="21"/>
@@ -5084,10 +5279,11 @@
       <c r="CX16" s="1"/>
       <c r="CY16" s="1"/>
       <c r="CZ16" s="1"/>
-      <c r="DA16" s="1"/>
-      <c r="DB16" s="1"/>
+      <c r="DA16" s="47"/>
+      <c r="DB16" s="47"/>
+      <c r="DC16" s="1"/>
     </row>
-    <row r="17" spans="1:106">
+    <row r="17" spans="1:107">
       <c r="A17" s="1" t="s">
         <v>235</v>
       </c>
@@ -5110,7 +5306,7 @@
       <c r="H17" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I17" s="48" t="s">
+      <c r="I17" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J17" s="14"/>
@@ -5212,10 +5408,11 @@
       <c r="CX17" s="1"/>
       <c r="CY17" s="1"/>
       <c r="CZ17" s="1"/>
-      <c r="DA17" s="1"/>
-      <c r="DB17" s="1"/>
+      <c r="DA17" s="47"/>
+      <c r="DB17" s="47"/>
+      <c r="DC17" s="1"/>
     </row>
-    <row r="18" spans="1:106">
+    <row r="18" spans="1:107">
       <c r="A18" s="1" t="s">
         <v>240</v>
       </c>
@@ -5236,7 +5433,7 @@
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
-      <c r="I18" s="48" t="s">
+      <c r="I18" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J18" s="14" t="s">
@@ -5342,10 +5539,11 @@
       <c r="CX18" s="1"/>
       <c r="CY18" s="1"/>
       <c r="CZ18" s="1"/>
-      <c r="DA18" s="1"/>
-      <c r="DB18" s="1"/>
+      <c r="DA18" s="47"/>
+      <c r="DB18" s="47"/>
+      <c r="DC18" s="1"/>
     </row>
-    <row r="19" spans="1:106">
+    <row r="19" spans="1:107">
       <c r="A19" s="1" t="s">
         <v>247</v>
       </c>
@@ -5366,7 +5564,7 @@
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
-      <c r="I19" s="48" t="s">
+      <c r="I19" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J19" s="14"/>
@@ -5470,10 +5668,11 @@
       <c r="CX19" s="1"/>
       <c r="CY19" s="1"/>
       <c r="CZ19" s="1"/>
-      <c r="DA19" s="1"/>
-      <c r="DB19" s="1"/>
+      <c r="DA19" s="47"/>
+      <c r="DB19" s="47"/>
+      <c r="DC19" s="1"/>
     </row>
-    <row r="20" spans="1:106">
+    <row r="20" spans="1:107">
       <c r="A20" s="1" t="s">
         <v>276</v>
       </c>
@@ -5494,7 +5693,7 @@
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
-      <c r="I20" s="48" t="s">
+      <c r="I20" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J20" s="14"/>
@@ -5602,10 +5801,11 @@
       <c r="CX20" s="1"/>
       <c r="CY20" s="1"/>
       <c r="CZ20" s="1"/>
-      <c r="DA20" s="1"/>
-      <c r="DB20" s="1"/>
+      <c r="DA20" s="47"/>
+      <c r="DB20" s="47"/>
+      <c r="DC20" s="1"/>
     </row>
-    <row r="21" spans="1:106">
+    <row r="21" spans="1:107">
       <c r="A21" s="1" t="s">
         <v>277</v>
       </c>
@@ -5630,7 +5830,7 @@
       <c r="H21" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="I21" s="48" t="s">
+      <c r="I21" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J21" s="14"/>
@@ -5738,10 +5938,11 @@
       <c r="CX21" s="1"/>
       <c r="CY21" s="1"/>
       <c r="CZ21" s="1"/>
-      <c r="DA21" s="1"/>
-      <c r="DB21" s="1"/>
+      <c r="DA21" s="47"/>
+      <c r="DB21" s="47"/>
+      <c r="DC21" s="1"/>
     </row>
-    <row r="22" spans="1:106">
+    <row r="22" spans="1:107">
       <c r="A22" s="1" t="s">
         <v>278</v>
       </c>
@@ -5766,7 +5967,7 @@
       <c r="H22" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I22" s="48" t="s">
+      <c r="I22" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J22" s="14"/>
@@ -5870,10 +6071,11 @@
       <c r="CX22" s="1"/>
       <c r="CY22" s="1"/>
       <c r="CZ22" s="1"/>
-      <c r="DA22" s="1"/>
-      <c r="DB22" s="1"/>
+      <c r="DA22" s="47"/>
+      <c r="DB22" s="47"/>
+      <c r="DC22" s="1"/>
     </row>
-    <row r="23" spans="1:106">
+    <row r="23" spans="1:107">
       <c r="A23" s="1" t="s">
         <v>279</v>
       </c>
@@ -5898,7 +6100,7 @@
       <c r="H23" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="I23" s="48" t="s">
+      <c r="I23" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J23" s="14"/>
@@ -6006,10 +6208,11 @@
       <c r="CX23" s="1"/>
       <c r="CY23" s="1"/>
       <c r="CZ23" s="1"/>
-      <c r="DA23" s="1"/>
-      <c r="DB23" s="1"/>
+      <c r="DA23" s="47"/>
+      <c r="DB23" s="47"/>
+      <c r="DC23" s="1"/>
     </row>
-    <row r="24" spans="1:106">
+    <row r="24" spans="1:107">
       <c r="A24" s="1" t="s">
         <v>280</v>
       </c>
@@ -6034,7 +6237,7 @@
       <c r="H24" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="I24" s="48" t="s">
+      <c r="I24" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J24" s="14"/>
@@ -6140,10 +6343,11 @@
       <c r="CX24" s="1"/>
       <c r="CY24" s="1"/>
       <c r="CZ24" s="1"/>
-      <c r="DA24" s="1"/>
-      <c r="DB24" s="1"/>
+      <c r="DA24" s="47"/>
+      <c r="DB24" s="47"/>
+      <c r="DC24" s="1"/>
     </row>
-    <row r="25" spans="1:106">
+    <row r="25" spans="1:107">
       <c r="A25" s="1" t="s">
         <v>281</v>
       </c>
@@ -6168,7 +6372,7 @@
       <c r="H25" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I25" s="48" t="s">
+      <c r="I25" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J25" s="14"/>
@@ -6274,10 +6478,11 @@
       <c r="CX25" s="1"/>
       <c r="CY25" s="1"/>
       <c r="CZ25" s="1"/>
-      <c r="DA25" s="1"/>
-      <c r="DB25" s="1"/>
+      <c r="DA25" s="47"/>
+      <c r="DB25" s="47"/>
+      <c r="DC25" s="1"/>
     </row>
-    <row r="26" spans="1:106">
+    <row r="26" spans="1:107">
       <c r="A26" s="1" t="s">
         <v>282</v>
       </c>
@@ -6302,7 +6507,7 @@
       <c r="H26" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I26" s="48" t="s">
+      <c r="I26" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J26" s="14"/>
@@ -6408,10 +6613,11 @@
       <c r="CX26" s="1"/>
       <c r="CY26" s="1"/>
       <c r="CZ26" s="1"/>
-      <c r="DA26" s="1"/>
-      <c r="DB26" s="1"/>
+      <c r="DA26" s="47"/>
+      <c r="DB26" s="47"/>
+      <c r="DC26" s="1"/>
     </row>
-    <row r="27" spans="1:106">
+    <row r="27" spans="1:107">
       <c r="A27" s="1" t="s">
         <v>283</v>
       </c>
@@ -6436,7 +6642,7 @@
       <c r="H27" s="1" t="s">
         <v>314</v>
       </c>
-      <c r="I27" s="48" t="s">
+      <c r="I27" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J27" s="14"/>
@@ -6540,10 +6746,11 @@
       <c r="CX27" s="1"/>
       <c r="CY27" s="1"/>
       <c r="CZ27" s="1"/>
-      <c r="DA27" s="1"/>
-      <c r="DB27" s="1"/>
+      <c r="DA27" s="47"/>
+      <c r="DB27" s="47"/>
+      <c r="DC27" s="1"/>
     </row>
-    <row r="28" spans="1:106">
+    <row r="28" spans="1:107">
       <c r="A28" s="1" t="s">
         <v>284</v>
       </c>
@@ -6568,7 +6775,7 @@
       <c r="H28" s="1" t="s">
         <v>316</v>
       </c>
-      <c r="I28" s="48" t="s">
+      <c r="I28" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J28" s="14"/>
@@ -6672,10 +6879,11 @@
       <c r="CX28" s="1"/>
       <c r="CY28" s="1"/>
       <c r="CZ28" s="1"/>
-      <c r="DA28" s="1"/>
-      <c r="DB28" s="1"/>
+      <c r="DA28" s="47"/>
+      <c r="DB28" s="47"/>
+      <c r="DC28" s="1"/>
     </row>
-    <row r="29" spans="1:106">
+    <row r="29" spans="1:107">
       <c r="A29" s="1" t="s">
         <v>285</v>
       </c>
@@ -6700,7 +6908,7 @@
       <c r="H29" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J29" s="14"/>
@@ -6806,10 +7014,11 @@
       <c r="CX29" s="1"/>
       <c r="CY29" s="1"/>
       <c r="CZ29" s="1"/>
-      <c r="DA29" s="1"/>
-      <c r="DB29" s="1"/>
+      <c r="DA29" s="47"/>
+      <c r="DB29" s="47"/>
+      <c r="DC29" s="1"/>
     </row>
-    <row r="30" spans="1:106">
+    <row r="30" spans="1:107">
       <c r="A30" s="1" t="s">
         <v>286</v>
       </c>
@@ -6834,7 +7043,7 @@
       <c r="H30" s="1" t="s">
         <v>319</v>
       </c>
-      <c r="I30" s="48" t="s">
+      <c r="I30" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J30" s="14"/>
@@ -6942,10 +7151,11 @@
       <c r="CX30" s="1"/>
       <c r="CY30" s="1"/>
       <c r="CZ30" s="1"/>
-      <c r="DA30" s="1"/>
-      <c r="DB30" s="1"/>
+      <c r="DA30" s="47"/>
+      <c r="DB30" s="47"/>
+      <c r="DC30" s="1"/>
     </row>
-    <row r="31" spans="1:106">
+    <row r="31" spans="1:107">
       <c r="A31" s="1" t="s">
         <v>287</v>
       </c>
@@ -6970,7 +7180,7 @@
       <c r="H31" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="I31" s="48" t="s">
+      <c r="I31" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J31" s="14"/>
@@ -7078,10 +7288,11 @@
       <c r="CX31" s="1"/>
       <c r="CY31" s="1"/>
       <c r="CZ31" s="1"/>
-      <c r="DA31" s="1"/>
-      <c r="DB31" s="1"/>
+      <c r="DA31" s="47"/>
+      <c r="DB31" s="47"/>
+      <c r="DC31" s="1"/>
     </row>
-    <row r="32" spans="1:106">
+    <row r="32" spans="1:107">
       <c r="A32" s="11" t="s">
         <v>288</v>
       </c>
@@ -7106,7 +7317,7 @@
       <c r="H32" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="I32" s="48" t="s">
+      <c r="I32" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J32" s="17"/>
@@ -7210,10 +7421,11 @@
       <c r="CX32" s="1"/>
       <c r="CY32" s="1"/>
       <c r="CZ32" s="1"/>
-      <c r="DA32" s="1"/>
-      <c r="DB32" s="1"/>
+      <c r="DA32" s="47"/>
+      <c r="DB32" s="47"/>
+      <c r="DC32" s="1"/>
     </row>
-    <row r="33" spans="1:106">
+    <row r="33" spans="1:107">
       <c r="A33" s="1" t="s">
         <v>524</v>
       </c>
@@ -7236,7 +7448,7 @@
         <v>526</v>
       </c>
       <c r="H33" s="1"/>
-      <c r="I33" s="48" t="s">
+      <c r="I33" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J33" s="1"/>
@@ -7334,15 +7546,16 @@
       <c r="CX33" s="1"/>
       <c r="CY33" s="1"/>
       <c r="CZ33" s="1"/>
-      <c r="DA33" s="1"/>
-      <c r="DB33" s="1"/>
+      <c r="DA33" s="47"/>
+      <c r="DB33" s="47"/>
+      <c r="DC33" s="1"/>
     </row>
-    <row r="34" spans="1:106">
+    <row r="34" spans="1:107">
       <c r="A34" s="31" t="s">
         <v>275</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>258</v>
@@ -7358,8 +7571,8 @@
       </c>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
-      <c r="I34" s="46" t="s">
-        <v>553</v>
+      <c r="I34" s="62" t="s">
+        <v>183</v>
       </c>
       <c r="J34" s="32" t="s">
         <v>274</v>
@@ -7496,10 +7709,11 @@
       <c r="CX34" s="1"/>
       <c r="CY34" s="1"/>
       <c r="CZ34" s="1"/>
-      <c r="DA34" s="1"/>
-      <c r="DB34" s="1"/>
+      <c r="DA34" s="47"/>
+      <c r="DB34" s="47"/>
+      <c r="DC34" s="1"/>
     </row>
-    <row r="35" spans="1:106" ht="20.25" customHeight="1">
+    <row r="35" spans="1:107" ht="20.25" customHeight="1">
       <c r="A35" s="1" t="s">
         <v>365</v>
       </c>
@@ -7524,7 +7738,7 @@
       <c r="H35" s="1" t="s">
         <v>368</v>
       </c>
-      <c r="I35" s="48" t="s">
+      <c r="I35" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J35" s="1"/>
@@ -7632,10 +7846,11 @@
       <c r="CX35" s="1"/>
       <c r="CY35" s="1"/>
       <c r="CZ35" s="1"/>
-      <c r="DA35" s="1"/>
-      <c r="DB35" s="1"/>
+      <c r="DA35" s="47"/>
+      <c r="DB35" s="47"/>
+      <c r="DC35" s="1"/>
     </row>
-    <row r="36" spans="1:106" ht="19.5" customHeight="1">
+    <row r="36" spans="1:107" ht="19.5" customHeight="1">
       <c r="A36" s="1" t="s">
         <v>373</v>
       </c>
@@ -7660,7 +7875,7 @@
       <c r="H36" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="I36" s="48" t="s">
+      <c r="I36" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J36" s="1"/>
@@ -7768,10 +7983,11 @@
       <c r="CX36" s="1"/>
       <c r="CY36" s="1"/>
       <c r="CZ36" s="1"/>
-      <c r="DA36" s="1"/>
-      <c r="DB36" s="1"/>
+      <c r="DA36" s="47"/>
+      <c r="DB36" s="47"/>
+      <c r="DC36" s="1"/>
     </row>
-    <row r="37" spans="1:106">
+    <row r="37" spans="1:107">
       <c r="A37" s="1" t="s">
         <v>380</v>
       </c>
@@ -7796,7 +8012,7 @@
       <c r="H37" s="30" t="s">
         <v>383</v>
       </c>
-      <c r="I37" s="48" t="s">
+      <c r="I37" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J37" s="1"/>
@@ -7900,10 +8116,11 @@
       <c r="CX37" s="1"/>
       <c r="CY37" s="1"/>
       <c r="CZ37" s="1"/>
-      <c r="DA37" s="1"/>
-      <c r="DB37" s="1"/>
+      <c r="DA37" s="47"/>
+      <c r="DB37" s="47"/>
+      <c r="DC37" s="1"/>
     </row>
-    <row r="38" spans="1:106">
+    <row r="38" spans="1:107">
       <c r="A38" s="1" t="s">
         <v>385</v>
       </c>
@@ -7928,7 +8145,7 @@
       <c r="H38" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="I38" s="48" t="s">
+      <c r="I38" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J38" s="1"/>
@@ -8032,10 +8249,11 @@
       <c r="CX38" s="1"/>
       <c r="CY38" s="1"/>
       <c r="CZ38" s="1"/>
-      <c r="DA38" s="1"/>
-      <c r="DB38" s="1"/>
+      <c r="DA38" s="47"/>
+      <c r="DB38" s="47"/>
+      <c r="DC38" s="1"/>
     </row>
-    <row r="39" spans="1:106">
+    <row r="39" spans="1:107">
       <c r="A39" s="1" t="s">
         <v>390</v>
       </c>
@@ -8060,7 +8278,7 @@
       <c r="H39" s="1" t="s">
         <v>393</v>
       </c>
-      <c r="I39" s="48" t="s">
+      <c r="I39" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J39" s="1"/>
@@ -8164,10 +8382,11 @@
       <c r="CX39" s="1"/>
       <c r="CY39" s="1"/>
       <c r="CZ39" s="1"/>
-      <c r="DA39" s="1"/>
-      <c r="DB39" s="1"/>
+      <c r="DA39" s="47"/>
+      <c r="DB39" s="47"/>
+      <c r="DC39" s="1"/>
     </row>
-    <row r="40" spans="1:106">
+    <row r="40" spans="1:107">
       <c r="A40" s="1" t="s">
         <v>395</v>
       </c>
@@ -8192,7 +8411,7 @@
       <c r="H40" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="I40" s="48" t="s">
+      <c r="I40" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J40" s="1"/>
@@ -8296,10 +8515,11 @@
       <c r="CX40" s="1"/>
       <c r="CY40" s="1"/>
       <c r="CZ40" s="1"/>
-      <c r="DA40" s="1"/>
-      <c r="DB40" s="1"/>
+      <c r="DA40" s="47"/>
+      <c r="DB40" s="47"/>
+      <c r="DC40" s="1"/>
     </row>
-    <row r="41" spans="1:106">
+    <row r="41" spans="1:107">
       <c r="A41" s="1" t="s">
         <v>400</v>
       </c>
@@ -8324,7 +8544,7 @@
       <c r="H41" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="I41" s="48" t="s">
+      <c r="I41" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J41" s="1"/>
@@ -8428,10 +8648,11 @@
       <c r="CX41" s="1"/>
       <c r="CY41" s="1"/>
       <c r="CZ41" s="1"/>
-      <c r="DA41" s="1"/>
-      <c r="DB41" s="1"/>
+      <c r="DA41" s="47"/>
+      <c r="DB41" s="47"/>
+      <c r="DC41" s="1"/>
     </row>
-    <row r="42" spans="1:106">
+    <row r="42" spans="1:107">
       <c r="A42" s="1" t="s">
         <v>405</v>
       </c>
@@ -8456,7 +8677,7 @@
       <c r="H42" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="I42" s="48" t="s">
+      <c r="I42" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J42" s="1"/>
@@ -8560,10 +8781,11 @@
       <c r="CX42" s="1"/>
       <c r="CY42" s="1"/>
       <c r="CZ42" s="1"/>
-      <c r="DA42" s="1"/>
-      <c r="DB42" s="1"/>
+      <c r="DA42" s="47"/>
+      <c r="DB42" s="47"/>
+      <c r="DC42" s="1"/>
     </row>
-    <row r="43" spans="1:106">
+    <row r="43" spans="1:107">
       <c r="A43" s="1" t="s">
         <v>410</v>
       </c>
@@ -8588,7 +8810,7 @@
       <c r="H43" s="1" t="s">
         <v>413</v>
       </c>
-      <c r="I43" s="48" t="s">
+      <c r="I43" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J43" s="1"/>
@@ -8692,10 +8914,11 @@
       <c r="CX43" s="1"/>
       <c r="CY43" s="1"/>
       <c r="CZ43" s="1"/>
-      <c r="DA43" s="1"/>
-      <c r="DB43" s="1"/>
+      <c r="DA43" s="47"/>
+      <c r="DB43" s="47"/>
+      <c r="DC43" s="1"/>
     </row>
-    <row r="44" spans="1:106">
+    <row r="44" spans="1:107">
       <c r="A44" s="1" t="s">
         <v>415</v>
       </c>
@@ -8720,7 +8943,7 @@
       <c r="H44" s="1" t="s">
         <v>418</v>
       </c>
-      <c r="I44" s="48" t="s">
+      <c r="I44" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J44" s="1"/>
@@ -8824,10 +9047,11 @@
       <c r="CX44" s="1"/>
       <c r="CY44" s="1"/>
       <c r="CZ44" s="1"/>
-      <c r="DA44" s="1"/>
-      <c r="DB44" s="1"/>
+      <c r="DA44" s="47"/>
+      <c r="DB44" s="47"/>
+      <c r="DC44" s="1"/>
     </row>
-    <row r="45" spans="1:106">
+    <row r="45" spans="1:107">
       <c r="A45" s="1" t="s">
         <v>420</v>
       </c>
@@ -8850,7 +9074,7 @@
         <v>422</v>
       </c>
       <c r="H45" s="1"/>
-      <c r="I45" s="48" t="s">
+      <c r="I45" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J45" s="1"/>
@@ -8954,10 +9178,11 @@
       <c r="CX45" s="1"/>
       <c r="CY45" s="1"/>
       <c r="CZ45" s="1"/>
-      <c r="DA45" s="1"/>
-      <c r="DB45" s="1"/>
+      <c r="DA45" s="47"/>
+      <c r="DB45" s="47"/>
+      <c r="DC45" s="1"/>
     </row>
-    <row r="46" spans="1:106">
+    <row r="46" spans="1:107">
       <c r="A46" s="1" t="s">
         <v>424</v>
       </c>
@@ -8980,7 +9205,7 @@
         <v>426</v>
       </c>
       <c r="H46" s="1"/>
-      <c r="I46" s="48" t="s">
+      <c r="I46" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J46" s="1"/>
@@ -9084,10 +9309,11 @@
       <c r="CX46" s="1"/>
       <c r="CY46" s="1"/>
       <c r="CZ46" s="1"/>
-      <c r="DA46" s="1"/>
-      <c r="DB46" s="1"/>
+      <c r="DA46" s="47"/>
+      <c r="DB46" s="47"/>
+      <c r="DC46" s="1"/>
     </row>
-    <row r="47" spans="1:106">
+    <row r="47" spans="1:107">
       <c r="A47" s="1" t="s">
         <v>428</v>
       </c>
@@ -9110,7 +9336,7 @@
         <v>430</v>
       </c>
       <c r="H47" s="1"/>
-      <c r="I47" s="48" t="s">
+      <c r="I47" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J47" s="1"/>
@@ -9214,10 +9440,11 @@
       <c r="CX47" s="1"/>
       <c r="CY47" s="1"/>
       <c r="CZ47" s="1"/>
-      <c r="DA47" s="1"/>
-      <c r="DB47" s="1"/>
+      <c r="DA47" s="47"/>
+      <c r="DB47" s="47"/>
+      <c r="DC47" s="1"/>
     </row>
-    <row r="48" spans="1:106">
+    <row r="48" spans="1:107">
       <c r="A48" s="1" t="s">
         <v>432</v>
       </c>
@@ -9240,7 +9467,7 @@
         <v>434</v>
       </c>
       <c r="H48" s="1"/>
-      <c r="I48" s="48" t="s">
+      <c r="I48" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J48" s="1"/>
@@ -9344,10 +9571,11 @@
       <c r="CX48" s="1"/>
       <c r="CY48" s="1"/>
       <c r="CZ48" s="1"/>
-      <c r="DA48" s="1"/>
-      <c r="DB48" s="1"/>
+      <c r="DA48" s="47"/>
+      <c r="DB48" s="47"/>
+      <c r="DC48" s="1"/>
     </row>
-    <row r="49" spans="1:106">
+    <row r="49" spans="1:107">
       <c r="A49" s="1" t="s">
         <v>436</v>
       </c>
@@ -9372,7 +9600,7 @@
       <c r="H49" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="I49" s="48" t="s">
+      <c r="I49" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J49" s="1"/>
@@ -9476,10 +9704,11 @@
       <c r="CX49" s="1"/>
       <c r="CY49" s="1"/>
       <c r="CZ49" s="1"/>
-      <c r="DA49" s="1"/>
-      <c r="DB49" s="1"/>
+      <c r="DA49" s="47"/>
+      <c r="DB49" s="47"/>
+      <c r="DC49" s="1"/>
     </row>
-    <row r="50" spans="1:106">
+    <row r="50" spans="1:107">
       <c r="A50" s="1" t="s">
         <v>441</v>
       </c>
@@ -9504,7 +9733,7 @@
       <c r="H50" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="I50" s="48" t="s">
+      <c r="I50" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J50" s="1"/>
@@ -9608,10 +9837,11 @@
       <c r="CX50" s="1"/>
       <c r="CY50" s="1"/>
       <c r="CZ50" s="1"/>
-      <c r="DA50" s="1"/>
-      <c r="DB50" s="1"/>
+      <c r="DA50" s="47"/>
+      <c r="DB50" s="47"/>
+      <c r="DC50" s="1"/>
     </row>
-    <row r="51" spans="1:106">
+    <row r="51" spans="1:107">
       <c r="A51" s="1" t="s">
         <v>446</v>
       </c>
@@ -9636,7 +9866,7 @@
       <c r="H51" s="1" t="s">
         <v>449</v>
       </c>
-      <c r="I51" s="48" t="s">
+      <c r="I51" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J51" s="1"/>
@@ -9740,10 +9970,11 @@
       <c r="CX51" s="1"/>
       <c r="CY51" s="1"/>
       <c r="CZ51" s="1"/>
-      <c r="DA51" s="1"/>
-      <c r="DB51" s="1"/>
+      <c r="DA51" s="47"/>
+      <c r="DB51" s="47"/>
+      <c r="DC51" s="1"/>
     </row>
-    <row r="52" spans="1:106">
+    <row r="52" spans="1:107">
       <c r="A52" s="1" t="s">
         <v>451</v>
       </c>
@@ -9768,7 +9999,7 @@
       <c r="H52" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="I52" s="48" t="s">
+      <c r="I52" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J52" s="1"/>
@@ -9872,10 +10103,11 @@
       <c r="CX52" s="1"/>
       <c r="CY52" s="1"/>
       <c r="CZ52" s="1"/>
-      <c r="DA52" s="1"/>
-      <c r="DB52" s="1"/>
+      <c r="DA52" s="47"/>
+      <c r="DB52" s="47"/>
+      <c r="DC52" s="1"/>
     </row>
-    <row r="53" spans="1:106">
+    <row r="53" spans="1:107">
       <c r="A53" s="1" t="s">
         <v>456</v>
       </c>
@@ -9898,7 +10130,7 @@
         <v>458</v>
       </c>
       <c r="H53" s="1"/>
-      <c r="I53" s="48" t="s">
+      <c r="I53" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J53" s="1"/>
@@ -10002,10 +10234,11 @@
       <c r="CX53" s="1"/>
       <c r="CY53" s="1"/>
       <c r="CZ53" s="1"/>
-      <c r="DA53" s="1"/>
-      <c r="DB53" s="1"/>
+      <c r="DA53" s="47"/>
+      <c r="DB53" s="47"/>
+      <c r="DC53" s="1"/>
     </row>
-    <row r="54" spans="1:106">
+    <row r="54" spans="1:107">
       <c r="A54" s="1" t="s">
         <v>460</v>
       </c>
@@ -10028,7 +10261,7 @@
         <v>462</v>
       </c>
       <c r="H54" s="1"/>
-      <c r="I54" s="48" t="s">
+      <c r="I54" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J54" s="1"/>
@@ -10132,10 +10365,11 @@
       <c r="CX54" s="1"/>
       <c r="CY54" s="1"/>
       <c r="CZ54" s="1"/>
-      <c r="DA54" s="1"/>
-      <c r="DB54" s="1"/>
+      <c r="DA54" s="47"/>
+      <c r="DB54" s="47"/>
+      <c r="DC54" s="1"/>
     </row>
-    <row r="55" spans="1:106">
+    <row r="55" spans="1:107">
       <c r="A55" s="1" t="s">
         <v>464</v>
       </c>
@@ -10160,7 +10394,7 @@
       <c r="H55" s="1" t="s">
         <v>467</v>
       </c>
-      <c r="I55" s="48" t="s">
+      <c r="I55" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J55" s="1"/>
@@ -10264,10 +10498,11 @@
       <c r="CX55" s="1"/>
       <c r="CY55" s="1"/>
       <c r="CZ55" s="1"/>
-      <c r="DA55" s="1"/>
-      <c r="DB55" s="1"/>
+      <c r="DA55" s="47"/>
+      <c r="DB55" s="47"/>
+      <c r="DC55" s="1"/>
     </row>
-    <row r="56" spans="1:106">
+    <row r="56" spans="1:107">
       <c r="A56" s="1" t="s">
         <v>469</v>
       </c>
@@ -10292,7 +10527,7 @@
       <c r="H56" s="1" t="s">
         <v>472</v>
       </c>
-      <c r="I56" s="48" t="s">
+      <c r="I56" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J56" s="1"/>
@@ -10396,10 +10631,11 @@
       <c r="CX56" s="1"/>
       <c r="CY56" s="1"/>
       <c r="CZ56" s="1"/>
-      <c r="DA56" s="1"/>
-      <c r="DB56" s="1"/>
+      <c r="DA56" s="47"/>
+      <c r="DB56" s="47"/>
+      <c r="DC56" s="1"/>
     </row>
-    <row r="57" spans="1:106">
+    <row r="57" spans="1:107">
       <c r="A57" s="1" t="s">
         <v>474</v>
       </c>
@@ -10422,7 +10658,7 @@
         <v>476</v>
       </c>
       <c r="H57" s="1"/>
-      <c r="I57" s="48" t="s">
+      <c r="I57" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J57" s="1"/>
@@ -10528,10 +10764,11 @@
       <c r="CX57" s="1"/>
       <c r="CY57" s="1"/>
       <c r="CZ57" s="1"/>
-      <c r="DA57" s="1"/>
-      <c r="DB57" s="1"/>
+      <c r="DA57" s="47"/>
+      <c r="DB57" s="47"/>
+      <c r="DC57" s="1"/>
     </row>
-    <row r="58" spans="1:106">
+    <row r="58" spans="1:107">
       <c r="A58" s="1" t="s">
         <v>479</v>
       </c>
@@ -10554,7 +10791,7 @@
         <v>481</v>
       </c>
       <c r="H58" s="1"/>
-      <c r="I58" s="48" t="s">
+      <c r="I58" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J58" s="1"/>
@@ -10660,10 +10897,11 @@
       <c r="CX58" s="1"/>
       <c r="CY58" s="1"/>
       <c r="CZ58" s="1"/>
-      <c r="DA58" s="1"/>
-      <c r="DB58" s="1"/>
+      <c r="DA58" s="47"/>
+      <c r="DB58" s="47"/>
+      <c r="DC58" s="1"/>
     </row>
-    <row r="59" spans="1:106">
+    <row r="59" spans="1:107">
       <c r="A59" s="1" t="s">
         <v>483</v>
       </c>
@@ -10688,7 +10926,7 @@
       <c r="H59" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="I59" s="48" t="s">
+      <c r="I59" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J59" s="1"/>
@@ -10794,10 +11032,11 @@
       <c r="CX59" s="1"/>
       <c r="CY59" s="1"/>
       <c r="CZ59" s="1"/>
-      <c r="DA59" s="1"/>
-      <c r="DB59" s="1"/>
+      <c r="DA59" s="47"/>
+      <c r="DB59" s="47"/>
+      <c r="DC59" s="1"/>
     </row>
-    <row r="60" spans="1:106">
+    <row r="60" spans="1:107">
       <c r="A60" s="1" t="s">
         <v>489</v>
       </c>
@@ -10822,7 +11061,7 @@
       <c r="H60" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="I60" s="48" t="s">
+      <c r="I60" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J60" s="1"/>
@@ -10928,10 +11167,11 @@
       <c r="CX60" s="1"/>
       <c r="CY60" s="1"/>
       <c r="CZ60" s="1"/>
-      <c r="DA60" s="1"/>
-      <c r="DB60" s="1"/>
+      <c r="DA60" s="47"/>
+      <c r="DB60" s="47"/>
+      <c r="DC60" s="1"/>
     </row>
-    <row r="61" spans="1:106">
+    <row r="61" spans="1:107">
       <c r="A61" s="1" t="s">
         <v>493</v>
       </c>
@@ -10956,7 +11196,7 @@
       <c r="H61" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I61" s="48" t="s">
+      <c r="I61" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J61" s="1"/>
@@ -11062,10 +11302,11 @@
       <c r="CX61" s="1"/>
       <c r="CY61" s="1"/>
       <c r="CZ61" s="1"/>
-      <c r="DA61" s="1"/>
-      <c r="DB61" s="1"/>
+      <c r="DA61" s="47"/>
+      <c r="DB61" s="47"/>
+      <c r="DC61" s="1"/>
     </row>
-    <row r="62" spans="1:106">
+    <row r="62" spans="1:107">
       <c r="A62" s="1" t="s">
         <v>498</v>
       </c>
@@ -11090,7 +11331,7 @@
       <c r="H62" s="1" t="s">
         <v>496</v>
       </c>
-      <c r="I62" s="48" t="s">
+      <c r="I62" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J62" s="1"/>
@@ -11196,10 +11437,11 @@
       <c r="CX62" s="1"/>
       <c r="CY62" s="1"/>
       <c r="CZ62" s="1"/>
-      <c r="DA62" s="1"/>
-      <c r="DB62" s="1"/>
+      <c r="DA62" s="47"/>
+      <c r="DB62" s="47"/>
+      <c r="DC62" s="1"/>
     </row>
-    <row r="63" spans="1:106">
+    <row r="63" spans="1:107">
       <c r="A63" s="1" t="s">
         <v>502</v>
       </c>
@@ -11224,7 +11466,7 @@
       <c r="H63" s="1" t="s">
         <v>505</v>
       </c>
-      <c r="I63" s="48" t="s">
+      <c r="I63" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J63" s="1"/>
@@ -11330,10 +11572,11 @@
       <c r="CX63" s="1"/>
       <c r="CY63" s="1"/>
       <c r="CZ63" s="1"/>
-      <c r="DA63" s="1"/>
-      <c r="DB63" s="1"/>
+      <c r="DA63" s="47"/>
+      <c r="DB63" s="47"/>
+      <c r="DC63" s="1"/>
     </row>
-    <row r="64" spans="1:106">
+    <row r="64" spans="1:107">
       <c r="A64" s="1" t="s">
         <v>508</v>
       </c>
@@ -11358,7 +11601,7 @@
       <c r="H64" s="1" t="s">
         <v>511</v>
       </c>
-      <c r="I64" s="48" t="s">
+      <c r="I64" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J64" s="1"/>
@@ -11464,10 +11707,11 @@
       <c r="CX64" s="1"/>
       <c r="CY64" s="1"/>
       <c r="CZ64" s="1"/>
-      <c r="DA64" s="1"/>
-      <c r="DB64" s="1"/>
+      <c r="DA64" s="47"/>
+      <c r="DB64" s="47"/>
+      <c r="DC64" s="1"/>
     </row>
-    <row r="65" spans="1:106">
+    <row r="65" spans="1:107">
       <c r="A65" s="1" t="s">
         <v>513</v>
       </c>
@@ -11492,7 +11736,7 @@
       <c r="H65" s="1" t="s">
         <v>516</v>
       </c>
-      <c r="I65" s="48" t="s">
+      <c r="I65" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J65" s="1"/>
@@ -11598,10 +11842,11 @@
       <c r="CX65" s="1"/>
       <c r="CY65" s="1"/>
       <c r="CZ65" s="1"/>
-      <c r="DA65" s="1"/>
-      <c r="DB65" s="1"/>
+      <c r="DA65" s="47"/>
+      <c r="DB65" s="47"/>
+      <c r="DC65" s="1"/>
     </row>
-    <row r="66" spans="1:106">
+    <row r="66" spans="1:107">
       <c r="A66" s="11" t="s">
         <v>518</v>
       </c>
@@ -11626,7 +11871,7 @@
       <c r="H66" s="11" t="s">
         <v>521</v>
       </c>
-      <c r="I66" s="48" t="s">
+      <c r="I66" s="62" t="s">
         <v>183</v>
       </c>
       <c r="J66" s="11"/>
@@ -11732,10 +11977,11 @@
       <c r="CX66" s="11"/>
       <c r="CY66" s="11"/>
       <c r="CZ66" s="11"/>
-      <c r="DA66" s="11"/>
-      <c r="DB66" s="11"/>
+      <c r="DA66" s="48"/>
+      <c r="DB66" s="48"/>
+      <c r="DC66" s="11"/>
     </row>
-    <row r="67" spans="1:106">
+    <row r="67" spans="1:107">
       <c r="A67" s="11" t="s">
         <v>529</v>
       </c>
@@ -11868,14 +12114,15 @@
       <c r="CZ67" s="43" t="s">
         <v>533</v>
       </c>
-      <c r="DA67" s="43" t="s">
+      <c r="DA67" s="49" t="s">
         <v>535</v>
       </c>
-      <c r="DB67" s="11" t="s">
+      <c r="DB67" s="49"/>
+      <c r="DC67" s="11" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="68" spans="1:106">
+    <row r="68" spans="1:107">
       <c r="A68" s="1" t="s">
         <v>544</v>
       </c>
@@ -12016,8 +12263,408 @@
       <c r="CX68" s="1"/>
       <c r="CY68" s="37"/>
       <c r="CZ68" s="36"/>
-      <c r="DA68" s="26"/>
-      <c r="DB68" s="1"/>
+      <c r="DA68" s="50"/>
+      <c r="DB68" s="50"/>
+      <c r="DC68" s="1"/>
+    </row>
+    <row r="69" spans="1:107">
+      <c r="A69" s="1" t="s">
+        <v>554</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="60" t="s">
+        <v>553</v>
+      </c>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="39"/>
+      <c r="P69" s="39"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+      <c r="S69" s="1"/>
+      <c r="T69" s="1"/>
+      <c r="U69" s="1"/>
+      <c r="V69" s="1"/>
+      <c r="W69" s="1"/>
+      <c r="X69" s="1"/>
+      <c r="Y69" s="1"/>
+      <c r="Z69" s="1"/>
+      <c r="AA69" s="1"/>
+      <c r="AB69" s="1"/>
+      <c r="AC69" s="1"/>
+      <c r="AD69" s="1"/>
+      <c r="AE69" s="1"/>
+      <c r="AF69" s="1"/>
+      <c r="AG69" s="1"/>
+      <c r="AH69" s="1"/>
+      <c r="AI69" s="1"/>
+      <c r="AJ69" s="1"/>
+      <c r="AK69" s="1"/>
+      <c r="AL69" s="1"/>
+      <c r="AM69" s="1"/>
+      <c r="AN69" s="1"/>
+      <c r="AO69" s="1"/>
+      <c r="AP69" s="1"/>
+      <c r="AQ69" s="1"/>
+      <c r="AR69" s="1"/>
+      <c r="AS69" s="1"/>
+      <c r="AT69" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="AU69" s="1"/>
+      <c r="AV69" s="1"/>
+      <c r="AW69" s="29"/>
+      <c r="AX69" s="1"/>
+      <c r="AY69" s="1"/>
+      <c r="AZ69" s="1"/>
+      <c r="BA69" s="1"/>
+      <c r="BB69" s="1"/>
+      <c r="BC69" s="1"/>
+      <c r="BD69" s="1"/>
+      <c r="BE69" s="1"/>
+      <c r="BF69" s="1"/>
+      <c r="BG69" s="1"/>
+      <c r="BH69" s="1"/>
+      <c r="BI69" s="1"/>
+      <c r="BJ69" s="1"/>
+      <c r="BK69" s="1"/>
+      <c r="BL69" s="1"/>
+      <c r="BM69" s="1"/>
+      <c r="BN69" s="1"/>
+      <c r="BO69" s="1"/>
+      <c r="BP69" s="1"/>
+      <c r="BQ69" s="1"/>
+      <c r="BR69" s="1"/>
+      <c r="BS69" s="1"/>
+      <c r="BT69" s="1"/>
+      <c r="BU69" s="1"/>
+      <c r="BV69" s="1"/>
+      <c r="BW69" s="1"/>
+      <c r="BX69" s="1"/>
+      <c r="BY69" s="1"/>
+      <c r="BZ69" s="1"/>
+      <c r="CA69" s="1"/>
+      <c r="CB69" s="1"/>
+      <c r="CC69" s="1"/>
+      <c r="CD69" s="1"/>
+      <c r="CE69" s="1"/>
+      <c r="CF69" s="1"/>
+      <c r="CG69" s="1"/>
+      <c r="CH69" s="1"/>
+      <c r="CI69" s="1"/>
+      <c r="CJ69" s="1"/>
+      <c r="CK69" s="1"/>
+      <c r="CL69" s="1"/>
+      <c r="CM69" s="1"/>
+      <c r="CN69" s="1">
+        <v>168</v>
+      </c>
+      <c r="CO69" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CP69" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="CQ69" s="1"/>
+      <c r="CR69" s="1"/>
+      <c r="CS69" s="1"/>
+      <c r="CT69" s="1"/>
+      <c r="CU69" s="1"/>
+      <c r="CV69" s="1"/>
+      <c r="CW69" s="1"/>
+      <c r="CX69" s="1"/>
+      <c r="CY69" s="37"/>
+      <c r="CZ69" s="36"/>
+      <c r="DA69" s="50"/>
+      <c r="DB69" s="51" t="s">
+        <v>561</v>
+      </c>
+      <c r="DC69" s="1"/>
+    </row>
+    <row r="70" spans="1:107">
+      <c r="A70" s="1" t="s">
+        <v>562</v>
+      </c>
+      <c r="B70" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="60" t="s">
+        <v>553</v>
+      </c>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="39"/>
+      <c r="P70" s="39"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="1"/>
+      <c r="U70" s="1"/>
+      <c r="V70" s="1"/>
+      <c r="W70" s="1"/>
+      <c r="X70" s="1"/>
+      <c r="Y70" s="1"/>
+      <c r="Z70" s="1"/>
+      <c r="AA70" s="1"/>
+      <c r="AB70" s="1"/>
+      <c r="AC70" s="1"/>
+      <c r="AD70" s="1"/>
+      <c r="AE70" s="1"/>
+      <c r="AF70" s="1"/>
+      <c r="AG70" s="1"/>
+      <c r="AH70" s="1"/>
+      <c r="AI70" s="1"/>
+      <c r="AJ70" s="1"/>
+      <c r="AK70" s="1"/>
+      <c r="AL70" s="1"/>
+      <c r="AM70" s="1"/>
+      <c r="AN70" s="1"/>
+      <c r="AO70" s="1"/>
+      <c r="AP70" s="1"/>
+      <c r="AQ70" s="1"/>
+      <c r="AR70" s="1"/>
+      <c r="AS70" s="1"/>
+      <c r="AT70" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="AU70" s="1"/>
+      <c r="AV70" s="1"/>
+      <c r="AW70" s="29"/>
+      <c r="AX70" s="1"/>
+      <c r="AY70" s="1"/>
+      <c r="AZ70" s="1"/>
+      <c r="BA70" s="1"/>
+      <c r="BB70" s="1"/>
+      <c r="BC70" s="1"/>
+      <c r="BD70" s="1"/>
+      <c r="BE70" s="1"/>
+      <c r="BF70" s="1"/>
+      <c r="BG70" s="1"/>
+      <c r="BH70" s="1"/>
+      <c r="BI70" s="1"/>
+      <c r="BJ70" s="1"/>
+      <c r="BK70" s="1"/>
+      <c r="BL70" s="1"/>
+      <c r="BM70" s="1"/>
+      <c r="BN70" s="1"/>
+      <c r="BO70" s="1"/>
+      <c r="BP70" s="1"/>
+      <c r="BQ70" s="1"/>
+      <c r="BR70" s="1"/>
+      <c r="BS70" s="1"/>
+      <c r="BT70" s="1"/>
+      <c r="BU70" s="1"/>
+      <c r="BV70" s="1"/>
+      <c r="BW70" s="1"/>
+      <c r="BX70" s="1"/>
+      <c r="BY70" s="1"/>
+      <c r="BZ70" s="1"/>
+      <c r="CA70" s="1"/>
+      <c r="CB70" s="1"/>
+      <c r="CC70" s="1"/>
+      <c r="CD70" s="1"/>
+      <c r="CE70" s="1"/>
+      <c r="CF70" s="1"/>
+      <c r="CG70" s="1"/>
+      <c r="CH70" s="1"/>
+      <c r="CI70" s="1"/>
+      <c r="CJ70" s="1"/>
+      <c r="CK70" s="1"/>
+      <c r="CL70" s="1"/>
+      <c r="CM70" s="1"/>
+      <c r="CN70" s="1">
+        <v>168</v>
+      </c>
+      <c r="CO70" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CP70" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="CQ70" s="1"/>
+      <c r="CR70" s="1"/>
+      <c r="CS70" s="1"/>
+      <c r="CT70" s="1"/>
+      <c r="CU70" s="1"/>
+      <c r="CV70" s="1"/>
+      <c r="CW70" s="1"/>
+      <c r="CX70" s="1"/>
+      <c r="CY70" s="37"/>
+      <c r="CZ70" s="36"/>
+      <c r="DA70" s="50"/>
+      <c r="DB70" s="51" t="s">
+        <v>564</v>
+      </c>
+      <c r="DC70" s="1"/>
+    </row>
+    <row r="71" spans="1:107">
+      <c r="A71" s="1" t="s">
+        <v>565</v>
+      </c>
+      <c r="B71" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>555</v>
+      </c>
+      <c r="F71" s="1" t="s">
+        <v>570</v>
+      </c>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="60" t="s">
+        <v>553</v>
+      </c>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="39"/>
+      <c r="P71" s="39"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+      <c r="S71" s="1"/>
+      <c r="T71" s="1"/>
+      <c r="U71" s="1"/>
+      <c r="V71" s="1"/>
+      <c r="W71" s="1"/>
+      <c r="X71" s="1"/>
+      <c r="Y71" s="1"/>
+      <c r="Z71" s="1"/>
+      <c r="AA71" s="1"/>
+      <c r="AB71" s="1"/>
+      <c r="AC71" s="1"/>
+      <c r="AD71" s="1"/>
+      <c r="AE71" s="1"/>
+      <c r="AF71" s="1"/>
+      <c r="AG71" s="1"/>
+      <c r="AH71" s="1"/>
+      <c r="AI71" s="1"/>
+      <c r="AJ71" s="1"/>
+      <c r="AK71" s="1"/>
+      <c r="AL71" s="1"/>
+      <c r="AM71" s="1"/>
+      <c r="AN71" s="1"/>
+      <c r="AO71" s="1"/>
+      <c r="AP71" s="1"/>
+      <c r="AQ71" s="1"/>
+      <c r="AR71" s="1"/>
+      <c r="AS71" s="1"/>
+      <c r="AT71" s="1" t="s">
+        <v>556</v>
+      </c>
+      <c r="AU71" s="1"/>
+      <c r="AV71" s="1"/>
+      <c r="AW71" s="29"/>
+      <c r="AX71" s="1"/>
+      <c r="AY71" s="1"/>
+      <c r="AZ71" s="1"/>
+      <c r="BA71" s="1"/>
+      <c r="BB71" s="1"/>
+      <c r="BC71" s="1"/>
+      <c r="BD71" s="1"/>
+      <c r="BE71" s="1"/>
+      <c r="BF71" s="1"/>
+      <c r="BG71" s="1"/>
+      <c r="BH71" s="1"/>
+      <c r="BI71" s="1"/>
+      <c r="BJ71" s="1"/>
+      <c r="BK71" s="1"/>
+      <c r="BL71" s="1"/>
+      <c r="BM71" s="1"/>
+      <c r="BN71" s="1"/>
+      <c r="BO71" s="1"/>
+      <c r="BP71" s="1"/>
+      <c r="BQ71" s="1"/>
+      <c r="BR71" s="1"/>
+      <c r="BS71" s="1"/>
+      <c r="BT71" s="1"/>
+      <c r="BU71" s="1"/>
+      <c r="BV71" s="1"/>
+      <c r="BW71" s="1"/>
+      <c r="BX71" s="1"/>
+      <c r="BY71" s="1"/>
+      <c r="BZ71" s="1"/>
+      <c r="CA71" s="1"/>
+      <c r="CB71" s="1"/>
+      <c r="CC71" s="1"/>
+      <c r="CD71" s="1"/>
+      <c r="CE71" s="1"/>
+      <c r="CF71" s="1"/>
+      <c r="CG71" s="1"/>
+      <c r="CH71" s="1"/>
+      <c r="CI71" s="1"/>
+      <c r="CJ71" s="1"/>
+      <c r="CK71" s="1"/>
+      <c r="CL71" s="1"/>
+      <c r="CM71" s="1"/>
+      <c r="CN71" s="1">
+        <v>168</v>
+      </c>
+      <c r="CO71" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CP71" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="CQ71" s="1"/>
+      <c r="CR71" s="1"/>
+      <c r="CS71" s="1"/>
+      <c r="CT71" s="1"/>
+      <c r="CU71" s="1"/>
+      <c r="CV71" s="1"/>
+      <c r="CW71" s="1"/>
+      <c r="CX71" s="1"/>
+      <c r="CY71" s="37"/>
+      <c r="CZ71" s="36"/>
+      <c r="DA71" s="50"/>
+      <c r="DB71" s="51" t="s">
+        <v>567</v>
+      </c>
+      <c r="DC71" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>